<commit_message>
Update male CD4>500 durations to be 3 months (rate=4) so as to be larger than time step. In historicalSim, initiate HIV in all ages vs. only ages 10-49 to avoid NaN values when performing CD4 transitions across all ages. HIV infections initiated as acute vs. CD4>500. Update pathModifier.
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="102">
   <si>
     <t>Male</t>
   </si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t xml:space="preserve">Late-stage </t>
-  </si>
-  <si>
-    <t>making this 1/(current timestep)</t>
   </si>
   <si>
     <t>Transition rate forVL progression (years^-1)</t>
@@ -478,7 +475,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +491,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -736,21 +739,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -760,10 +748,33 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,13 +787,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,6 +796,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2479,8 +2488,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AX187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3669,10 +3678,10 @@
     </row>
     <row r="42" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="25"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="24"/>
       <c r="J42" s="23"/>
       <c r="K42" s="23"/>
@@ -3685,23 +3694,23 @@
     </row>
     <row r="43" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="31"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="60" t="s">
+      <c r="B43" s="63"/>
+      <c r="C43" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="65"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="60"/>
       <c r="H43" s="31"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="63" t="s">
+      <c r="I43" s="66"/>
+      <c r="J43" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="61"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="70"/>
       <c r="O43" s="31"/>
     </row>
     <row r="44" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
@@ -3751,30 +3760,30 @@
       <c r="AX44" s="18"/>
     </row>
     <row r="45" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C45" s="27">
-        <f>1/J45</f>
+        <f t="shared" ref="C45:C60" si="2">1/J45</f>
         <v>4</v>
       </c>
       <c r="D45" s="27">
-        <f>1/(1/6)</f>
-        <v>6</v>
+        <f>1/K45</f>
+        <v>1.8181818181818181</v>
       </c>
       <c r="E45" s="27">
-        <f>1/L45</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" ref="E45:E60" si="3">1/L45</f>
+        <v>0.25188916876574308</v>
       </c>
       <c r="F45" s="27">
-        <f>1/M45</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" ref="F45:F60" si="4">1/M45</f>
+        <v>0.19880715705765406</v>
       </c>
       <c r="G45" s="25"/>
-      <c r="H45" s="71" t="s">
+      <c r="H45" s="75" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -3784,46 +3793,45 @@
         <v>0.25</v>
       </c>
       <c r="K45" s="31">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L45" s="31">
-        <v>3.81</v>
+        <v>3.97</v>
       </c>
       <c r="M45" s="31">
-        <v>4.67</v>
+        <v>5.03</v>
       </c>
       <c r="N45" s="31">
         <v>2.13</v>
       </c>
       <c r="O45" s="31">
         <f>SUM(J45:N45)</f>
-        <v>10.86</v>
+        <v>11.93</v>
       </c>
       <c r="AX45" s="17"/>
     </row>
     <row r="46" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="68"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="27">
-        <f>1/J46</f>
-        <v>4</v>
-      </c>
-      <c r="D46" s="27">
-        <f t="shared" ref="D46:D60" si="2">1/(1/6)</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D46" s="68">
+        <v>4</v>
       </c>
       <c r="E46" s="27">
-        <f>1/L46</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F46" s="27">
-        <f>1/M46</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="25"/>
-      <c r="H46" s="72"/>
+      <c r="H46" s="76"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3843,34 +3851,33 @@
         <v>3.7</v>
       </c>
       <c r="O46" s="31">
-        <f t="shared" ref="O46:O60" si="3">SUM(J46:N46)</f>
+        <f t="shared" ref="O46:O60" si="5">SUM(J46:N46)</f>
         <v>12.43</v>
       </c>
       <c r="AX46" s="11"/>
     </row>
     <row r="47" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="68"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="27">
-        <f>1/J47</f>
-        <v>4</v>
-      </c>
-      <c r="D47" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D47" s="68">
+        <v>4</v>
       </c>
       <c r="E47" s="27">
-        <f>1/L47</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F47" s="27">
-        <f>1/M47</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="25"/>
-      <c r="H47" s="72"/>
+      <c r="H47" s="76"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3890,34 +3897,33 @@
         <v>3.7</v>
       </c>
       <c r="O47" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
       <c r="AX47" s="11"/>
     </row>
     <row r="48" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="68"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="27">
-        <f>1/J48</f>
-        <v>4</v>
-      </c>
-      <c r="D48" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D48" s="68">
+        <v>4</v>
       </c>
       <c r="E48" s="27">
-        <f>1/L48</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F48" s="27">
-        <f>1/M48</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="25"/>
-      <c r="H48" s="72"/>
+      <c r="H48" s="76"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3937,34 +3943,33 @@
         <v>3.7</v>
       </c>
       <c r="O48" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
       <c r="AX48" s="11"/>
     </row>
     <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="68"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="27">
-        <f>1/J49</f>
-        <v>4</v>
-      </c>
-      <c r="D49" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D49" s="68">
+        <v>4</v>
       </c>
       <c r="E49" s="27">
-        <f>1/L49</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F49" s="27">
-        <f>1/M49</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="25"/>
-      <c r="H49" s="72"/>
+      <c r="H49" s="76"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3984,33 +3989,32 @@
         <v>3.7</v>
       </c>
       <c r="O49" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="68"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="27">
-        <f>1/J50</f>
-        <v>4</v>
-      </c>
-      <c r="D50" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D50" s="68">
+        <v>4</v>
       </c>
       <c r="E50" s="27">
-        <f>1/L50</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F50" s="27">
-        <f>1/M50</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="25"/>
-      <c r="H50" s="72"/>
+      <c r="H50" s="76"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4030,33 +4034,32 @@
         <v>3.7</v>
       </c>
       <c r="O50" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="68"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="27">
-        <f>1/J51</f>
-        <v>4</v>
-      </c>
-      <c r="D51" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D51" s="68">
+        <v>4</v>
       </c>
       <c r="E51" s="27">
-        <f>1/L51</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F51" s="27">
-        <f>1/M51</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="25"/>
-      <c r="H51" s="72"/>
+      <c r="H51" s="76"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4076,33 +4079,32 @@
         <v>3.7</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="68"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="27">
-        <f>1/J52</f>
-        <v>4</v>
-      </c>
-      <c r="D52" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D52" s="68">
+        <v>4</v>
       </c>
       <c r="E52" s="27">
-        <f>1/L52</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F52" s="27">
-        <f>1/M52</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="25"/>
-      <c r="H52" s="72"/>
+      <c r="H52" s="76"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4122,33 +4124,32 @@
         <v>3.7</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="68"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="27">
-        <f>1/J53</f>
-        <v>4</v>
-      </c>
-      <c r="D53" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D53" s="68">
+        <v>4</v>
       </c>
       <c r="E53" s="27">
-        <f>1/L53</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F53" s="27">
-        <f>1/M53</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="25"/>
-      <c r="H53" s="72"/>
+      <c r="H53" s="76"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4168,33 +4169,32 @@
         <v>3.7</v>
       </c>
       <c r="O53" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="68"/>
+      <c r="A54" s="74"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="27">
-        <f>1/J54</f>
-        <v>4</v>
-      </c>
-      <c r="D54" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D54" s="68">
+        <v>4</v>
       </c>
       <c r="E54" s="27">
-        <f>1/L54</f>
+        <f t="shared" si="3"/>
         <v>0.26246719160104987</v>
       </c>
       <c r="F54" s="27">
-        <f>1/M54</f>
+        <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="25"/>
-      <c r="H54" s="72"/>
+      <c r="H54" s="76"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4214,33 +4214,32 @@
         <v>3.7</v>
       </c>
       <c r="O54" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="68"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C55" s="27">
-        <f>1/J55</f>
-        <v>4</v>
-      </c>
-      <c r="D55" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D55" s="68">
+        <v>4</v>
       </c>
       <c r="E55" s="27">
-        <f>1/L55</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F55" s="27">
-        <f>1/M55</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="25"/>
-      <c r="H55" s="72"/>
+      <c r="H55" s="76"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4251,42 +4250,41 @@
         <v>0</v>
       </c>
       <c r="L55" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M55" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N55" s="31">
         <v>1.85</v>
       </c>
       <c r="O55" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="68"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="27">
-        <f>1/J56</f>
-        <v>4</v>
-      </c>
-      <c r="D56" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D56" s="68">
+        <v>4</v>
       </c>
       <c r="E56" s="27">
-        <f>1/L56</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F56" s="27">
-        <f>1/M56</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="25"/>
-      <c r="H56" s="72"/>
+      <c r="H56" s="76"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4297,42 +4295,41 @@
         <v>0</v>
       </c>
       <c r="L56" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M56" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N56" s="31">
         <v>1.85</v>
       </c>
       <c r="O56" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="68"/>
+      <c r="A57" s="74"/>
       <c r="B57" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C57" s="27">
-        <f>1/J57</f>
-        <v>4</v>
-      </c>
-      <c r="D57" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D57" s="68">
+        <v>4</v>
       </c>
       <c r="E57" s="27">
-        <f>1/L57</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F57" s="27">
-        <f>1/M57</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="25"/>
-      <c r="H57" s="72"/>
+      <c r="H57" s="76"/>
       <c r="I57" s="42" t="s">
         <v>57</v>
       </c>
@@ -4343,42 +4340,41 @@
         <v>0</v>
       </c>
       <c r="L57" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M57" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N57" s="31">
         <v>1.85</v>
       </c>
       <c r="O57" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="68"/>
+      <c r="A58" s="74"/>
       <c r="B58" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="27">
-        <f>1/J58</f>
-        <v>4</v>
-      </c>
-      <c r="D58" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D58" s="68">
+        <v>4</v>
       </c>
       <c r="E58" s="27">
-        <f>1/L58</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F58" s="27">
-        <f>1/M58</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="H58" s="72"/>
+      <c r="H58" s="76"/>
       <c r="I58" s="42" t="s">
         <v>58</v>
       </c>
@@ -4389,42 +4385,41 @@
         <v>0</v>
       </c>
       <c r="L58" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M58" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N58" s="31">
         <v>1.85</v>
       </c>
       <c r="O58" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="59" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="68"/>
+      <c r="A59" s="74"/>
       <c r="B59" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C59" s="27">
-        <f>1/J59</f>
-        <v>4</v>
-      </c>
-      <c r="D59" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D59" s="68">
+        <v>4</v>
       </c>
       <c r="E59" s="27">
-        <f>1/L59</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F59" s="27">
-        <f>1/M59</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="H59" s="72"/>
+      <c r="H59" s="76"/>
       <c r="I59" s="42" t="s">
         <v>59</v>
       </c>
@@ -4435,42 +4430,41 @@
         <v>0</v>
       </c>
       <c r="L59" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M59" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N59" s="31">
         <v>1.85</v>
       </c>
       <c r="O59" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="60" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="68"/>
+      <c r="A60" s="74"/>
       <c r="B60" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C60" s="27">
-        <f>1/J60</f>
-        <v>4</v>
-      </c>
-      <c r="D60" s="27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D60" s="68">
+        <v>4</v>
       </c>
       <c r="E60" s="27">
-        <f>1/L60</f>
-        <v>0.26246719160104987</v>
+        <f t="shared" si="3"/>
+        <v>0.32258064516129031</v>
       </c>
       <c r="F60" s="27">
-        <f>1/M60</f>
-        <v>0.21413276231263384</v>
+        <f t="shared" si="4"/>
+        <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="H60" s="73"/>
+      <c r="H60" s="77"/>
       <c r="I60" s="42" t="s">
         <v>60</v>
       </c>
@@ -4481,31 +4475,29 @@
         <v>0</v>
       </c>
       <c r="L60" s="31">
-        <v>3.81</v>
+        <v>3.1</v>
       </c>
       <c r="M60" s="31">
-        <v>4.67</v>
+        <v>4.51</v>
       </c>
       <c r="N60" s="31">
         <v>1.85</v>
       </c>
       <c r="O60" s="31">
-        <f t="shared" si="3"/>
-        <v>10.58</v>
+        <f t="shared" si="5"/>
+        <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="61" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
-      <c r="B61" s="67"/>
+      <c r="B61" s="62"/>
       <c r="C61" s="24"/>
-      <c r="D61" s="24" t="s">
-        <v>101</v>
-      </c>
+      <c r="D61" s="24"/>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="25"/>
       <c r="H61" s="24"/>
-      <c r="I61" s="67"/>
+      <c r="I61" s="62"/>
       <c r="J61" s="24"/>
       <c r="K61" s="24"/>
       <c r="L61" s="24"/>
@@ -4514,30 +4506,30 @@
       <c r="O61" s="24"/>
     </row>
     <row r="62" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="75" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C62" s="27">
-        <f>1/J62</f>
+        <f t="shared" ref="C62:C77" si="6">1/J62</f>
         <v>4</v>
       </c>
       <c r="D62" s="27">
         <f>1/K62</f>
-        <v>1.075268817204301</v>
+        <v>0.69930069930069938</v>
       </c>
       <c r="E62" s="27">
-        <f>1/L62</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" ref="E62:E77" si="7">1/L62</f>
+        <v>0.25125628140703515</v>
       </c>
       <c r="F62" s="27">
-        <f>1/M62</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" ref="F62:F77" si="8">1/M62</f>
+        <v>0.25575447570332482</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="H62" s="71" t="s">
+      <c r="H62" s="75" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -4547,13 +4539,13 @@
         <v>0.25</v>
       </c>
       <c r="K62" s="31">
-        <v>0.93</v>
+        <v>1.43</v>
       </c>
       <c r="L62" s="31">
-        <v>3.71</v>
+        <v>3.98</v>
       </c>
       <c r="M62" s="31">
-        <v>4.68</v>
+        <v>3.91</v>
       </c>
       <c r="N62" s="31">
         <v>2.13</v>
@@ -4564,28 +4556,28 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="72"/>
+      <c r="A63" s="76"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C63" s="27">
-        <f>1/J63</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D63" s="27">
-        <f>1/K63</f>
+        <f t="shared" ref="D63:D77" si="9">1/K63</f>
         <v>1.075268817204301</v>
       </c>
       <c r="E63" s="27">
-        <f>1/L63</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F63" s="27">
-        <f>1/M63</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="25"/>
-      <c r="H63" s="72"/>
+      <c r="H63" s="76"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4605,33 +4597,33 @@
         <v>3.7</v>
       </c>
       <c r="O63" s="31">
-        <f t="shared" ref="O63:O77" si="4">SUM(J63:N63)</f>
+        <f t="shared" ref="O63:O77" si="10">SUM(J63:N63)</f>
         <v>13.27</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="72"/>
+      <c r="A64" s="76"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C64" s="27">
-        <f>1/J64</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D64" s="27">
-        <f>1/K64</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E64" s="27">
-        <f>1/L64</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F64" s="27">
-        <f>1/M64</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="25"/>
-      <c r="H64" s="72"/>
+      <c r="H64" s="76"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4651,33 +4643,33 @@
         <v>3.7</v>
       </c>
       <c r="O64" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="65" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="72"/>
+      <c r="A65" s="76"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="27">
-        <f>1/J65</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D65" s="27">
-        <f>1/K65</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E65" s="27">
-        <f>1/L65</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F65" s="27">
-        <f>1/M65</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="25"/>
-      <c r="H65" s="72"/>
+      <c r="H65" s="76"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4697,33 +4689,33 @@
         <v>3.7</v>
       </c>
       <c r="O65" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="66" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="72"/>
+      <c r="A66" s="76"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="27">
-        <f>1/J66</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D66" s="27">
-        <f>1/K66</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E66" s="27">
-        <f>1/L66</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F66" s="27">
-        <f>1/M66</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="25"/>
-      <c r="H66" s="72"/>
+      <c r="H66" s="76"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4743,33 +4735,33 @@
         <v>3.7</v>
       </c>
       <c r="O66" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="67" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="72"/>
+      <c r="A67" s="76"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="27">
-        <f>1/J67</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D67" s="27">
-        <f>1/K67</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E67" s="27">
-        <f>1/L67</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F67" s="27">
-        <f>1/M67</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="25"/>
-      <c r="H67" s="72"/>
+      <c r="H67" s="76"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4789,33 +4781,33 @@
         <v>3.7</v>
       </c>
       <c r="O67" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="68" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="72"/>
+      <c r="A68" s="76"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C68" s="27">
-        <f>1/J68</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D68" s="27">
-        <f>1/K68</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E68" s="27">
-        <f>1/L68</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F68" s="27">
-        <f>1/M68</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="25"/>
-      <c r="H68" s="72"/>
+      <c r="H68" s="76"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4835,33 +4827,33 @@
         <v>3.7</v>
       </c>
       <c r="O68" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="69" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="72"/>
+      <c r="A69" s="76"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="27">
-        <f>1/J69</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D69" s="27">
-        <f>1/K69</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E69" s="27">
-        <f>1/L69</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F69" s="27">
-        <f>1/M69</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="25"/>
-      <c r="H69" s="72"/>
+      <c r="H69" s="76"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4881,33 +4873,33 @@
         <v>3.7</v>
       </c>
       <c r="O69" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="70" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="72"/>
+      <c r="A70" s="76"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="27">
-        <f>1/J70</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D70" s="27">
-        <f>1/K70</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E70" s="27">
-        <f>1/L70</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F70" s="27">
-        <f>1/M70</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="25"/>
-      <c r="H70" s="72"/>
+      <c r="H70" s="76"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4927,33 +4919,33 @@
         <v>3.7</v>
       </c>
       <c r="O70" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="71" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="72"/>
+      <c r="A71" s="76"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="27">
-        <f>1/J71</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D71" s="27">
-        <f>1/K71</f>
+        <f t="shared" si="9"/>
         <v>1.075268817204301</v>
       </c>
       <c r="E71" s="27">
-        <f>1/L71</f>
+        <f t="shared" si="7"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F71" s="27">
-        <f>1/M71</f>
+        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="25"/>
-      <c r="H71" s="72"/>
+      <c r="H71" s="76"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4973,33 +4965,33 @@
         <v>3.7</v>
       </c>
       <c r="O71" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="72" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="72"/>
+      <c r="A72" s="76"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C72" s="27">
-        <f>1/J72</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D72" s="27">
-        <f>1/K72</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E72" s="27">
-        <f>1/L72</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F72" s="27">
-        <f>1/M72</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="25"/>
-      <c r="H72" s="72"/>
+      <c r="H72" s="76"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5007,45 +4999,45 @@
         <v>0.25</v>
       </c>
       <c r="K72" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L72" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M72" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N72" s="31">
         <v>1.85</v>
       </c>
       <c r="O72" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="72"/>
+      <c r="A73" s="76"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="27">
-        <f>1/J73</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D73" s="27">
-        <f>1/K73</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E73" s="27">
-        <f>1/L73</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F73" s="27">
-        <f>1/M73</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="25"/>
-      <c r="H73" s="72"/>
+      <c r="H73" s="76"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5053,45 +5045,45 @@
         <v>0.25</v>
       </c>
       <c r="K73" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L73" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M73" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N73" s="31">
         <v>1.85</v>
       </c>
       <c r="O73" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="74" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="72"/>
+      <c r="A74" s="76"/>
       <c r="B74" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C74" s="27">
-        <f>1/J74</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D74" s="27">
-        <f>1/K74</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E74" s="27">
-        <f>1/L74</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F74" s="27">
-        <f>1/M74</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="25"/>
-      <c r="H74" s="72"/>
+      <c r="H74" s="76"/>
       <c r="I74" s="42" t="s">
         <v>57</v>
       </c>
@@ -5099,45 +5091,45 @@
         <v>0.25</v>
       </c>
       <c r="K74" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L74" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M74" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N74" s="31">
         <v>1.85</v>
       </c>
       <c r="O74" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="75" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="72"/>
+      <c r="A75" s="76"/>
       <c r="B75" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C75" s="27">
-        <f>1/J75</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D75" s="27">
-        <f>1/K75</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E75" s="27">
-        <f>1/L75</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F75" s="27">
-        <f>1/M75</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="25"/>
-      <c r="H75" s="72"/>
+      <c r="H75" s="76"/>
       <c r="I75" s="42" t="s">
         <v>58</v>
       </c>
@@ -5145,45 +5137,45 @@
         <v>0.25</v>
       </c>
       <c r="K75" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L75" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M75" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N75" s="31">
         <v>1.85</v>
       </c>
       <c r="O75" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="76" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="72"/>
+      <c r="A76" s="76"/>
       <c r="B76" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C76" s="27">
-        <f>1/J76</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D76" s="27">
-        <f>1/K76</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E76" s="27">
-        <f>1/L76</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F76" s="27">
-        <f>1/M76</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="25"/>
-      <c r="H76" s="72"/>
+      <c r="H76" s="76"/>
       <c r="I76" s="42" t="s">
         <v>59</v>
       </c>
@@ -5191,45 +5183,45 @@
         <v>0.25</v>
       </c>
       <c r="K76" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L76" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M76" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N76" s="31">
         <v>1.85</v>
       </c>
       <c r="O76" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="77" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="73"/>
+      <c r="A77" s="77"/>
       <c r="B77" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C77" s="27">
-        <f>1/J77</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="D77" s="27">
-        <f>1/K77</f>
-        <v>1.075268817204301</v>
+        <f t="shared" si="9"/>
+        <v>3.4482758620689657</v>
       </c>
       <c r="E77" s="27">
-        <f>1/L77</f>
-        <v>0.26954177897574122</v>
+        <f t="shared" si="7"/>
+        <v>0.29940119760479045</v>
       </c>
       <c r="F77" s="27">
-        <f>1/M77</f>
-        <v>0.21367521367521369</v>
+        <f t="shared" si="8"/>
+        <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="25"/>
-      <c r="H77" s="73"/>
+      <c r="H77" s="77"/>
       <c r="I77" s="42" t="s">
         <v>60</v>
       </c>
@@ -5237,20 +5229,20 @@
         <v>0.25</v>
       </c>
       <c r="K77" s="31">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L77" s="31">
-        <v>3.71</v>
+        <v>3.34</v>
       </c>
       <c r="M77" s="31">
-        <v>4.68</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="N77" s="31">
         <v>1.85</v>
       </c>
       <c r="O77" s="31">
-        <f t="shared" si="4"/>
-        <v>11.42</v>
+        <f t="shared" si="10"/>
+        <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="78" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -5316,10 +5308,10 @@
     </row>
     <row r="81" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="24"/>
-      <c r="B81" s="64"/>
-      <c r="C81" s="64"/>
-      <c r="D81" s="64"/>
-      <c r="E81" s="64"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="72"/>
+      <c r="D81" s="72"/>
+      <c r="E81" s="72"/>
       <c r="F81" s="24"/>
       <c r="G81" s="55"/>
       <c r="H81" s="55"/>
@@ -5337,32 +5329,32 @@
     <row r="82" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="44"/>
       <c r="B82" s="44"/>
-      <c r="C82" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="D82" s="77"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="77"/>
+      <c r="C82" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="D82" s="78"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="78"/>
       <c r="G82" s="25"/>
       <c r="H82" s="31"/>
-      <c r="I82" s="75"/>
-      <c r="J82" s="63" t="s">
+      <c r="I82" s="66"/>
+      <c r="J82" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="K82" s="63"/>
-      <c r="L82" s="63"/>
-      <c r="M82" s="63"/>
-      <c r="N82" s="61"/>
+      <c r="K82" s="69"/>
+      <c r="L82" s="69"/>
+      <c r="M82" s="69"/>
+      <c r="N82" s="70"/>
       <c r="O82" s="31"/>
       <c r="P82" s="24"/>
       <c r="Q82" s="24"/>
       <c r="AB82" s="16"/>
     </row>
     <row r="83" spans="1:28" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="76" t="s">
+      <c r="A83" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B83" s="76" t="s">
+      <c r="B83" s="67" t="s">
         <v>26</v>
       </c>
       <c r="C83" s="5" t="s">
@@ -5378,10 +5370,10 @@
         <v>99</v>
       </c>
       <c r="G83" s="55"/>
-      <c r="H83" s="76" t="s">
+      <c r="H83" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="I83" s="76" t="s">
+      <c r="I83" s="67" t="s">
         <v>26</v>
       </c>
       <c r="J83" s="5" t="s">
@@ -5399,7 +5391,7 @@
       <c r="N83" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="O83" s="70" t="s">
+      <c r="O83" s="64" t="s">
         <v>48</v>
       </c>
       <c r="P83" s="24"/>
@@ -5407,7 +5399,7 @@
       <c r="AB83" s="16"/>
     </row>
     <row r="84" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="68" t="s">
+      <c r="A84" s="74" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5418,19 +5410,19 @@
         <v>4</v>
       </c>
       <c r="D84" s="27">
-        <f t="shared" ref="D84:F99" si="5">1/K84</f>
-        <v>0.19880715705765406</v>
+        <f t="shared" ref="D84:F99" si="11">1/K84</f>
+        <v>0.16393442622950821</v>
       </c>
       <c r="E84" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F84" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="55"/>
-      <c r="H84" s="71" t="s">
+      <c r="H84" s="75" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5440,7 +5432,7 @@
         <v>0.25</v>
       </c>
       <c r="K84" s="31">
-        <v>5.03</v>
+        <v>6.1</v>
       </c>
       <c r="L84" s="31">
         <v>4</v>
@@ -5453,34 +5445,34 @@
       </c>
       <c r="O84" s="31">
         <f>SUM(J84:N84)</f>
-        <v>10.860000000000001</v>
+        <v>11.93</v>
       </c>
       <c r="Q84" s="24"/>
       <c r="AB84" s="16"/>
     </row>
     <row r="85" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="68"/>
+      <c r="A85" s="74"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C85" s="27">
-        <f t="shared" ref="C85:C99" si="6">1/J85</f>
+        <f t="shared" ref="C85:C99" si="12">1/J85</f>
         <v>4</v>
       </c>
       <c r="D85" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E85" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F85" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="55"/>
-      <c r="H85" s="72"/>
+      <c r="H85" s="76"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5500,35 +5492,35 @@
         <v>0.83</v>
       </c>
       <c r="O85" s="31">
-        <f t="shared" ref="O85:O99" si="7">SUM(J85:N85)</f>
+        <f t="shared" ref="O85:O99" si="13">SUM(J85:N85)</f>
         <v>12.43</v>
       </c>
       <c r="Q85" s="55"/>
       <c r="AB85" s="16"/>
     </row>
     <row r="86" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="68"/>
+      <c r="A86" s="74"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C86" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D86" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E86" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F86" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="55"/>
-      <c r="H86" s="72"/>
+      <c r="H86" s="76"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5548,35 +5540,35 @@
         <v>0.83</v>
       </c>
       <c r="O86" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="Q86" s="25"/>
       <c r="AB86" s="16"/>
     </row>
     <row r="87" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="68"/>
+      <c r="A87" s="74"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D87" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E87" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F87" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="25"/>
-      <c r="H87" s="72"/>
+      <c r="H87" s="76"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5596,35 +5588,35 @@
         <v>0.83</v>
       </c>
       <c r="O87" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="Q87" s="25"/>
       <c r="AB87" s="16"/>
     </row>
     <row r="88" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="68"/>
+      <c r="A88" s="74"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C88" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D88" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E88" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F88" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="55"/>
-      <c r="H88" s="72"/>
+      <c r="H88" s="76"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5644,35 +5636,35 @@
         <v>0.83</v>
       </c>
       <c r="O88" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="Q88" s="25"/>
       <c r="AB88" s="16"/>
     </row>
     <row r="89" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A89" s="68"/>
+      <c r="A89" s="74"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D89" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E89" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F89" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="25"/>
-      <c r="H89" s="72"/>
+      <c r="H89" s="76"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5692,7 +5684,7 @@
         <v>0.83</v>
       </c>
       <c r="O89" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="P89" s="24"/>
@@ -5700,28 +5692,28 @@
       <c r="AB89" s="16"/>
     </row>
     <row r="90" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="68"/>
+      <c r="A90" s="74"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D90" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E90" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F90" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="55"/>
-      <c r="H90" s="72"/>
+      <c r="H90" s="76"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5741,34 +5733,34 @@
         <v>0.83</v>
       </c>
       <c r="O90" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="AB90" s="16"/>
     </row>
     <row r="91" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A91" s="68"/>
+      <c r="A91" s="74"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C91" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D91" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E91" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F91" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="55"/>
-      <c r="H91" s="72"/>
+      <c r="H91" s="76"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5788,34 +5780,34 @@
         <v>0.83</v>
       </c>
       <c r="O91" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="AB91" s="16"/>
     </row>
     <row r="92" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="68"/>
+      <c r="A92" s="74"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C92" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D92" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E92" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F92" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="55"/>
-      <c r="H92" s="72"/>
+      <c r="H92" s="76"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5835,34 +5827,34 @@
         <v>0.83</v>
       </c>
       <c r="O92" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="AB92" s="16"/>
     </row>
     <row r="93" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="68"/>
+      <c r="A93" s="74"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C93" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D93" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E93" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F93" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="55"/>
-      <c r="H93" s="72"/>
+      <c r="H93" s="76"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5882,34 +5874,34 @@
         <v>0.83</v>
       </c>
       <c r="O93" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.43</v>
       </c>
       <c r="AB93" s="16"/>
     </row>
     <row r="94" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A94" s="68"/>
+      <c r="A94" s="74"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D94" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E94" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F94" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="25"/>
-      <c r="H94" s="72"/>
+      <c r="H94" s="76"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5917,7 +5909,7 @@
         <v>0.25</v>
       </c>
       <c r="K94" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L94" s="31">
         <v>4</v>
@@ -5929,34 +5921,34 @@
         <v>0.83</v>
       </c>
       <c r="O94" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="AB94" s="16"/>
     </row>
     <row r="95" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="68"/>
+      <c r="A95" s="74"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C95" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D95" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E95" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F95" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="25"/>
-      <c r="H95" s="72"/>
+      <c r="H95" s="76"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5964,7 +5956,7 @@
         <v>0.25</v>
       </c>
       <c r="K95" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L95" s="31">
         <v>4</v>
@@ -5976,36 +5968,36 @@
         <v>0.83</v>
       </c>
       <c r="O95" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="P95" s="24"/>
       <c r="Q95" s="24"/>
       <c r="AB95" s="16"/>
     </row>
     <row r="96" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="68"/>
+      <c r="A96" s="74"/>
       <c r="B96" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C96" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D96" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E96" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F96" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="25"/>
-      <c r="H96" s="72"/>
+      <c r="H96" s="76"/>
       <c r="I96" s="42" t="s">
         <v>57</v>
       </c>
@@ -6013,7 +6005,7 @@
         <v>0.25</v>
       </c>
       <c r="K96" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L96" s="31">
         <v>4</v>
@@ -6025,36 +6017,36 @@
         <v>0.83</v>
       </c>
       <c r="O96" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="P96" s="24"/>
       <c r="Q96" s="24"/>
       <c r="AB96" s="16"/>
     </row>
     <row r="97" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="68"/>
+      <c r="A97" s="74"/>
       <c r="B97" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C97" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D97" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E97" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F97" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="24"/>
-      <c r="H97" s="72"/>
+      <c r="H97" s="76"/>
       <c r="I97" s="42" t="s">
         <v>58</v>
       </c>
@@ -6062,7 +6054,7 @@
         <v>0.25</v>
       </c>
       <c r="K97" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L97" s="31">
         <v>4</v>
@@ -6074,36 +6066,36 @@
         <v>0.83</v>
       </c>
       <c r="O97" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="P97" s="24"/>
       <c r="Q97" s="24"/>
       <c r="AB97" s="16"/>
     </row>
     <row r="98" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="68"/>
+      <c r="A98" s="74"/>
       <c r="B98" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C98" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D98" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E98" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F98" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="24"/>
-      <c r="H98" s="72"/>
+      <c r="H98" s="76"/>
       <c r="I98" s="42" t="s">
         <v>59</v>
       </c>
@@ -6111,7 +6103,7 @@
         <v>0.25</v>
       </c>
       <c r="K98" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L98" s="31">
         <v>4</v>
@@ -6123,35 +6115,35 @@
         <v>0.83</v>
       </c>
       <c r="O98" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="P98" s="24"/>
       <c r="Q98" s="24"/>
     </row>
     <row r="99" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A99" s="68"/>
+      <c r="A99" s="74"/>
       <c r="B99" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C99" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D99" s="27">
-        <f t="shared" si="5"/>
-        <v>0.21052631578947367</v>
+        <f t="shared" si="11"/>
+        <v>0.25773195876288663</v>
       </c>
       <c r="E99" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="F99" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="24"/>
-      <c r="H99" s="73"/>
+      <c r="H99" s="77"/>
       <c r="I99" s="42" t="s">
         <v>60</v>
       </c>
@@ -6159,7 +6151,7 @@
         <v>0.25</v>
       </c>
       <c r="K99" s="31">
-        <v>4.75</v>
+        <v>3.88</v>
       </c>
       <c r="L99" s="31">
         <v>4</v>
@@ -6171,22 +6163,22 @@
         <v>0.83</v>
       </c>
       <c r="O99" s="31">
-        <f t="shared" si="7"/>
-        <v>10.58</v>
+        <f t="shared" si="13"/>
+        <v>9.7099999999999991</v>
       </c>
       <c r="P99" s="24"/>
       <c r="Q99" s="24"/>
     </row>
     <row r="100" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="24"/>
-      <c r="B100" s="67"/>
+      <c r="B100" s="62"/>
       <c r="C100" s="24"/>
       <c r="D100" s="24"/>
       <c r="E100" s="24"/>
       <c r="F100" s="24"/>
       <c r="G100" s="24"/>
       <c r="H100" s="24"/>
-      <c r="I100" s="67"/>
+      <c r="I100" s="62"/>
       <c r="J100" s="24"/>
       <c r="K100" s="24"/>
       <c r="L100" s="24"/>
@@ -6197,7 +6189,7 @@
       <c r="Q100" s="24"/>
     </row>
     <row r="101" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="71" t="s">
+      <c r="A101" s="75" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6208,19 +6200,19 @@
         <v>4</v>
       </c>
       <c r="D101" s="27">
-        <f t="shared" ref="D101:F116" si="8">1/K101</f>
+        <f t="shared" ref="D101:F116" si="14">1/K101</f>
         <v>0.17035775127768313</v>
       </c>
       <c r="E101" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F101" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="24"/>
-      <c r="H101" s="71" t="s">
+      <c r="H101" s="75" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6249,28 +6241,28 @@
       <c r="Q101" s="24"/>
     </row>
     <row r="102" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="72"/>
+      <c r="A102" s="76"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C102" s="27">
-        <f t="shared" ref="C102:C116" si="9">1/J102</f>
+        <f t="shared" ref="C102:C116" si="15">1/J102</f>
         <v>4</v>
       </c>
       <c r="D102" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E102" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F102" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="24"/>
-      <c r="H102" s="72"/>
+      <c r="H102" s="76"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6290,35 +6282,35 @@
         <v>0.83</v>
       </c>
       <c r="O102" s="31">
-        <f t="shared" ref="O102:O116" si="10">SUM(J102:N102)</f>
+        <f t="shared" ref="O102:O116" si="16">SUM(J102:N102)</f>
         <v>13.270000000000001</v>
       </c>
       <c r="P102" s="24"/>
       <c r="Q102" s="24"/>
     </row>
     <row r="103" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="72"/>
+      <c r="A103" s="76"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D103" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E103" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F103" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="24"/>
-      <c r="H103" s="72"/>
+      <c r="H103" s="76"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6338,35 +6330,35 @@
         <v>0.83</v>
       </c>
       <c r="O103" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P103" s="24"/>
       <c r="Q103" s="24"/>
     </row>
     <row r="104" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="72"/>
+      <c r="A104" s="76"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D104" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E104" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F104" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="24"/>
-      <c r="H104" s="72"/>
+      <c r="H104" s="76"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6386,35 +6378,35 @@
         <v>0.83</v>
       </c>
       <c r="O104" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P104" s="24"/>
       <c r="Q104" s="24"/>
     </row>
     <row r="105" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="72"/>
+      <c r="A105" s="76"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D105" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E105" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F105" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="24"/>
-      <c r="H105" s="72"/>
+      <c r="H105" s="76"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6434,35 +6426,35 @@
         <v>0.83</v>
       </c>
       <c r="O105" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P105" s="24"/>
       <c r="Q105" s="24"/>
     </row>
     <row r="106" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="72"/>
+      <c r="A106" s="76"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C106" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D106" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E106" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F106" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="24"/>
-      <c r="H106" s="72"/>
+      <c r="H106" s="76"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6482,35 +6474,35 @@
         <v>0.83</v>
       </c>
       <c r="O106" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P106" s="24"/>
       <c r="Q106" s="24"/>
     </row>
     <row r="107" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="72"/>
+      <c r="A107" s="76"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D107" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E107" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F107" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="24"/>
-      <c r="H107" s="72"/>
+      <c r="H107" s="76"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6530,35 +6522,35 @@
         <v>0.83</v>
       </c>
       <c r="O107" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P107" s="24"/>
       <c r="Q107" s="24"/>
     </row>
     <row r="108" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="72"/>
+      <c r="A108" s="76"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C108" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D108" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E108" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F108" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="24"/>
-      <c r="H108" s="72"/>
+      <c r="H108" s="76"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6578,35 +6570,35 @@
         <v>0.83</v>
       </c>
       <c r="O108" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P108" s="24"/>
       <c r="Q108" s="24"/>
     </row>
     <row r="109" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A109" s="72"/>
+      <c r="A109" s="76"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C109" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D109" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E109" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F109" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="24"/>
-      <c r="H109" s="72"/>
+      <c r="H109" s="76"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6626,35 +6618,35 @@
         <v>0.83</v>
       </c>
       <c r="O109" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P109" s="24"/>
       <c r="Q109" s="24"/>
     </row>
     <row r="110" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="72"/>
+      <c r="A110" s="76"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C110" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D110" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E110" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F110" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="24"/>
-      <c r="H110" s="72"/>
+      <c r="H110" s="76"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6674,35 +6666,35 @@
         <v>0.83</v>
       </c>
       <c r="O110" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P110" s="24"/>
       <c r="Q110" s="24"/>
     </row>
     <row r="111" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="72"/>
+      <c r="A111" s="76"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C111" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D111" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E111" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F111" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="24"/>
-      <c r="H111" s="72"/>
+      <c r="H111" s="76"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6710,7 +6702,7 @@
         <v>0.25</v>
       </c>
       <c r="K111" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L111" s="31">
         <v>4</v>
@@ -6722,35 +6714,35 @@
         <v>0.83</v>
       </c>
       <c r="O111" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P111" s="24"/>
       <c r="Q111" s="24"/>
     </row>
     <row r="112" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="72"/>
+      <c r="A112" s="76"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C112" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D112" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E112" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F112" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="24"/>
-      <c r="H112" s="72"/>
+      <c r="H112" s="76"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6758,7 +6750,7 @@
         <v>0.25</v>
       </c>
       <c r="K112" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L112" s="31">
         <v>4</v>
@@ -6770,35 +6762,35 @@
         <v>0.83</v>
       </c>
       <c r="O112" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P112" s="24"/>
       <c r="Q112" s="24"/>
     </row>
     <row r="113" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A113" s="72"/>
+      <c r="A113" s="76"/>
       <c r="B113" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C113" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D113" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E113" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F113" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="24"/>
-      <c r="H113" s="72"/>
+      <c r="H113" s="76"/>
       <c r="I113" s="42" t="s">
         <v>57</v>
       </c>
@@ -6806,7 +6798,7 @@
         <v>0.25</v>
       </c>
       <c r="K113" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L113" s="31">
         <v>4</v>
@@ -6818,35 +6810,35 @@
         <v>0.83</v>
       </c>
       <c r="O113" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P113" s="24"/>
       <c r="Q113" s="24"/>
     </row>
     <row r="114" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="72"/>
+      <c r="A114" s="76"/>
       <c r="B114" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C114" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D114" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E114" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F114" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="24"/>
-      <c r="H114" s="72"/>
+      <c r="H114" s="76"/>
       <c r="I114" s="42" t="s">
         <v>58</v>
       </c>
@@ -6854,7 +6846,7 @@
         <v>0.25</v>
       </c>
       <c r="K114" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L114" s="31">
         <v>4</v>
@@ -6866,35 +6858,35 @@
         <v>0.83</v>
       </c>
       <c r="O114" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P114" s="24"/>
       <c r="Q114" s="24"/>
     </row>
     <row r="115" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="72"/>
+      <c r="A115" s="76"/>
       <c r="B115" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C115" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D115" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E115" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F115" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="24"/>
-      <c r="H115" s="72"/>
+      <c r="H115" s="76"/>
       <c r="I115" s="42" t="s">
         <v>59</v>
       </c>
@@ -6902,7 +6894,7 @@
         <v>0.25</v>
       </c>
       <c r="K115" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L115" s="31">
         <v>4</v>
@@ -6914,35 +6906,35 @@
         <v>0.83</v>
       </c>
       <c r="O115" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P115" s="24"/>
       <c r="Q115" s="24"/>
     </row>
     <row r="116" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="73"/>
+      <c r="A116" s="77"/>
       <c r="B116" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C116" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="D116" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17889087656529518</v>
+        <f t="shared" si="14"/>
+        <v>0.24213075060532688</v>
       </c>
       <c r="E116" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F116" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="16"/>
-      <c r="H116" s="73"/>
+      <c r="H116" s="77"/>
       <c r="I116" s="42" t="s">
         <v>60</v>
       </c>
@@ -6950,7 +6942,7 @@
         <v>0.25</v>
       </c>
       <c r="K116" s="31">
-        <v>5.59</v>
+        <v>4.13</v>
       </c>
       <c r="L116" s="31">
         <v>4</v>
@@ -6962,15 +6954,15 @@
         <v>0.83</v>
       </c>
       <c r="O116" s="31">
-        <f t="shared" si="10"/>
-        <v>11.42</v>
+        <f t="shared" si="16"/>
+        <v>9.9599999999999991</v>
       </c>
       <c r="P116" s="24"/>
       <c r="Q116" s="24"/>
     </row>
     <row r="117" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H117" s="74"/>
-      <c r="I117" s="67"/>
+      <c r="H117" s="65"/>
+      <c r="I117" s="62"/>
       <c r="J117" s="25"/>
       <c r="K117" s="25"/>
       <c r="L117" s="25"/>
@@ -6981,8 +6973,8 @@
       <c r="Q117" s="24"/>
     </row>
     <row r="118" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H118" s="74"/>
-      <c r="I118" s="67"/>
+      <c r="H118" s="65"/>
+      <c r="I118" s="62"/>
       <c r="J118" s="25"/>
       <c r="K118" s="25"/>
       <c r="L118" s="25"/>
@@ -6993,8 +6985,8 @@
       <c r="Q118" s="24"/>
     </row>
     <row r="119" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H119" s="74"/>
-      <c r="I119" s="67"/>
+      <c r="H119" s="65"/>
+      <c r="I119" s="62"/>
       <c r="J119" s="25"/>
       <c r="K119" s="25"/>
       <c r="L119" s="25"/>
@@ -7005,8 +6997,8 @@
       <c r="Q119" s="24"/>
     </row>
     <row r="120" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="H120" s="74"/>
-      <c r="I120" s="67"/>
+      <c r="H120" s="65"/>
+      <c r="I120" s="62"/>
       <c r="J120" s="25"/>
       <c r="K120" s="25"/>
       <c r="L120" s="25"/>
@@ -7098,11 +7090,11 @@
         <v>3</v>
       </c>
       <c r="B124" s="3">
-        <f t="shared" ref="B124:B138" si="11">-LN(0.94)</f>
+        <f t="shared" ref="B124:B138" si="17">-LN(0.94)</f>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C124" s="3">
-        <f t="shared" ref="C124:C138" si="12">-LN(0.94)</f>
+        <f t="shared" ref="C124:C138" si="18">-LN(0.94)</f>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D124" s="3">
@@ -7127,11 +7119,11 @@
         <v>4</v>
       </c>
       <c r="B125" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C125" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D125" s="3">
@@ -7156,11 +7148,11 @@
         <v>5</v>
       </c>
       <c r="B126" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C126" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D126" s="3">
@@ -7185,11 +7177,11 @@
         <v>6</v>
       </c>
       <c r="B127" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C127" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D127" s="3">
@@ -7214,11 +7206,11 @@
         <v>7</v>
       </c>
       <c r="B128" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C128" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D128" s="3">
@@ -7243,11 +7235,11 @@
         <v>13</v>
       </c>
       <c r="B129" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C129" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D129" s="3">
@@ -7272,11 +7264,11 @@
         <v>8</v>
       </c>
       <c r="B130" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C130" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D130" s="3">
@@ -7301,11 +7293,11 @@
         <v>9</v>
       </c>
       <c r="B131" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C131" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D131" s="3">
@@ -7330,11 +7322,11 @@
         <v>10</v>
       </c>
       <c r="B132" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C132" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D132" s="3">
@@ -7359,11 +7351,11 @@
         <v>11</v>
       </c>
       <c r="B133" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C133" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D133" s="3">
@@ -7388,11 +7380,11 @@
         <v>12</v>
       </c>
       <c r="B134" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C134" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D134" s="3">
@@ -7417,11 +7409,11 @@
         <v>57</v>
       </c>
       <c r="B135" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C135" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D135" s="3">
@@ -7446,11 +7438,11 @@
         <v>58</v>
       </c>
       <c r="B136" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C136" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D136" s="3">
@@ -7475,11 +7467,11 @@
         <v>59</v>
       </c>
       <c r="B137" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C137" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D137" s="3">
@@ -7504,11 +7496,11 @@
         <v>60</v>
       </c>
       <c r="B138" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C138" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D138" s="3">
@@ -7666,10 +7658,10 @@
       <c r="Q145" s="24"/>
     </row>
     <row r="146" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="60" t="s">
+      <c r="A146" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B146" s="61"/>
+      <c r="B146" s="70"/>
       <c r="C146" s="24"/>
       <c r="D146" s="24"/>
       <c r="E146" s="24"/>
@@ -7775,10 +7767,10 @@
       <c r="Q150" s="24"/>
     </row>
     <row r="151" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="62" t="s">
+      <c r="A151" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="B151" s="62"/>
+      <c r="B151" s="73"/>
       <c r="C151" s="24"/>
       <c r="D151" s="24"/>
       <c r="E151" s="24"/>
@@ -8083,27 +8075,27 @@
         <v>40</v>
       </c>
       <c r="K164" s="22">
-        <f t="shared" ref="K164:P164" si="13">$B$164*B167</f>
+        <f t="shared" ref="K164:P164" si="19">$B$164*B167</f>
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="L164" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="M164" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3.4799999999999996E-3</v>
       </c>
       <c r="N164" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>4.1399999999999996E-3</v>
       </c>
       <c r="O164" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>7.1399999999999996E-3</v>
       </c>
       <c r="P164" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.3999999999999997E-5</v>
       </c>
       <c r="Q164" s="24"/>
@@ -8122,27 +8114,27 @@
         <v>31</v>
       </c>
       <c r="K165" s="31">
-        <f t="shared" ref="K165:P165" si="14">$C$164*B167</f>
+        <f t="shared" ref="K165:P165" si="20">$C$164*B167</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L165" s="31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.01</v>
       </c>
       <c r="M165" s="31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>5.7999999999999996E-2</v>
       </c>
       <c r="N165" s="31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="O165" s="31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0.11900000000000001</v>
       </c>
       <c r="P165" s="31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="Q165" s="24"/>
@@ -8175,27 +8167,27 @@
         <v>32</v>
       </c>
       <c r="K166" s="31">
-        <f t="shared" ref="K166:P166" si="15">MIN($D$164*B167,1)</f>
+        <f t="shared" ref="K166:P166" si="21">MIN($D$164*B167,1)</f>
         <v>0.98000000000000009</v>
       </c>
       <c r="L166" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M166" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.81200000000000006</v>
       </c>
       <c r="N166" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0.96600000000000019</v>
       </c>
       <c r="O166" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="P166" s="31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>5.6000000000000008E-3</v>
       </c>
       <c r="Q166" s="24"/>
@@ -8222,7 +8214,7 @@
       <c r="G167" s="3">
         <v>0.04</v>
       </c>
-      <c r="H167" s="66"/>
+      <c r="H167" s="61"/>
       <c r="I167" s="24"/>
       <c r="J167" s="24" t="s">
         <v>41</v>
@@ -8564,6 +8556,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="A84:A99"/>
+    <mergeCell ref="A101:A116"/>
     <mergeCell ref="J82:N82"/>
     <mergeCell ref="H84:H99"/>
     <mergeCell ref="H101:H116"/>
@@ -8572,14 +8572,6 @@
     <mergeCell ref="A62:A77"/>
     <mergeCell ref="H62:H77"/>
     <mergeCell ref="H45:H60"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="A84:A99"/>
-    <mergeCell ref="A101:A116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update CD4 and VL transition rates. Update baseline transmission rates to be different for males and females.
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25310" windowHeight="10820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -475,7 +475,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +491,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3399"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -759,7 +753,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2488,8 +2481,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AX187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R104" sqref="R104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3678,10 +3671,10 @@
     </row>
     <row r="42" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="25"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="24"/>
       <c r="J42" s="23"/>
       <c r="K42" s="23"/>
@@ -3695,22 +3688,22 @@
     <row r="43" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="31"/>
       <c r="B43" s="63"/>
-      <c r="C43" s="71" t="s">
+      <c r="C43" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="70"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="69"/>
       <c r="G43" s="60"/>
       <c r="H43" s="31"/>
       <c r="I43" s="66"/>
-      <c r="J43" s="69" t="s">
+      <c r="J43" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="69"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="70"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="69"/>
       <c r="O43" s="31"/>
     </row>
     <row r="44" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
@@ -3760,7 +3753,7 @@
       <c r="AX44" s="18"/>
     </row>
     <row r="45" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="74" t="s">
+      <c r="A45" s="73" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3772,18 +3765,18 @@
       </c>
       <c r="D45" s="27">
         <f>1/K45</f>
-        <v>1.8181818181818181</v>
+        <v>4</v>
       </c>
       <c r="E45" s="27">
         <f t="shared" ref="E45:E60" si="3">1/L45</f>
-        <v>0.25188916876574308</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F45" s="27">
         <f t="shared" ref="F45:F60" si="4">1/M45</f>
-        <v>0.19880715705765406</v>
+        <v>0.21413276231263384</v>
       </c>
       <c r="G45" s="25"/>
-      <c r="H45" s="75" t="s">
+      <c r="H45" s="74" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -3793,25 +3786,25 @@
         <v>0.25</v>
       </c>
       <c r="K45" s="31">
-        <v>0.55000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="L45" s="31">
-        <v>3.97</v>
+        <v>3.56</v>
       </c>
       <c r="M45" s="31">
-        <v>5.03</v>
+        <v>4.67</v>
       </c>
       <c r="N45" s="31">
         <v>2.13</v>
       </c>
       <c r="O45" s="31">
         <f>SUM(J45:N45)</f>
-        <v>11.93</v>
+        <v>10.86</v>
       </c>
       <c r="AX45" s="17"/>
     </row>
     <row r="46" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="74"/>
+      <c r="A46" s="73"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3819,19 +3812,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D46" s="68">
+      <c r="D46" s="27">
+        <f t="shared" ref="D46:D60" si="5">1/K46</f>
         <v>4</v>
       </c>
       <c r="E46" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F46" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="25"/>
-      <c r="H46" s="76"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3839,10 +3833,10 @@
         <v>0.25</v>
       </c>
       <c r="K46" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L46" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M46" s="31">
         <v>4.67</v>
@@ -3851,13 +3845,13 @@
         <v>3.7</v>
       </c>
       <c r="O46" s="31">
-        <f t="shared" ref="O46:O60" si="5">SUM(J46:N46)</f>
+        <f t="shared" ref="O46:O60" si="6">SUM(J46:N46)</f>
         <v>12.43</v>
       </c>
       <c r="AX46" s="11"/>
     </row>
     <row r="47" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="74"/>
+      <c r="A47" s="73"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3865,19 +3859,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D47" s="68">
+      <c r="D47" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E47" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F47" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="25"/>
-      <c r="H47" s="76"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3885,10 +3880,10 @@
         <v>0.25</v>
       </c>
       <c r="K47" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L47" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M47" s="31">
         <v>4.67</v>
@@ -3897,13 +3892,13 @@
         <v>3.7</v>
       </c>
       <c r="O47" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
       <c r="AX47" s="11"/>
     </row>
     <row r="48" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="74"/>
+      <c r="A48" s="73"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3911,19 +3906,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D48" s="68">
+      <c r="D48" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E48" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F48" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="25"/>
-      <c r="H48" s="76"/>
+      <c r="H48" s="75"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3931,10 +3927,10 @@
         <v>0.25</v>
       </c>
       <c r="K48" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L48" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M48" s="31">
         <v>4.67</v>
@@ -3943,13 +3939,13 @@
         <v>3.7</v>
       </c>
       <c r="O48" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
       <c r="AX48" s="11"/>
     </row>
     <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="74"/>
+      <c r="A49" s="73"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3957,19 +3953,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D49" s="68">
+      <c r="D49" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E49" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F49" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="25"/>
-      <c r="H49" s="76"/>
+      <c r="H49" s="75"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3977,10 +3974,10 @@
         <v>0.25</v>
       </c>
       <c r="K49" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L49" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M49" s="31">
         <v>4.67</v>
@@ -3989,12 +3986,12 @@
         <v>3.7</v>
       </c>
       <c r="O49" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="74"/>
+      <c r="A50" s="73"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4002,19 +3999,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D50" s="68">
+      <c r="D50" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E50" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F50" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="25"/>
-      <c r="H50" s="76"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4022,10 +4020,10 @@
         <v>0.25</v>
       </c>
       <c r="K50" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L50" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M50" s="31">
         <v>4.67</v>
@@ -4034,12 +4032,12 @@
         <v>3.7</v>
       </c>
       <c r="O50" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="74"/>
+      <c r="A51" s="73"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4047,19 +4045,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D51" s="68">
+      <c r="D51" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E51" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F51" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="25"/>
-      <c r="H51" s="76"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4067,10 +4066,10 @@
         <v>0.25</v>
       </c>
       <c r="K51" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L51" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M51" s="31">
         <v>4.67</v>
@@ -4079,12 +4078,12 @@
         <v>3.7</v>
       </c>
       <c r="O51" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="74"/>
+      <c r="A52" s="73"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4092,19 +4091,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D52" s="68">
+      <c r="D52" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E52" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F52" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="25"/>
-      <c r="H52" s="76"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4112,10 +4112,10 @@
         <v>0.25</v>
       </c>
       <c r="K52" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L52" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M52" s="31">
         <v>4.67</v>
@@ -4124,12 +4124,12 @@
         <v>3.7</v>
       </c>
       <c r="O52" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="74"/>
+      <c r="A53" s="73"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4137,19 +4137,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D53" s="68">
+      <c r="D53" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E53" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F53" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="25"/>
-      <c r="H53" s="76"/>
+      <c r="H53" s="75"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4157,10 +4158,10 @@
         <v>0.25</v>
       </c>
       <c r="K53" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L53" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M53" s="31">
         <v>4.67</v>
@@ -4169,12 +4170,12 @@
         <v>3.7</v>
       </c>
       <c r="O53" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="74"/>
+      <c r="A54" s="73"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4182,19 +4183,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D54" s="68">
+      <c r="D54" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E54" s="27">
         <f t="shared" si="3"/>
-        <v>0.26246719160104987</v>
+        <v>0.2808988764044944</v>
       </c>
       <c r="F54" s="27">
         <f t="shared" si="4"/>
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="25"/>
-      <c r="H54" s="76"/>
+      <c r="H54" s="75"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4202,10 +4204,10 @@
         <v>0.25</v>
       </c>
       <c r="K54" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L54" s="31">
-        <v>3.81</v>
+        <v>3.56</v>
       </c>
       <c r="M54" s="31">
         <v>4.67</v>
@@ -4214,12 +4216,12 @@
         <v>3.7</v>
       </c>
       <c r="O54" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.43</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="74"/>
+      <c r="A55" s="73"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4227,19 +4229,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D55" s="68">
+      <c r="D55" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E55" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F55" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="25"/>
-      <c r="H55" s="76"/>
+      <c r="H55" s="75"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4247,10 +4250,10 @@
         <v>0.25</v>
       </c>
       <c r="K55" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L55" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M55" s="31">
         <v>4.51</v>
@@ -4259,12 +4262,12 @@
         <v>1.85</v>
       </c>
       <c r="O55" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="74"/>
+      <c r="A56" s="73"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4272,19 +4275,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D56" s="68">
+      <c r="D56" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E56" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F56" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="25"/>
-      <c r="H56" s="76"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4292,10 +4296,10 @@
         <v>0.25</v>
       </c>
       <c r="K56" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L56" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M56" s="31">
         <v>4.51</v>
@@ -4304,12 +4308,12 @@
         <v>1.85</v>
       </c>
       <c r="O56" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="74"/>
+      <c r="A57" s="73"/>
       <c r="B57" s="42" t="s">
         <v>57</v>
       </c>
@@ -4317,19 +4321,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D57" s="68">
+      <c r="D57" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E57" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F57" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="25"/>
-      <c r="H57" s="76"/>
+      <c r="H57" s="75"/>
       <c r="I57" s="42" t="s">
         <v>57</v>
       </c>
@@ -4337,10 +4342,10 @@
         <v>0.25</v>
       </c>
       <c r="K57" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L57" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M57" s="31">
         <v>4.51</v>
@@ -4349,12 +4354,12 @@
         <v>1.85</v>
       </c>
       <c r="O57" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="74"/>
+      <c r="A58" s="73"/>
       <c r="B58" s="42" t="s">
         <v>58</v>
       </c>
@@ -4362,19 +4367,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D58" s="68">
+      <c r="D58" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E58" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F58" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="H58" s="76"/>
+      <c r="H58" s="75"/>
       <c r="I58" s="42" t="s">
         <v>58</v>
       </c>
@@ -4382,10 +4388,10 @@
         <v>0.25</v>
       </c>
       <c r="K58" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L58" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M58" s="31">
         <v>4.51</v>
@@ -4394,12 +4400,12 @@
         <v>1.85</v>
       </c>
       <c r="O58" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="59" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="74"/>
+      <c r="A59" s="73"/>
       <c r="B59" s="42" t="s">
         <v>59</v>
       </c>
@@ -4407,19 +4413,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D59" s="68">
+      <c r="D59" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E59" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F59" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="H59" s="76"/>
+      <c r="H59" s="75"/>
       <c r="I59" s="42" t="s">
         <v>59</v>
       </c>
@@ -4427,10 +4434,10 @@
         <v>0.25</v>
       </c>
       <c r="K59" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L59" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M59" s="31">
         <v>4.51</v>
@@ -4439,12 +4446,12 @@
         <v>1.85</v>
       </c>
       <c r="O59" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
     <row r="60" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="74"/>
+      <c r="A60" s="73"/>
       <c r="B60" s="42" t="s">
         <v>60</v>
       </c>
@@ -4452,19 +4459,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D60" s="68">
+      <c r="D60" s="27">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E60" s="27">
         <f t="shared" si="3"/>
-        <v>0.32258064516129031</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="F60" s="27">
         <f t="shared" si="4"/>
         <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="H60" s="77"/>
+      <c r="H60" s="76"/>
       <c r="I60" s="42" t="s">
         <v>60</v>
       </c>
@@ -4472,10 +4480,10 @@
         <v>0.25</v>
       </c>
       <c r="K60" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L60" s="31">
-        <v>3.1</v>
+        <v>2.85</v>
       </c>
       <c r="M60" s="31">
         <v>4.51</v>
@@ -4484,7 +4492,7 @@
         <v>1.85</v>
       </c>
       <c r="O60" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.7099999999999991</v>
       </c>
     </row>
@@ -4506,30 +4514,30 @@
       <c r="O61" s="24"/>
     </row>
     <row r="62" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="75" t="s">
+      <c r="A62" s="74" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C62" s="27">
-        <f t="shared" ref="C62:C77" si="6">1/J62</f>
+        <f t="shared" ref="C62:C77" si="7">1/J62</f>
         <v>4</v>
       </c>
       <c r="D62" s="27">
         <f>1/K62</f>
-        <v>0.69930069930069938</v>
+        <v>1.075268817204301</v>
       </c>
       <c r="E62" s="27">
-        <f t="shared" ref="E62:E77" si="7">1/L62</f>
-        <v>0.25125628140703515</v>
+        <f t="shared" ref="E62:E77" si="8">1/L62</f>
+        <v>0.26954177897574122</v>
       </c>
       <c r="F62" s="27">
-        <f t="shared" ref="F62:F77" si="8">1/M62</f>
-        <v>0.25575447570332482</v>
+        <f t="shared" ref="F62:F77" si="9">1/M62</f>
+        <v>0.21367521367521369</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="H62" s="75" t="s">
+      <c r="H62" s="74" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -4539,13 +4547,13 @@
         <v>0.25</v>
       </c>
       <c r="K62" s="31">
-        <v>1.43</v>
+        <v>0.93</v>
       </c>
       <c r="L62" s="31">
-        <v>3.98</v>
+        <v>3.71</v>
       </c>
       <c r="M62" s="31">
-        <v>3.91</v>
+        <v>4.68</v>
       </c>
       <c r="N62" s="31">
         <v>2.13</v>
@@ -4556,28 +4564,28 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="76"/>
+      <c r="A63" s="75"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C63" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D63" s="27">
-        <f t="shared" ref="D63:D77" si="9">1/K63</f>
+        <f t="shared" ref="D63:D77" si="10">1/K63</f>
         <v>1.075268817204301</v>
       </c>
       <c r="E63" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.26954177897574122</v>
       </c>
       <c r="F63" s="27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="25"/>
-      <c r="H63" s="76"/>
+      <c r="H63" s="75"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4597,33 +4605,33 @@
         <v>3.7</v>
       </c>
       <c r="O63" s="31">
-        <f t="shared" ref="O63:O77" si="10">SUM(J63:N63)</f>
+        <f t="shared" ref="O63:O77" si="11">SUM(J63:N63)</f>
         <v>13.27</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="76"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C64" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D64" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E64" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F64" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E64" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F64" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="25"/>
-      <c r="H64" s="76"/>
+      <c r="H64" s="75"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4643,33 +4651,33 @@
         <v>3.7</v>
       </c>
       <c r="O64" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="65" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="76"/>
+      <c r="A65" s="75"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D65" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E65" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F65" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E65" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F65" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="25"/>
-      <c r="H65" s="76"/>
+      <c r="H65" s="75"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4689,33 +4697,33 @@
         <v>3.7</v>
       </c>
       <c r="O65" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="66" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="76"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D66" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E66" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F66" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E66" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F66" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="25"/>
-      <c r="H66" s="76"/>
+      <c r="H66" s="75"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4735,33 +4743,33 @@
         <v>3.7</v>
       </c>
       <c r="O66" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="67" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="76"/>
+      <c r="A67" s="75"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D67" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E67" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F67" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E67" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F67" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="25"/>
-      <c r="H67" s="76"/>
+      <c r="H67" s="75"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4781,33 +4789,33 @@
         <v>3.7</v>
       </c>
       <c r="O67" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="68" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="76"/>
+      <c r="A68" s="75"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C68" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D68" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E68" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F68" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E68" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F68" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="25"/>
-      <c r="H68" s="76"/>
+      <c r="H68" s="75"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4827,33 +4835,33 @@
         <v>3.7</v>
       </c>
       <c r="O68" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="69" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="76"/>
+      <c r="A69" s="75"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D69" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E69" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F69" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E69" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F69" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="25"/>
-      <c r="H69" s="76"/>
+      <c r="H69" s="75"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4873,33 +4881,33 @@
         <v>3.7</v>
       </c>
       <c r="O69" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="70" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="76"/>
+      <c r="A70" s="75"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C70" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D70" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E70" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F70" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E70" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F70" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="25"/>
-      <c r="H70" s="76"/>
+      <c r="H70" s="75"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4919,33 +4927,33 @@
         <v>3.7</v>
       </c>
       <c r="O70" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="71" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="76"/>
+      <c r="A71" s="75"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D71" s="27">
+        <f t="shared" si="10"/>
+        <v>1.075268817204301</v>
+      </c>
+      <c r="E71" s="27">
+        <f t="shared" si="8"/>
+        <v>0.26954177897574122</v>
+      </c>
+      <c r="F71" s="27">
         <f t="shared" si="9"/>
-        <v>1.075268817204301</v>
-      </c>
-      <c r="E71" s="27">
-        <f t="shared" si="7"/>
-        <v>0.26954177897574122</v>
-      </c>
-      <c r="F71" s="27">
-        <f t="shared" si="8"/>
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="25"/>
-      <c r="H71" s="76"/>
+      <c r="H71" s="75"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4965,33 +4973,33 @@
         <v>3.7</v>
       </c>
       <c r="O71" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13.27</v>
       </c>
     </row>
     <row r="72" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="76"/>
+      <c r="A72" s="75"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C72" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D72" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E72" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F72" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E72" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F72" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="25"/>
-      <c r="H72" s="76"/>
+      <c r="H72" s="75"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5011,33 +5019,33 @@
         <v>1.85</v>
       </c>
       <c r="O72" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="76"/>
+      <c r="A73" s="75"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D73" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E73" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F73" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E73" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F73" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="25"/>
-      <c r="H73" s="76"/>
+      <c r="H73" s="75"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5057,33 +5065,33 @@
         <v>1.85</v>
       </c>
       <c r="O73" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="74" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="76"/>
+      <c r="A74" s="75"/>
       <c r="B74" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C74" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D74" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E74" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F74" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E74" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F74" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="25"/>
-      <c r="H74" s="76"/>
+      <c r="H74" s="75"/>
       <c r="I74" s="42" t="s">
         <v>57</v>
       </c>
@@ -5103,33 +5111,33 @@
         <v>1.85</v>
       </c>
       <c r="O74" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="75" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="76"/>
+      <c r="A75" s="75"/>
       <c r="B75" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C75" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D75" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E75" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F75" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E75" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F75" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="25"/>
-      <c r="H75" s="76"/>
+      <c r="H75" s="75"/>
       <c r="I75" s="42" t="s">
         <v>58</v>
       </c>
@@ -5149,33 +5157,33 @@
         <v>1.85</v>
       </c>
       <c r="O75" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="76" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="76"/>
+      <c r="A76" s="75"/>
       <c r="B76" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C76" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D76" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E76" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F76" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E76" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F76" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="25"/>
-      <c r="H76" s="76"/>
+      <c r="H76" s="75"/>
       <c r="I76" s="42" t="s">
         <v>59</v>
       </c>
@@ -5195,33 +5203,33 @@
         <v>1.85</v>
       </c>
       <c r="O76" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="77" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="77"/>
+      <c r="A77" s="76"/>
       <c r="B77" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C77" s="27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D77" s="27">
+        <f t="shared" si="10"/>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="E77" s="27">
+        <f t="shared" si="8"/>
+        <v>0.29940119760479045</v>
+      </c>
+      <c r="F77" s="27">
         <f t="shared" si="9"/>
-        <v>3.4482758620689657</v>
-      </c>
-      <c r="E77" s="27">
-        <f t="shared" si="7"/>
-        <v>0.29940119760479045</v>
-      </c>
-      <c r="F77" s="27">
-        <f t="shared" si="8"/>
         <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="25"/>
-      <c r="H77" s="77"/>
+      <c r="H77" s="76"/>
       <c r="I77" s="42" t="s">
         <v>60</v>
       </c>
@@ -5241,7 +5249,7 @@
         <v>1.85</v>
       </c>
       <c r="O77" s="31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.9599999999999991</v>
       </c>
     </row>
@@ -5308,10 +5316,10 @@
     </row>
     <row r="81" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="24"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="72"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="71"/>
+      <c r="E81" s="71"/>
       <c r="F81" s="24"/>
       <c r="G81" s="55"/>
       <c r="H81" s="55"/>
@@ -5329,22 +5337,22 @@
     <row r="82" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="44"/>
       <c r="B82" s="44"/>
-      <c r="C82" s="78" t="s">
+      <c r="C82" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="D82" s="78"/>
-      <c r="E82" s="78"/>
-      <c r="F82" s="78"/>
+      <c r="D82" s="77"/>
+      <c r="E82" s="77"/>
+      <c r="F82" s="77"/>
       <c r="G82" s="25"/>
       <c r="H82" s="31"/>
       <c r="I82" s="66"/>
-      <c r="J82" s="69" t="s">
+      <c r="J82" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="K82" s="69"/>
-      <c r="L82" s="69"/>
-      <c r="M82" s="69"/>
-      <c r="N82" s="70"/>
+      <c r="K82" s="68"/>
+      <c r="L82" s="68"/>
+      <c r="M82" s="68"/>
+      <c r="N82" s="69"/>
       <c r="O82" s="31"/>
       <c r="P82" s="24"/>
       <c r="Q82" s="24"/>
@@ -5399,7 +5407,7 @@
       <c r="AB83" s="16"/>
     </row>
     <row r="84" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="74" t="s">
+      <c r="A84" s="73" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5410,19 +5418,19 @@
         <v>4</v>
       </c>
       <c r="D84" s="27">
-        <f t="shared" ref="D84:F99" si="11">1/K84</f>
-        <v>0.16393442622950821</v>
+        <f t="shared" ref="D84:F99" si="12">1/K84</f>
+        <v>0.19880715705765406</v>
       </c>
       <c r="E84" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F84" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="55"/>
-      <c r="H84" s="75" t="s">
+      <c r="H84" s="74" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5432,7 +5440,7 @@
         <v>0.25</v>
       </c>
       <c r="K84" s="31">
-        <v>6.1</v>
+        <v>5.03</v>
       </c>
       <c r="L84" s="31">
         <v>4</v>
@@ -5445,34 +5453,34 @@
       </c>
       <c r="O84" s="31">
         <f>SUM(J84:N84)</f>
-        <v>11.93</v>
+        <v>10.860000000000001</v>
       </c>
       <c r="Q84" s="24"/>
       <c r="AB84" s="16"/>
     </row>
     <row r="85" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="74"/>
+      <c r="A85" s="73"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C85" s="27">
-        <f t="shared" ref="C85:C99" si="12">1/J85</f>
+        <f t="shared" ref="C85:C99" si="13">1/J85</f>
         <v>4</v>
       </c>
       <c r="D85" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E85" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F85" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="55"/>
-      <c r="H85" s="76"/>
+      <c r="H85" s="75"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5492,35 +5500,35 @@
         <v>0.83</v>
       </c>
       <c r="O85" s="31">
-        <f t="shared" ref="O85:O99" si="13">SUM(J85:N85)</f>
+        <f t="shared" ref="O85:O99" si="14">SUM(J85:N85)</f>
         <v>12.43</v>
       </c>
       <c r="Q85" s="55"/>
       <c r="AB85" s="16"/>
     </row>
     <row r="86" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="74"/>
+      <c r="A86" s="73"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C86" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D86" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D86" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E86" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F86" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="55"/>
-      <c r="H86" s="76"/>
+      <c r="H86" s="75"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5540,35 +5548,35 @@
         <v>0.83</v>
       </c>
       <c r="O86" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="Q86" s="25"/>
       <c r="AB86" s="16"/>
     </row>
     <row r="87" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="74"/>
+      <c r="A87" s="73"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C87" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D87" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D87" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E87" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F87" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="25"/>
-      <c r="H87" s="76"/>
+      <c r="H87" s="75"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5588,35 +5596,35 @@
         <v>0.83</v>
       </c>
       <c r="O87" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="Q87" s="25"/>
       <c r="AB87" s="16"/>
     </row>
     <row r="88" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="74"/>
+      <c r="A88" s="73"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C88" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D88" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D88" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E88" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F88" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="55"/>
-      <c r="H88" s="76"/>
+      <c r="H88" s="75"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5636,35 +5644,35 @@
         <v>0.83</v>
       </c>
       <c r="O88" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="Q88" s="25"/>
       <c r="AB88" s="16"/>
     </row>
     <row r="89" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A89" s="74"/>
+      <c r="A89" s="73"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D89" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D89" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E89" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F89" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="25"/>
-      <c r="H89" s="76"/>
+      <c r="H89" s="75"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5684,7 +5692,7 @@
         <v>0.83</v>
       </c>
       <c r="O89" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="P89" s="24"/>
@@ -5692,28 +5700,28 @@
       <c r="AB89" s="16"/>
     </row>
     <row r="90" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="74"/>
+      <c r="A90" s="73"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D90" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D90" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E90" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F90" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="55"/>
-      <c r="H90" s="76"/>
+      <c r="H90" s="75"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5733,34 +5741,34 @@
         <v>0.83</v>
       </c>
       <c r="O90" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="AB90" s="16"/>
     </row>
     <row r="91" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A91" s="74"/>
+      <c r="A91" s="73"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C91" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D91" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D91" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E91" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F91" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="55"/>
-      <c r="H91" s="76"/>
+      <c r="H91" s="75"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5780,34 +5788,34 @@
         <v>0.83</v>
       </c>
       <c r="O91" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="AB91" s="16"/>
     </row>
     <row r="92" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="74"/>
+      <c r="A92" s="73"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C92" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D92" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D92" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E92" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F92" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="55"/>
-      <c r="H92" s="76"/>
+      <c r="H92" s="75"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5827,34 +5835,34 @@
         <v>0.83</v>
       </c>
       <c r="O92" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="AB92" s="16"/>
     </row>
     <row r="93" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="74"/>
+      <c r="A93" s="73"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C93" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D93" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D93" s="27">
-        <f t="shared" si="11"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="E93" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F93" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="55"/>
-      <c r="H93" s="76"/>
+      <c r="H93" s="75"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5874,34 +5882,34 @@
         <v>0.83</v>
       </c>
       <c r="O93" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12.43</v>
       </c>
       <c r="AB93" s="16"/>
     </row>
     <row r="94" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A94" s="74"/>
+      <c r="A94" s="73"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D94" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D94" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E94" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F94" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="25"/>
-      <c r="H94" s="76"/>
+      <c r="H94" s="75"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5921,34 +5929,34 @@
         <v>0.83</v>
       </c>
       <c r="O94" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="AB94" s="16"/>
     </row>
     <row r="95" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="74"/>
+      <c r="A95" s="73"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C95" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D95" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D95" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E95" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F95" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="25"/>
-      <c r="H95" s="76"/>
+      <c r="H95" s="75"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5968,7 +5976,7 @@
         <v>0.83</v>
       </c>
       <c r="O95" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="P95" s="24"/>
@@ -5976,28 +5984,28 @@
       <c r="AB95" s="16"/>
     </row>
     <row r="96" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="74"/>
+      <c r="A96" s="73"/>
       <c r="B96" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C96" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D96" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D96" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E96" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F96" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="25"/>
-      <c r="H96" s="76"/>
+      <c r="H96" s="75"/>
       <c r="I96" s="42" t="s">
         <v>57</v>
       </c>
@@ -6017,7 +6025,7 @@
         <v>0.83</v>
       </c>
       <c r="O96" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="P96" s="24"/>
@@ -6025,28 +6033,28 @@
       <c r="AB96" s="16"/>
     </row>
     <row r="97" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="74"/>
+      <c r="A97" s="73"/>
       <c r="B97" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C97" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D97" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D97" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E97" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F97" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="24"/>
-      <c r="H97" s="76"/>
+      <c r="H97" s="75"/>
       <c r="I97" s="42" t="s">
         <v>58</v>
       </c>
@@ -6066,7 +6074,7 @@
         <v>0.83</v>
       </c>
       <c r="O97" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="P97" s="24"/>
@@ -6074,28 +6082,28 @@
       <c r="AB97" s="16"/>
     </row>
     <row r="98" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="74"/>
+      <c r="A98" s="73"/>
       <c r="B98" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C98" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D98" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D98" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E98" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F98" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="24"/>
-      <c r="H98" s="76"/>
+      <c r="H98" s="75"/>
       <c r="I98" s="42" t="s">
         <v>59</v>
       </c>
@@ -6115,35 +6123,35 @@
         <v>0.83</v>
       </c>
       <c r="O98" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="P98" s="24"/>
       <c r="Q98" s="24"/>
     </row>
     <row r="99" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A99" s="74"/>
+      <c r="A99" s="73"/>
       <c r="B99" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C99" s="27">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="D99" s="27">
         <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="D99" s="27">
-        <f t="shared" si="11"/>
         <v>0.25773195876288663</v>
       </c>
       <c r="E99" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="F99" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="24"/>
-      <c r="H99" s="77"/>
+      <c r="H99" s="76"/>
       <c r="I99" s="42" t="s">
         <v>60</v>
       </c>
@@ -6163,7 +6171,7 @@
         <v>0.83</v>
       </c>
       <c r="O99" s="31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7099999999999991</v>
       </c>
       <c r="P99" s="24"/>
@@ -6189,7 +6197,7 @@
       <c r="Q100" s="24"/>
     </row>
     <row r="101" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="75" t="s">
+      <c r="A101" s="74" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6200,19 +6208,19 @@
         <v>4</v>
       </c>
       <c r="D101" s="27">
-        <f t="shared" ref="D101:F116" si="14">1/K101</f>
+        <f t="shared" ref="D101:F116" si="15">1/K101</f>
         <v>0.17035775127768313</v>
       </c>
       <c r="E101" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F101" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="24"/>
-      <c r="H101" s="75" t="s">
+      <c r="H101" s="74" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6241,28 +6249,28 @@
       <c r="Q101" s="24"/>
     </row>
     <row r="102" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="76"/>
+      <c r="A102" s="75"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C102" s="27">
-        <f t="shared" ref="C102:C116" si="15">1/J102</f>
+        <f t="shared" ref="C102:C116" si="16">1/J102</f>
         <v>4</v>
       </c>
       <c r="D102" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E102" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F102" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="24"/>
-      <c r="H102" s="76"/>
+      <c r="H102" s="75"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6282,35 +6290,35 @@
         <v>0.83</v>
       </c>
       <c r="O102" s="31">
-        <f t="shared" ref="O102:O116" si="16">SUM(J102:N102)</f>
+        <f t="shared" ref="O102:O116" si="17">SUM(J102:N102)</f>
         <v>13.270000000000001</v>
       </c>
       <c r="P102" s="24"/>
       <c r="Q102" s="24"/>
     </row>
     <row r="103" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="76"/>
+      <c r="A103" s="75"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D103" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D103" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F103" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="24"/>
-      <c r="H103" s="76"/>
+      <c r="H103" s="75"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6330,35 +6338,35 @@
         <v>0.83</v>
       </c>
       <c r="O103" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P103" s="24"/>
       <c r="Q103" s="24"/>
     </row>
     <row r="104" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="76"/>
+      <c r="A104" s="75"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D104" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D104" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E104" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F104" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="24"/>
-      <c r="H104" s="76"/>
+      <c r="H104" s="75"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6378,35 +6386,35 @@
         <v>0.83</v>
       </c>
       <c r="O104" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P104" s="24"/>
       <c r="Q104" s="24"/>
     </row>
     <row r="105" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="76"/>
+      <c r="A105" s="75"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D105" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D105" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E105" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F105" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="24"/>
-      <c r="H105" s="76"/>
+      <c r="H105" s="75"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6426,35 +6434,35 @@
         <v>0.83</v>
       </c>
       <c r="O105" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P105" s="24"/>
       <c r="Q105" s="24"/>
     </row>
     <row r="106" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="76"/>
+      <c r="A106" s="75"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C106" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D106" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D106" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E106" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F106" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="24"/>
-      <c r="H106" s="76"/>
+      <c r="H106" s="75"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6474,35 +6482,35 @@
         <v>0.83</v>
       </c>
       <c r="O106" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P106" s="24"/>
       <c r="Q106" s="24"/>
     </row>
     <row r="107" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="76"/>
+      <c r="A107" s="75"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D107" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D107" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E107" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F107" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="24"/>
-      <c r="H107" s="76"/>
+      <c r="H107" s="75"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6522,35 +6530,35 @@
         <v>0.83</v>
       </c>
       <c r="O107" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P107" s="24"/>
       <c r="Q107" s="24"/>
     </row>
     <row r="108" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="76"/>
+      <c r="A108" s="75"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C108" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D108" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D108" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E108" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F108" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="24"/>
-      <c r="H108" s="76"/>
+      <c r="H108" s="75"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6570,35 +6578,35 @@
         <v>0.83</v>
       </c>
       <c r="O108" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P108" s="24"/>
       <c r="Q108" s="24"/>
     </row>
     <row r="109" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A109" s="76"/>
+      <c r="A109" s="75"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C109" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D109" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D109" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E109" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F109" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="24"/>
-      <c r="H109" s="76"/>
+      <c r="H109" s="75"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6618,35 +6626,35 @@
         <v>0.83</v>
       </c>
       <c r="O109" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P109" s="24"/>
       <c r="Q109" s="24"/>
     </row>
     <row r="110" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="76"/>
+      <c r="A110" s="75"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C110" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D110" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D110" s="27">
-        <f t="shared" si="14"/>
         <v>0.13440860215053763</v>
       </c>
       <c r="E110" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F110" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="24"/>
-      <c r="H110" s="76"/>
+      <c r="H110" s="75"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6666,35 +6674,35 @@
         <v>0.83</v>
       </c>
       <c r="O110" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13.270000000000001</v>
       </c>
       <c r="P110" s="24"/>
       <c r="Q110" s="24"/>
     </row>
     <row r="111" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="76"/>
+      <c r="A111" s="75"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C111" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D111" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D111" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E111" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F111" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="24"/>
-      <c r="H111" s="76"/>
+      <c r="H111" s="75"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6714,35 +6722,35 @@
         <v>0.83</v>
       </c>
       <c r="O111" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P111" s="24"/>
       <c r="Q111" s="24"/>
     </row>
     <row r="112" spans="1:28" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="76"/>
+      <c r="A112" s="75"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C112" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D112" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D112" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E112" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F112" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="24"/>
-      <c r="H112" s="76"/>
+      <c r="H112" s="75"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6762,35 +6770,35 @@
         <v>0.83</v>
       </c>
       <c r="O112" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P112" s="24"/>
       <c r="Q112" s="24"/>
     </row>
     <row r="113" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A113" s="76"/>
+      <c r="A113" s="75"/>
       <c r="B113" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C113" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D113" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D113" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E113" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F113" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="24"/>
-      <c r="H113" s="76"/>
+      <c r="H113" s="75"/>
       <c r="I113" s="42" t="s">
         <v>57</v>
       </c>
@@ -6810,35 +6818,35 @@
         <v>0.83</v>
       </c>
       <c r="O113" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P113" s="24"/>
       <c r="Q113" s="24"/>
     </row>
     <row r="114" spans="1:17" s="16" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="76"/>
+      <c r="A114" s="75"/>
       <c r="B114" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C114" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D114" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D114" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E114" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F114" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="24"/>
-      <c r="H114" s="76"/>
+      <c r="H114" s="75"/>
       <c r="I114" s="42" t="s">
         <v>58</v>
       </c>
@@ -6858,35 +6866,35 @@
         <v>0.83</v>
       </c>
       <c r="O114" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P114" s="24"/>
       <c r="Q114" s="24"/>
     </row>
     <row r="115" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="76"/>
+      <c r="A115" s="75"/>
       <c r="B115" s="42" t="s">
         <v>59</v>
       </c>
       <c r="C115" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D115" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D115" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E115" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F115" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="24"/>
-      <c r="H115" s="76"/>
+      <c r="H115" s="75"/>
       <c r="I115" s="42" t="s">
         <v>59</v>
       </c>
@@ -6906,35 +6914,35 @@
         <v>0.83</v>
       </c>
       <c r="O115" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P115" s="24"/>
       <c r="Q115" s="24"/>
     </row>
     <row r="116" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="77"/>
+      <c r="A116" s="76"/>
       <c r="B116" s="42" t="s">
         <v>60</v>
       </c>
       <c r="C116" s="27">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D116" s="27">
         <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="D116" s="27">
-        <f t="shared" si="14"/>
         <v>0.24213075060532688</v>
       </c>
       <c r="E116" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="F116" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="16"/>
-      <c r="H116" s="77"/>
+      <c r="H116" s="76"/>
       <c r="I116" s="42" t="s">
         <v>60</v>
       </c>
@@ -6954,7 +6962,7 @@
         <v>0.83</v>
       </c>
       <c r="O116" s="31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.9599999999999991</v>
       </c>
       <c r="P116" s="24"/>
@@ -7090,11 +7098,11 @@
         <v>3</v>
       </c>
       <c r="B124" s="3">
-        <f t="shared" ref="B124:B138" si="17">-LN(0.94)</f>
+        <f t="shared" ref="B124:B138" si="18">-LN(0.94)</f>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C124" s="3">
-        <f t="shared" ref="C124:C138" si="18">-LN(0.94)</f>
+        <f t="shared" ref="C124:C138" si="19">-LN(0.94)</f>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D124" s="3">
@@ -7119,11 +7127,11 @@
         <v>4</v>
       </c>
       <c r="B125" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C125" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D125" s="3">
@@ -7148,11 +7156,11 @@
         <v>5</v>
       </c>
       <c r="B126" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C126" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D126" s="3">
@@ -7177,11 +7185,11 @@
         <v>6</v>
       </c>
       <c r="B127" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C127" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D127" s="3">
@@ -7206,11 +7214,11 @@
         <v>7</v>
       </c>
       <c r="B128" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C128" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D128" s="3">
@@ -7235,11 +7243,11 @@
         <v>13</v>
       </c>
       <c r="B129" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C129" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D129" s="3">
@@ -7264,11 +7272,11 @@
         <v>8</v>
       </c>
       <c r="B130" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C130" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D130" s="3">
@@ -7293,11 +7301,11 @@
         <v>9</v>
       </c>
       <c r="B131" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C131" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D131" s="3">
@@ -7322,11 +7330,11 @@
         <v>10</v>
       </c>
       <c r="B132" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C132" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D132" s="3">
@@ -7351,11 +7359,11 @@
         <v>11</v>
       </c>
       <c r="B133" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C133" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D133" s="3">
@@ -7380,11 +7388,11 @@
         <v>12</v>
       </c>
       <c r="B134" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C134" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D134" s="3">
@@ -7409,11 +7417,11 @@
         <v>57</v>
       </c>
       <c r="B135" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C135" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D135" s="3">
@@ -7438,11 +7446,11 @@
         <v>58</v>
       </c>
       <c r="B136" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C136" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D136" s="3">
@@ -7467,11 +7475,11 @@
         <v>59</v>
       </c>
       <c r="B137" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C137" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D137" s="3">
@@ -7496,11 +7504,11 @@
         <v>60</v>
       </c>
       <c r="B138" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="C138" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6.1875403718087529E-2</v>
       </c>
       <c r="D138" s="3">
@@ -7658,10 +7666,10 @@
       <c r="Q145" s="24"/>
     </row>
     <row r="146" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="71" t="s">
+      <c r="A146" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="B146" s="70"/>
+      <c r="B146" s="69"/>
       <c r="C146" s="24"/>
       <c r="D146" s="24"/>
       <c r="E146" s="24"/>
@@ -7767,10 +7775,10 @@
       <c r="Q150" s="24"/>
     </row>
     <row r="151" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="73" t="s">
+      <c r="A151" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="B151" s="73"/>
+      <c r="B151" s="72"/>
       <c r="C151" s="24"/>
       <c r="D151" s="24"/>
       <c r="E151" s="24"/>
@@ -8075,27 +8083,27 @@
         <v>40</v>
       </c>
       <c r="K164" s="22">
-        <f t="shared" ref="K164:P164" si="19">$B$164*B167</f>
+        <f t="shared" ref="K164:P164" si="20">$B$164*B167</f>
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="L164" s="22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="M164" s="22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3.4799999999999996E-3</v>
       </c>
       <c r="N164" s="22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4.1399999999999996E-3</v>
       </c>
       <c r="O164" s="22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.1399999999999996E-3</v>
       </c>
       <c r="P164" s="22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.3999999999999997E-5</v>
       </c>
       <c r="Q164" s="24"/>
@@ -8114,27 +8122,27 @@
         <v>31</v>
       </c>
       <c r="K165" s="31">
-        <f t="shared" ref="K165:P165" si="20">$C$164*B167</f>
+        <f t="shared" ref="K165:P165" si="21">$C$164*B167</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L165" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.01</v>
       </c>
       <c r="M165" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5.7999999999999996E-2</v>
       </c>
       <c r="N165" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="O165" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.11900000000000001</v>
       </c>
       <c r="P165" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="Q165" s="24"/>
@@ -8167,27 +8175,27 @@
         <v>32</v>
       </c>
       <c r="K166" s="31">
-        <f t="shared" ref="K166:P166" si="21">MIN($D$164*B167,1)</f>
+        <f t="shared" ref="K166:P166" si="22">MIN($D$164*B167,1)</f>
         <v>0.98000000000000009</v>
       </c>
       <c r="L166" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M166" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.81200000000000006</v>
       </c>
       <c r="N166" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.96600000000000019</v>
       </c>
       <c r="O166" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="P166" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.6000000000000008E-3</v>
       </c>
       <c r="Q166" s="24"/>

</xml_diff>

<commit_message>
Change value in HIV-associated mortality matrix from 0.01 to 0.02.
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -637,6 +637,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -647,6 +661,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,23 +679,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2382,7 +2382,7 @@
   <dimension ref="A1:AX187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="23">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D30" s="13">
         <f t="shared" si="1"/>
@@ -3571,10 +3571,10 @@
     </row>
     <row r="42" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="21"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="20"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
@@ -3588,22 +3588,22 @@
     <row r="43" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="27"/>
       <c r="B43" s="55"/>
-      <c r="C43" s="62" t="s">
+      <c r="C43" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="61"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="67"/>
       <c r="G43" s="52"/>
       <c r="H43" s="27"/>
       <c r="I43" s="58"/>
-      <c r="J43" s="60" t="s">
+      <c r="J43" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="K43" s="60"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="60"/>
-      <c r="N43" s="61"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="67"/>
       <c r="O43" s="27"/>
     </row>
     <row r="44" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
@@ -3653,7 +3653,7 @@
       <c r="AX44" s="17"/>
     </row>
     <row r="45" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="64" t="s">
+      <c r="A45" s="71" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3676,7 +3676,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G45" s="21"/>
-      <c r="H45" s="65" t="s">
+      <c r="H45" s="72" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -3704,7 +3704,7 @@
       <c r="AX45" s="16"/>
     </row>
     <row r="46" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="64"/>
+      <c r="A46" s="71"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="21"/>
-      <c r="H46" s="66"/>
+      <c r="H46" s="73"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="AX46" s="10"/>
     </row>
     <row r="47" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="64"/>
+      <c r="A47" s="71"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="21"/>
-      <c r="H47" s="66"/>
+      <c r="H47" s="73"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3798,7 +3798,7 @@
       <c r="AX47" s="10"/>
     </row>
     <row r="48" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="64"/>
+      <c r="A48" s="71"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="21"/>
-      <c r="H48" s="66"/>
+      <c r="H48" s="73"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3845,7 +3845,7 @@
       <c r="AX48" s="10"/>
     </row>
     <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="64"/>
+      <c r="A49" s="71"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="21"/>
-      <c r="H49" s="66"/>
+      <c r="H49" s="73"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3891,7 +3891,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="64"/>
+      <c r="A50" s="71"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="21"/>
-      <c r="H50" s="66"/>
+      <c r="H50" s="73"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -3937,7 +3937,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="64"/>
+      <c r="A51" s="71"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="21"/>
-      <c r="H51" s="66"/>
+      <c r="H51" s="73"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -3983,7 +3983,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="64"/>
+      <c r="A52" s="71"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="21"/>
-      <c r="H52" s="66"/>
+      <c r="H52" s="73"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4029,7 +4029,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="64"/>
+      <c r="A53" s="71"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="21"/>
-      <c r="H53" s="66"/>
+      <c r="H53" s="73"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4075,7 +4075,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="64"/>
+      <c r="A54" s="71"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="21"/>
-      <c r="H54" s="66"/>
+      <c r="H54" s="73"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4121,7 +4121,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="64"/>
+      <c r="A55" s="71"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="21"/>
-      <c r="H55" s="66"/>
+      <c r="H55" s="73"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4167,7 +4167,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="64"/>
+      <c r="A56" s="71"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="21"/>
-      <c r="H56" s="66"/>
+      <c r="H56" s="73"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4213,7 +4213,7 @@
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="64"/>
+      <c r="A57" s="71"/>
       <c r="B57" s="38" t="s">
         <v>41</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="21"/>
-      <c r="H57" s="66"/>
+      <c r="H57" s="73"/>
       <c r="I57" s="38" t="s">
         <v>41</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="64"/>
+      <c r="A58" s="71"/>
       <c r="B58" s="38" t="s">
         <v>42</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="21"/>
-      <c r="H58" s="66"/>
+      <c r="H58" s="73"/>
       <c r="I58" s="38" t="s">
         <v>42</v>
       </c>
@@ -4305,7 +4305,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="64"/>
+      <c r="A59" s="71"/>
       <c r="B59" s="38" t="s">
         <v>43</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="21"/>
-      <c r="H59" s="66"/>
+      <c r="H59" s="73"/>
       <c r="I59" s="38" t="s">
         <v>43</v>
       </c>
@@ -4351,7 +4351,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="64"/>
+      <c r="A60" s="71"/>
       <c r="B60" s="38" t="s">
         <v>44</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="21"/>
-      <c r="H60" s="67"/>
+      <c r="H60" s="74"/>
       <c r="I60" s="38" t="s">
         <v>44</v>
       </c>
@@ -4414,7 +4414,7 @@
       <c r="O61" s="20"/>
     </row>
     <row r="62" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="72" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -4437,7 +4437,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G62" s="21"/>
-      <c r="H62" s="65" t="s">
+      <c r="H62" s="72" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -4464,7 +4464,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="66"/>
+      <c r="A63" s="73"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="21"/>
-      <c r="H63" s="66"/>
+      <c r="H63" s="73"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4510,7 +4510,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="66"/>
+      <c r="A64" s="73"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="21"/>
-      <c r="H64" s="66"/>
+      <c r="H64" s="73"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4556,7 +4556,7 @@
       </c>
     </row>
     <row r="65" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="66"/>
+      <c r="A65" s="73"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="21"/>
-      <c r="H65" s="66"/>
+      <c r="H65" s="73"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4602,7 +4602,7 @@
       </c>
     </row>
     <row r="66" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="66"/>
+      <c r="A66" s="73"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="21"/>
-      <c r="H66" s="66"/>
+      <c r="H66" s="73"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4648,7 +4648,7 @@
       </c>
     </row>
     <row r="67" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="66"/>
+      <c r="A67" s="73"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="21"/>
-      <c r="H67" s="66"/>
+      <c r="H67" s="73"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4694,7 +4694,7 @@
       </c>
     </row>
     <row r="68" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="66"/>
+      <c r="A68" s="73"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="21"/>
-      <c r="H68" s="66"/>
+      <c r="H68" s="73"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4740,7 +4740,7 @@
       </c>
     </row>
     <row r="69" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="66"/>
+      <c r="A69" s="73"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="21"/>
-      <c r="H69" s="66"/>
+      <c r="H69" s="73"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
     </row>
     <row r="70" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="66"/>
+      <c r="A70" s="73"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="21"/>
-      <c r="H70" s="66"/>
+      <c r="H70" s="73"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4832,7 +4832,7 @@
       </c>
     </row>
     <row r="71" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="66"/>
+      <c r="A71" s="73"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="21"/>
-      <c r="H71" s="66"/>
+      <c r="H71" s="73"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4878,7 +4878,7 @@
       </c>
     </row>
     <row r="72" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="66"/>
+      <c r="A72" s="73"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="21"/>
-      <c r="H72" s="66"/>
+      <c r="H72" s="73"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -4924,7 +4924,7 @@
       </c>
     </row>
     <row r="73" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="66"/>
+      <c r="A73" s="73"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="21"/>
-      <c r="H73" s="66"/>
+      <c r="H73" s="73"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -4970,7 +4970,7 @@
       </c>
     </row>
     <row r="74" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="66"/>
+      <c r="A74" s="73"/>
       <c r="B74" s="38" t="s">
         <v>41</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="21"/>
-      <c r="H74" s="66"/>
+      <c r="H74" s="73"/>
       <c r="I74" s="38" t="s">
         <v>41</v>
       </c>
@@ -5016,7 +5016,7 @@
       </c>
     </row>
     <row r="75" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="66"/>
+      <c r="A75" s="73"/>
       <c r="B75" s="38" t="s">
         <v>42</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="21"/>
-      <c r="H75" s="66"/>
+      <c r="H75" s="73"/>
       <c r="I75" s="38" t="s">
         <v>42</v>
       </c>
@@ -5062,7 +5062,7 @@
       </c>
     </row>
     <row r="76" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="66"/>
+      <c r="A76" s="73"/>
       <c r="B76" s="38" t="s">
         <v>43</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="21"/>
-      <c r="H76" s="66"/>
+      <c r="H76" s="73"/>
       <c r="I76" s="38" t="s">
         <v>43</v>
       </c>
@@ -5108,7 +5108,7 @@
       </c>
     </row>
     <row r="77" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="67"/>
+      <c r="A77" s="74"/>
       <c r="B77" s="38" t="s">
         <v>44</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="21"/>
-      <c r="H77" s="67"/>
+      <c r="H77" s="74"/>
       <c r="I77" s="38" t="s">
         <v>44</v>
       </c>
@@ -5216,10 +5216,10 @@
     </row>
     <row r="81" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="20"/>
-      <c r="B81" s="63"/>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
+      <c r="B81" s="69"/>
+      <c r="C81" s="69"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="69"/>
       <c r="F81" s="20"/>
       <c r="G81" s="50"/>
       <c r="H81" s="50"/>
@@ -5237,22 +5237,22 @@
     <row r="82" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
+      <c r="D82" s="75"/>
+      <c r="E82" s="75"/>
+      <c r="F82" s="75"/>
       <c r="G82" s="21"/>
       <c r="H82" s="27"/>
       <c r="I82" s="58"/>
-      <c r="J82" s="60" t="s">
+      <c r="J82" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="K82" s="60"/>
-      <c r="L82" s="60"/>
-      <c r="M82" s="60"/>
-      <c r="N82" s="61"/>
+      <c r="K82" s="66"/>
+      <c r="L82" s="66"/>
+      <c r="M82" s="66"/>
+      <c r="N82" s="67"/>
       <c r="O82" s="27"/>
       <c r="P82" s="20"/>
       <c r="Q82" s="20"/>
@@ -5307,7 +5307,7 @@
       <c r="AB83" s="15"/>
     </row>
     <row r="84" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="64" t="s">
+      <c r="A84" s="71" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5330,7 +5330,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="50"/>
-      <c r="H84" s="65" t="s">
+      <c r="H84" s="72" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5359,7 +5359,7 @@
       <c r="AB84" s="15"/>
     </row>
     <row r="85" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="64"/>
+      <c r="A85" s="71"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="50"/>
-      <c r="H85" s="66"/>
+      <c r="H85" s="73"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5407,7 +5407,7 @@
       <c r="AB85" s="15"/>
     </row>
     <row r="86" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="64"/>
+      <c r="A86" s="71"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="50"/>
-      <c r="H86" s="66"/>
+      <c r="H86" s="73"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5455,7 +5455,7 @@
       <c r="AB86" s="15"/>
     </row>
     <row r="87" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="64"/>
+      <c r="A87" s="71"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="21"/>
-      <c r="H87" s="66"/>
+      <c r="H87" s="73"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5503,7 +5503,7 @@
       <c r="AB87" s="15"/>
     </row>
     <row r="88" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="64"/>
+      <c r="A88" s="71"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="50"/>
-      <c r="H88" s="66"/>
+      <c r="H88" s="73"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5551,7 +5551,7 @@
       <c r="AB88" s="15"/>
     </row>
     <row r="89" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A89" s="64"/>
+      <c r="A89" s="71"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="21"/>
-      <c r="H89" s="66"/>
+      <c r="H89" s="73"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5600,7 +5600,7 @@
       <c r="AB89" s="15"/>
     </row>
     <row r="90" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="64"/>
+      <c r="A90" s="71"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="50"/>
-      <c r="H90" s="66"/>
+      <c r="H90" s="73"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5647,7 +5647,7 @@
       <c r="AB90" s="15"/>
     </row>
     <row r="91" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A91" s="64"/>
+      <c r="A91" s="71"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="50"/>
-      <c r="H91" s="66"/>
+      <c r="H91" s="73"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="AB91" s="15"/>
     </row>
     <row r="92" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="64"/>
+      <c r="A92" s="71"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="50"/>
-      <c r="H92" s="66"/>
+      <c r="H92" s="73"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5741,7 +5741,7 @@
       <c r="AB92" s="15"/>
     </row>
     <row r="93" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="64"/>
+      <c r="A93" s="71"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="50"/>
-      <c r="H93" s="66"/>
+      <c r="H93" s="73"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5788,7 +5788,7 @@
       <c r="AB93" s="15"/>
     </row>
     <row r="94" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A94" s="64"/>
+      <c r="A94" s="71"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="21"/>
-      <c r="H94" s="66"/>
+      <c r="H94" s="73"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5835,7 +5835,7 @@
       <c r="AB94" s="15"/>
     </row>
     <row r="95" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="64"/>
+      <c r="A95" s="71"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="21"/>
-      <c r="H95" s="66"/>
+      <c r="H95" s="73"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="AB95" s="15"/>
     </row>
     <row r="96" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="64"/>
+      <c r="A96" s="71"/>
       <c r="B96" s="38" t="s">
         <v>41</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="21"/>
-      <c r="H96" s="66"/>
+      <c r="H96" s="73"/>
       <c r="I96" s="38" t="s">
         <v>41</v>
       </c>
@@ -5933,7 +5933,7 @@
       <c r="AB96" s="15"/>
     </row>
     <row r="97" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="64"/>
+      <c r="A97" s="71"/>
       <c r="B97" s="38" t="s">
         <v>42</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="20"/>
-      <c r="H97" s="66"/>
+      <c r="H97" s="73"/>
       <c r="I97" s="38" t="s">
         <v>42</v>
       </c>
@@ -5982,7 +5982,7 @@
       <c r="AB97" s="15"/>
     </row>
     <row r="98" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A98" s="64"/>
+      <c r="A98" s="71"/>
       <c r="B98" s="38" t="s">
         <v>43</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="20"/>
-      <c r="H98" s="66"/>
+      <c r="H98" s="73"/>
       <c r="I98" s="38" t="s">
         <v>43</v>
       </c>
@@ -6030,7 +6030,7 @@
       <c r="Q98" s="20"/>
     </row>
     <row r="99" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A99" s="64"/>
+      <c r="A99" s="71"/>
       <c r="B99" s="38" t="s">
         <v>44</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="20"/>
-      <c r="H99" s="67"/>
+      <c r="H99" s="74"/>
       <c r="I99" s="38" t="s">
         <v>44</v>
       </c>
@@ -6097,7 +6097,7 @@
       <c r="Q100" s="20"/>
     </row>
     <row r="101" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="65" t="s">
+      <c r="A101" s="72" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6120,7 +6120,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="20"/>
-      <c r="H101" s="65" t="s">
+      <c r="H101" s="72" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6149,7 +6149,7 @@
       <c r="Q101" s="20"/>
     </row>
     <row r="102" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="66"/>
+      <c r="A102" s="73"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="20"/>
-      <c r="H102" s="66"/>
+      <c r="H102" s="73"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6197,7 +6197,7 @@
       <c r="Q102" s="20"/>
     </row>
     <row r="103" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="66"/>
+      <c r="A103" s="73"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="20"/>
-      <c r="H103" s="66"/>
+      <c r="H103" s="73"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6245,7 +6245,7 @@
       <c r="Q103" s="20"/>
     </row>
     <row r="104" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="66"/>
+      <c r="A104" s="73"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="20"/>
-      <c r="H104" s="66"/>
+      <c r="H104" s="73"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6293,7 +6293,7 @@
       <c r="Q104" s="20"/>
     </row>
     <row r="105" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="66"/>
+      <c r="A105" s="73"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="20"/>
-      <c r="H105" s="66"/>
+      <c r="H105" s="73"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6341,7 +6341,7 @@
       <c r="Q105" s="20"/>
     </row>
     <row r="106" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="66"/>
+      <c r="A106" s="73"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="20"/>
-      <c r="H106" s="66"/>
+      <c r="H106" s="73"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="Q106" s="20"/>
     </row>
     <row r="107" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="66"/>
+      <c r="A107" s="73"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="20"/>
-      <c r="H107" s="66"/>
+      <c r="H107" s="73"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6437,7 +6437,7 @@
       <c r="Q107" s="20"/>
     </row>
     <row r="108" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="66"/>
+      <c r="A108" s="73"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="20"/>
-      <c r="H108" s="66"/>
+      <c r="H108" s="73"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6485,7 +6485,7 @@
       <c r="Q108" s="20"/>
     </row>
     <row r="109" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A109" s="66"/>
+      <c r="A109" s="73"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="20"/>
-      <c r="H109" s="66"/>
+      <c r="H109" s="73"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6533,7 +6533,7 @@
       <c r="Q109" s="20"/>
     </row>
     <row r="110" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="66"/>
+      <c r="A110" s="73"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="20"/>
-      <c r="H110" s="66"/>
+      <c r="H110" s="73"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6581,7 +6581,7 @@
       <c r="Q110" s="20"/>
     </row>
     <row r="111" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="66"/>
+      <c r="A111" s="73"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="20"/>
-      <c r="H111" s="66"/>
+      <c r="H111" s="73"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6629,7 +6629,7 @@
       <c r="Q111" s="20"/>
     </row>
     <row r="112" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="66"/>
+      <c r="A112" s="73"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="20"/>
-      <c r="H112" s="66"/>
+      <c r="H112" s="73"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6677,7 +6677,7 @@
       <c r="Q112" s="20"/>
     </row>
     <row r="113" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A113" s="66"/>
+      <c r="A113" s="73"/>
       <c r="B113" s="38" t="s">
         <v>41</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="20"/>
-      <c r="H113" s="66"/>
+      <c r="H113" s="73"/>
       <c r="I113" s="38" t="s">
         <v>41</v>
       </c>
@@ -6725,7 +6725,7 @@
       <c r="Q113" s="20"/>
     </row>
     <row r="114" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="66"/>
+      <c r="A114" s="73"/>
       <c r="B114" s="38" t="s">
         <v>42</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="20"/>
-      <c r="H114" s="66"/>
+      <c r="H114" s="73"/>
       <c r="I114" s="38" t="s">
         <v>42</v>
       </c>
@@ -6773,7 +6773,7 @@
       <c r="Q114" s="20"/>
     </row>
     <row r="115" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="66"/>
+      <c r="A115" s="73"/>
       <c r="B115" s="38" t="s">
         <v>43</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="20"/>
-      <c r="H115" s="66"/>
+      <c r="H115" s="73"/>
       <c r="I115" s="38" t="s">
         <v>43</v>
       </c>
@@ -6821,7 +6821,7 @@
       <c r="Q115" s="20"/>
     </row>
     <row r="116" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="67"/>
+      <c r="A116" s="74"/>
       <c r="B116" s="38" t="s">
         <v>44</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="15"/>
-      <c r="H116" s="67"/>
+      <c r="H116" s="74"/>
       <c r="I116" s="38" t="s">
         <v>44</v>
       </c>
@@ -6888,8 +6888,8 @@
       <c r="E118" s="10"/>
       <c r="F118" s="10"/>
       <c r="G118" s="10"/>
-      <c r="H118" s="73"/>
-      <c r="I118" s="74"/>
+      <c r="H118" s="64"/>
+      <c r="I118" s="65"/>
       <c r="J118" s="28"/>
       <c r="K118" s="28"/>
       <c r="L118" s="28"/>
@@ -6913,8 +6913,8 @@
       <c r="E119" s="10"/>
       <c r="F119" s="10"/>
       <c r="G119" s="10"/>
-      <c r="H119" s="73"/>
-      <c r="I119" s="74"/>
+      <c r="H119" s="64"/>
+      <c r="I119" s="65"/>
       <c r="J119" s="28"/>
       <c r="K119" s="28"/>
       <c r="L119" s="28"/>
@@ -6938,8 +6938,8 @@
       <c r="E120" s="10"/>
       <c r="F120" s="10"/>
       <c r="G120" s="10"/>
-      <c r="H120" s="73"/>
-      <c r="I120" s="74"/>
+      <c r="H120" s="64"/>
+      <c r="I120" s="65"/>
       <c r="J120" s="28"/>
       <c r="K120" s="28"/>
       <c r="L120" s="28"/>
@@ -6956,7 +6956,7 @@
       <c r="W120" s="10"/>
     </row>
     <row r="121" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A121" s="71"/>
+      <c r="A121" s="62"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="1"/>
@@ -6982,8 +6982,8 @@
     </row>
     <row r="122" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A122" s="16"/>
-      <c r="B122" s="71"/>
-      <c r="C122" s="71"/>
+      <c r="B122" s="62"/>
+      <c r="C122" s="62"/>
       <c r="D122" s="16"/>
       <c r="E122" s="28"/>
       <c r="F122" s="28"/>
@@ -7306,7 +7306,7 @@
       <c r="W134" s="10"/>
     </row>
     <row r="135" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A135" s="74"/>
+      <c r="A135" s="65"/>
       <c r="B135" s="53"/>
       <c r="C135" s="53"/>
       <c r="D135" s="53"/>
@@ -7331,7 +7331,7 @@
       <c r="W135" s="10"/>
     </row>
     <row r="136" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A136" s="74"/>
+      <c r="A136" s="65"/>
       <c r="B136" s="53"/>
       <c r="C136" s="53"/>
       <c r="D136" s="53"/>
@@ -7356,7 +7356,7 @@
       <c r="W136" s="10"/>
     </row>
     <row r="137" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="74"/>
+      <c r="A137" s="65"/>
       <c r="B137" s="53"/>
       <c r="C137" s="53"/>
       <c r="D137" s="53"/>
@@ -7381,7 +7381,7 @@
       <c r="W137" s="10"/>
     </row>
     <row r="138" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="74"/>
+      <c r="A138" s="65"/>
       <c r="B138" s="53"/>
       <c r="C138" s="53"/>
       <c r="D138" s="53"/>
@@ -7531,7 +7531,7 @@
       <c r="W143" s="10"/>
     </row>
     <row r="144" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="69"/>
+      <c r="A144" s="60"/>
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -7556,7 +7556,7 @@
       <c r="W144" s="10"/>
     </row>
     <row r="145" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A145" s="70"/>
+      <c r="A145" s="61"/>
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -7581,8 +7581,8 @@
       <c r="W145" s="10"/>
     </row>
     <row r="146" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="75"/>
-      <c r="B146" s="75"/>
+      <c r="A146" s="70"/>
+      <c r="B146" s="70"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
       <c r="E146" s="28"/>
@@ -7706,8 +7706,8 @@
       <c r="W150" s="10"/>
     </row>
     <row r="151" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A151" s="75"/>
-      <c r="B151" s="75"/>
+      <c r="A151" s="70"/>
+      <c r="B151" s="70"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
       <c r="E151" s="28"/>
@@ -7949,7 +7949,7 @@
       <c r="AI159" s="10"/>
     </row>
     <row r="160" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A160" s="69"/>
+      <c r="A160" s="60"/>
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -7986,7 +7986,7 @@
       <c r="AI160" s="10"/>
     </row>
     <row r="161" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A161" s="70"/>
+      <c r="A161" s="61"/>
       <c r="B161" s="28"/>
       <c r="C161" s="28"/>
       <c r="D161" s="28"/>
@@ -8023,7 +8023,7 @@
       <c r="AI161" s="10"/>
     </row>
     <row r="162" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A162" s="70"/>
+      <c r="A162" s="61"/>
       <c r="B162" s="28"/>
       <c r="C162" s="28"/>
       <c r="D162" s="28"/>
@@ -8061,21 +8061,21 @@
     </row>
     <row r="163" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A163" s="28"/>
-      <c r="B163" s="69"/>
-      <c r="C163" s="69"/>
-      <c r="D163" s="69"/>
+      <c r="B163" s="60"/>
+      <c r="C163" s="60"/>
+      <c r="D163" s="60"/>
       <c r="E163" s="28"/>
       <c r="F163" s="28"/>
       <c r="G163" s="28"/>
       <c r="H163" s="28"/>
       <c r="I163" s="28"/>
-      <c r="J163" s="71"/>
-      <c r="K163" s="71"/>
-      <c r="L163" s="71"/>
-      <c r="M163" s="71"/>
-      <c r="N163" s="71"/>
-      <c r="O163" s="71"/>
-      <c r="P163" s="71"/>
+      <c r="J163" s="62"/>
+      <c r="K163" s="62"/>
+      <c r="L163" s="62"/>
+      <c r="M163" s="62"/>
+      <c r="N163" s="62"/>
+      <c r="O163" s="62"/>
+      <c r="P163" s="62"/>
       <c r="Q163" s="28"/>
       <c r="R163" s="10"/>
       <c r="S163" s="10"/>
@@ -8097,7 +8097,7 @@
       <c r="AI163" s="10"/>
     </row>
     <row r="164" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A164" s="72"/>
+      <c r="A164" s="63"/>
       <c r="B164" s="28"/>
       <c r="C164" s="28"/>
       <c r="D164" s="28"/>
@@ -8106,7 +8106,7 @@
       <c r="G164" s="28"/>
       <c r="H164" s="28"/>
       <c r="I164" s="28"/>
-      <c r="J164" s="71"/>
+      <c r="J164" s="62"/>
       <c r="K164" s="1"/>
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
@@ -8143,7 +8143,7 @@
       <c r="G165" s="28"/>
       <c r="H165" s="28"/>
       <c r="I165" s="28"/>
-      <c r="J165" s="69"/>
+      <c r="J165" s="60"/>
       <c r="K165" s="28"/>
       <c r="L165" s="28"/>
       <c r="M165" s="28"/>
@@ -8171,16 +8171,16 @@
       <c r="AI165" s="10"/>
     </row>
     <row r="166" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A166" s="71"/>
-      <c r="B166" s="71"/>
-      <c r="C166" s="71"/>
-      <c r="D166" s="71"/>
-      <c r="E166" s="71"/>
-      <c r="F166" s="71"/>
-      <c r="G166" s="71"/>
-      <c r="H166" s="71"/>
+      <c r="A166" s="62"/>
+      <c r="B166" s="62"/>
+      <c r="C166" s="62"/>
+      <c r="D166" s="62"/>
+      <c r="E166" s="62"/>
+      <c r="F166" s="62"/>
+      <c r="G166" s="62"/>
+      <c r="H166" s="62"/>
       <c r="I166" s="28"/>
-      <c r="J166" s="69"/>
+      <c r="J166" s="60"/>
       <c r="K166" s="28"/>
       <c r="L166" s="28"/>
       <c r="M166" s="28"/>
@@ -8208,7 +8208,7 @@
       <c r="AI166" s="10"/>
     </row>
     <row r="167" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A167" s="71"/>
+      <c r="A167" s="62"/>
       <c r="B167" s="1"/>
       <c r="C167" s="53"/>
       <c r="D167" s="53"/>

</xml_diff>

<commit_message>
Load data on all PLWHIV on ART and virally suppressed
ART coverage values we were using before 2017 did not take into account
viral suppression, and the 2017 value we were using was actually just
proportion virally suppressed, not those on ART and virally suppressed.

Related to #67
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="84">
   <si>
     <t>Male</t>
   </si>
@@ -305,6 +305,18 @@
   <si>
     <t>Transition rate forVL progression (years^-1)</t>
   </si>
+  <si>
+    <t>See "Plots and estimates" tab on ART_Coverage_data.xlsx spreadsheet for calculations, references, and other details</t>
+  </si>
+  <si>
+    <t>Females</t>
+  </si>
+  <si>
+    <t>Males</t>
+  </si>
+  <si>
+    <t>Viral suppression among all PLWHIV on ART in KZN</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +397,19 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -526,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -681,6 +706,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,23 +1003,23 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>46</v>
       </c>
@@ -1023,7 +1057,7 @@
       <c r="AH1" s="4"/>
       <c r="AI1" s="4"/>
     </row>
-    <row r="2" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>45</v>
       </c>
@@ -1061,7 +1095,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>15</v>
       </c>
@@ -1091,7 +1125,7 @@
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
     </row>
-    <row r="4" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1155,7 @@
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
     </row>
-    <row r="5" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -1145,7 +1179,7 @@
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
     </row>
-    <row r="6" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1172,7 +1206,7 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
     </row>
-    <row r="7" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1199,7 +1233,7 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
     </row>
-    <row r="8" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -1226,7 +1260,7 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
     </row>
-    <row r="9" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -1253,7 +1287,7 @@
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
     </row>
-    <row r="10" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>47</v>
       </c>
@@ -1291,7 +1325,7 @@
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
     </row>
-    <row r="11" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>51</v>
       </c>
@@ -1329,7 +1363,7 @@
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
     </row>
-    <row r="12" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>48</v>
       </c>
@@ -1367,7 +1401,7 @@
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
     </row>
-    <row r="13" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>49</v>
       </c>
@@ -1405,7 +1439,7 @@
       <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
     </row>
-    <row r="14" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>50</v>
       </c>
@@ -1443,7 +1477,7 @@
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
     </row>
-    <row r="15" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>52</v>
       </c>
@@ -1481,7 +1515,7 @@
       <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
     </row>
-    <row r="16" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>53</v>
       </c>
@@ -1519,7 +1553,7 @@
       <c r="AH16" s="4"/>
       <c r="AI16" s="4"/>
     </row>
-    <row r="17" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="27" t="s">
         <v>26</v>
@@ -1550,7 +1584,7 @@
       <c r="AH17" s="4"/>
       <c r="AI17" s="4"/>
     </row>
-    <row r="18" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>27</v>
       </c>
@@ -1579,7 +1613,7 @@
       <c r="AH18" s="4"/>
       <c r="AI18" s="4"/>
     </row>
-    <row r="19" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>30</v>
       </c>
@@ -1612,7 +1646,7 @@
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
     </row>
-    <row r="20" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -1636,7 +1670,7 @@
       <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
     </row>
-    <row r="21" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>54</v>
       </c>
@@ -1661,8 +1695,8 @@
       <c r="AH21" s="4"/>
       <c r="AI21" s="4"/>
     </row>
-    <row r="22" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="9"/>
@@ -1687,7 +1721,7 @@
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
     </row>
-    <row r="23" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
@@ -1715,7 +1749,7 @@
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
     </row>
-    <row r="24" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -1743,7 +1777,7 @@
       <c r="AH24" s="4"/>
       <c r="AI24" s="4"/>
     </row>
-    <row r="25" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -1772,7 +1806,7 @@
       <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
     </row>
-    <row r="26" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -1796,7 +1830,7 @@
       <c r="AH26" s="4"/>
       <c r="AI26" s="4"/>
     </row>
-    <row r="27" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -1820,7 +1854,7 @@
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
     </row>
-    <row r="28" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -1844,7 +1878,7 @@
       <c r="AH28" s="4"/>
       <c r="AI28" s="4"/>
     </row>
-    <row r="29" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -1868,10 +1902,24 @@
       <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
     </row>
-    <row r="30" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+    <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="76"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -1892,10 +1940,24 @@
       <c r="AH30" s="4"/>
       <c r="AI30" s="4"/>
     </row>
-    <row r="31" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
+    <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
+      <c r="O31" s="77"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -1916,10 +1978,16 @@
       <c r="AH31" s="4"/>
       <c r="AI31" s="4"/>
     </row>
-    <row r="32" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
+    <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
@@ -1940,10 +2008,16 @@
       <c r="AH32" s="4"/>
       <c r="AI32" s="4"/>
     </row>
-    <row r="33" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
+    <row r="33" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="80">
+        <v>2004</v>
+      </c>
+      <c r="B33" s="80">
+        <v>0</v>
+      </c>
+      <c r="C33" s="80">
+        <v>0</v>
+      </c>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
@@ -1964,10 +2038,17 @@
       <c r="AH33" s="4"/>
       <c r="AI33" s="4"/>
     </row>
-    <row r="34" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+    <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="80">
+        <v>2005</v>
+      </c>
+      <c r="B34" s="80">
+        <v>7.7450763443239652E-3</v>
+      </c>
+      <c r="C34" s="80">
+        <f>0.74*B34</f>
+        <v>5.7313564947997341E-3</v>
+      </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
@@ -1988,10 +2069,17 @@
       <c r="AH34" s="4"/>
       <c r="AI34" s="4"/>
     </row>
-    <row r="35" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
+    <row r="35" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="80">
+        <v>2006</v>
+      </c>
+      <c r="B35" s="80">
+        <v>2.9431290108431069E-2</v>
+      </c>
+      <c r="C35" s="80">
+        <f>0.74*B35</f>
+        <v>2.1779154680238992E-2</v>
+      </c>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
@@ -2012,10 +2100,17 @@
       <c r="AH35" s="4"/>
       <c r="AI35" s="4"/>
     </row>
-    <row r="36" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
+    <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="80">
+        <v>2007</v>
+      </c>
+      <c r="B36" s="80">
+        <v>6.4284133657888917E-2</v>
+      </c>
+      <c r="C36" s="80">
+        <f>0.74*B36</f>
+        <v>4.7570258906837797E-2</v>
+      </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
@@ -2036,10 +2131,17 @@
       <c r="AH36" s="4"/>
       <c r="AI36" s="4"/>
     </row>
-    <row r="37" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
+    <row r="37" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="80">
+        <v>2008</v>
+      </c>
+      <c r="B37" s="80">
+        <v>0.11075459172383269</v>
+      </c>
+      <c r="C37" s="80">
+        <f>0.74*B37</f>
+        <v>8.1958397875636191E-2</v>
+      </c>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
@@ -2060,10 +2162,17 @@
       <c r="AH37" s="4"/>
       <c r="AI37" s="4"/>
     </row>
-    <row r="38" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
+    <row r="38" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="80">
+        <v>2009</v>
+      </c>
+      <c r="B38" s="80">
+        <v>0.15567603452091172</v>
+      </c>
+      <c r="C38" s="80">
+        <f>0.74*B38</f>
+        <v>0.11520026554547468</v>
+      </c>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
@@ -2084,10 +2193,17 @@
       <c r="AH38" s="4"/>
       <c r="AI38" s="4"/>
     </row>
-    <row r="39" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
+    <row r="39" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="80">
+        <v>2010</v>
+      </c>
+      <c r="B39" s="80">
+        <v>0.19130338570480196</v>
+      </c>
+      <c r="C39" s="80">
+        <f>0.74*B39</f>
+        <v>0.14156450542155344</v>
+      </c>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
@@ -2108,10 +2224,17 @@
       <c r="AH39" s="4"/>
       <c r="AI39" s="4"/>
     </row>
-    <row r="40" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
+    <row r="40" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="80">
+        <v>2011</v>
+      </c>
+      <c r="B40" s="80">
+        <v>0.23777384377074573</v>
+      </c>
+      <c r="C40" s="80">
+        <f>0.74*B40</f>
+        <v>0.17595264439035183</v>
+      </c>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
@@ -2132,10 +2255,17 @@
       <c r="AH40" s="4"/>
       <c r="AI40" s="4"/>
     </row>
-    <row r="41" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
+    <row r="41" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="80">
+        <v>2017</v>
+      </c>
+      <c r="B41" s="80">
+        <v>0.59747731799070602</v>
+      </c>
+      <c r="C41" s="80">
+        <f>0.74*B41</f>
+        <v>0.44213321531312244</v>
+      </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
@@ -2156,10 +2286,10 @@
       <c r="AH41" s="4"/>
       <c r="AI41" s="4"/>
     </row>
-    <row r="42" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+    <row r="42" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="78"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
@@ -2180,7 +2310,10 @@
       <c r="AH42" s="4"/>
       <c r="AI42" s="4"/>
     </row>
-    <row r="43" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="78"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="78"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
@@ -2201,7 +2334,10 @@
       <c r="AH43" s="4"/>
       <c r="AI43" s="4"/>
     </row>
-    <row r="44" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="78"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="78"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
@@ -2222,7 +2358,10 @@
       <c r="AH44" s="4"/>
       <c r="AI44" s="4"/>
     </row>
-    <row r="45" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="78"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
@@ -2243,7 +2382,10 @@
       <c r="AH45" s="4"/>
       <c r="AI45" s="4"/>
     </row>
-    <row r="46" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="78"/>
+      <c r="B46" s="78"/>
+      <c r="C46" s="78"/>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
@@ -2264,7 +2406,7 @@
       <c r="AH46" s="4"/>
       <c r="AI46" s="4"/>
     </row>
-    <row r="47" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
@@ -2285,7 +2427,7 @@
       <c r="AH47" s="4"/>
       <c r="AI47" s="4"/>
     </row>
-    <row r="48" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
@@ -2306,7 +2448,7 @@
       <c r="AH48" s="4"/>
       <c r="AI48" s="4"/>
     </row>
-    <row r="49" spans="17:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="17:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
@@ -2327,7 +2469,7 @@
       <c r="AH49" s="4"/>
       <c r="AI49" s="4"/>
     </row>
-    <row r="50" spans="17:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="17:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
@@ -2348,7 +2490,7 @@
       <c r="AH50" s="4"/>
       <c r="AI50" s="4"/>
     </row>
-    <row r="51" spans="17:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="17:35" x14ac:dyDescent="0.25">
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
@@ -2371,6 +2513,10 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="2">
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A31:O31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2381,55 +2527,54 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AX187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.08984375" customWidth="1"/>
-    <col min="2" max="4" width="29.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="35.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="4" width="29.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
     <col min="14" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7265625" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.08984375" customWidth="1"/>
-    <col min="31" max="31" width="14.90625" customWidth="1"/>
-    <col min="32" max="32" width="12.54296875" customWidth="1"/>
-    <col min="33" max="33" width="12.6328125" customWidth="1"/>
-    <col min="34" max="34" width="13.81640625" customWidth="1"/>
-    <col min="40" max="40" width="14.453125" customWidth="1"/>
-    <col min="41" max="41" width="14.6328125" customWidth="1"/>
-    <col min="42" max="42" width="18.08984375" customWidth="1"/>
-    <col min="44" max="44" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.1796875" customWidth="1"/>
-    <col min="51" max="51" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.08984375" customWidth="1"/>
-    <col min="53" max="53" width="13.1796875" customWidth="1"/>
-    <col min="55" max="55" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" customWidth="1"/>
+    <col min="32" max="33" width="12.5703125" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" customWidth="1"/>
+    <col min="41" max="41" width="14.5703125" customWidth="1"/>
+    <col min="42" max="42" width="18.140625" customWidth="1"/>
+    <col min="44" max="44" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.140625" customWidth="1"/>
+    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.140625" customWidth="1"/>
+    <col min="53" max="53" width="13.140625" customWidth="1"/>
+    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="18" customWidth="1"/>
-    <col min="57" max="57" width="13.36328125" customWidth="1"/>
-    <col min="58" max="58" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.36328125" customWidth="1"/>
-    <col min="60" max="60" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.42578125" customWidth="1"/>
+    <col min="58" max="58" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.42578125" customWidth="1"/>
+    <col min="60" max="60" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="15" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>63</v>
       </c>
@@ -2451,7 +2596,7 @@
       <c r="Q1" s="14"/>
       <c r="R1" s="14"/>
     </row>
-    <row r="2" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>64</v>
       </c>
@@ -2475,7 +2620,7 @@
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="47">
         <v>2005</v>
       </c>
@@ -2499,7 +2644,7 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="1:38" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:38" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>66</v>
       </c>
@@ -2523,7 +2668,7 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>15</v>
       </c>
@@ -2538,7 +2683,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
@@ -2553,7 +2698,7 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2005</v>
       </c>
@@ -2568,7 +2713,7 @@
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>
@@ -2583,7 +2728,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -2594,7 +2739,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -2605,7 +2750,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -2616,7 +2761,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -2627,7 +2772,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -2638,7 +2783,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>61</v>
       </c>
@@ -2670,7 +2815,7 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>55</v>
       </c>
@@ -2704,7 +2849,7 @@
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:38" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:38" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>56</v>
       </c>
@@ -2738,7 +2883,7 @@
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
     </row>
-    <row r="17" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>57</v>
       </c>
@@ -2772,7 +2917,7 @@
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18" spans="1:38" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:38" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>62</v>
       </c>
@@ -2796,7 +2941,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>14</v>
       </c>
@@ -2834,7 +2979,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="1:38" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:38" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2873,7 +3018,7 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
     </row>
-    <row r="21" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -2913,7 +3058,7 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
     </row>
-    <row r="22" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -2953,7 +3098,7 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
     </row>
-    <row r="23" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -2993,7 +3138,7 @@
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
     </row>
-    <row r="24" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -3033,7 +3178,7 @@
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
     </row>
-    <row r="25" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -3073,7 +3218,7 @@
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
     </row>
-    <row r="26" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3113,7 +3258,7 @@
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3153,7 +3298,7 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
     </row>
-    <row r="28" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3193,7 +3338,7 @@
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
     </row>
-    <row r="29" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3233,7 +3378,7 @@
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
     </row>
-    <row r="30" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3273,7 +3418,7 @@
       <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
     </row>
-    <row r="31" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -3313,7 +3458,7 @@
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
     </row>
-    <row r="32" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
         <v>41</v>
       </c>
@@ -3353,7 +3498,7 @@
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="38" t="s">
         <v>42</v>
       </c>
@@ -3393,7 +3538,7 @@
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
     </row>
-    <row r="34" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>43</v>
       </c>
@@ -3433,7 +3578,7 @@
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
     </row>
-    <row r="35" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="38" t="s">
         <v>44</v>
       </c>
@@ -3473,7 +3618,7 @@
       <c r="AK35" s="4"/>
       <c r="AL35" s="4"/>
     </row>
-    <row r="36" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -3485,7 +3630,7 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -3497,7 +3642,7 @@
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -3509,7 +3654,7 @@
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:50" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -3528,7 +3673,7 @@
       <c r="P39" s="20"/>
       <c r="Q39" s="20"/>
     </row>
-    <row r="40" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -3547,7 +3692,7 @@
       <c r="P40" s="20"/>
       <c r="Q40" s="20"/>
     </row>
-    <row r="41" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>70</v>
       </c>
@@ -3569,7 +3714,7 @@
       <c r="Q41" s="25"/>
       <c r="R41" s="14"/>
     </row>
-    <row r="42" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="69"/>
       <c r="C42" s="69"/>
@@ -3585,7 +3730,7 @@
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
     </row>
-    <row r="43" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="27"/>
       <c r="B43" s="55"/>
       <c r="C43" s="68" t="s">
@@ -3606,7 +3751,7 @@
       <c r="N43" s="67"/>
       <c r="O43" s="27"/>
     </row>
-    <row r="44" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
         <v>35</v>
       </c>
@@ -3652,7 +3797,7 @@
       </c>
       <c r="AX44" s="17"/>
     </row>
-    <row r="45" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="71" t="s">
         <v>0</v>
       </c>
@@ -3703,7 +3848,7 @@
       </c>
       <c r="AX45" s="16"/>
     </row>
-    <row r="46" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="71"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
@@ -3750,7 +3895,7 @@
       </c>
       <c r="AX46" s="10"/>
     </row>
-    <row r="47" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="71"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
@@ -3797,7 +3942,7 @@
       </c>
       <c r="AX47" s="10"/>
     </row>
-    <row r="48" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="71"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
@@ -3844,7 +3989,7 @@
       </c>
       <c r="AX48" s="10"/>
     </row>
-    <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="71"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
@@ -3890,7 +4035,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="71"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
@@ -3936,7 +4081,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="71"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
@@ -3982,7 +4127,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="71"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
@@ -4028,7 +4173,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="71"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
@@ -4074,7 +4219,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="71"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
@@ -4120,7 +4265,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="71"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
@@ -4166,7 +4311,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="71"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
@@ -4212,7 +4357,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="71"/>
       <c r="B57" s="38" t="s">
         <v>41</v>
@@ -4258,7 +4403,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="71"/>
       <c r="B58" s="38" t="s">
         <v>42</v>
@@ -4304,7 +4449,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="71"/>
       <c r="B59" s="38" t="s">
         <v>43</v>
@@ -4350,7 +4495,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="71"/>
       <c r="B60" s="38" t="s">
         <v>44</v>
@@ -4396,7 +4541,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
       <c r="B61" s="54"/>
       <c r="C61" s="20"/>
@@ -4413,7 +4558,7 @@
       <c r="N61" s="20"/>
       <c r="O61" s="20"/>
     </row>
-    <row r="62" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="72" t="s">
         <v>1</v>
       </c>
@@ -4463,7 +4608,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="73"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
@@ -4509,7 +4654,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="73"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
@@ -4555,7 +4700,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="73"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
@@ -4601,7 +4746,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="73"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
@@ -4647,7 +4792,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="73"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
@@ -4693,7 +4838,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="73"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
@@ -4739,7 +4884,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="73"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
@@ -4785,7 +4930,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="73"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
@@ -4831,7 +4976,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="73"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
@@ -4877,7 +5022,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="73"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
@@ -4923,7 +5068,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="73"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
@@ -4969,7 +5114,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="73"/>
       <c r="B74" s="38" t="s">
         <v>41</v>
@@ -5015,7 +5160,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="73"/>
       <c r="B75" s="38" t="s">
         <v>42</v>
@@ -5061,7 +5206,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="73"/>
       <c r="B76" s="38" t="s">
         <v>43</v>
@@ -5107,7 +5252,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="74"/>
       <c r="B77" s="38" t="s">
         <v>44</v>
@@ -5153,7 +5298,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
       <c r="C78" s="20"/>
@@ -5172,7 +5317,7 @@
       <c r="P78" s="20"/>
       <c r="Q78" s="20"/>
     </row>
-    <row r="79" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
       <c r="C79" s="20"/>
@@ -5191,7 +5336,7 @@
       <c r="P79" s="20"/>
       <c r="Q79" s="20"/>
     </row>
-    <row r="80" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
         <v>71</v>
       </c>
@@ -5214,7 +5359,7 @@
       <c r="R80" s="14"/>
       <c r="AB80" s="15"/>
     </row>
-    <row r="81" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="B81" s="69"/>
       <c r="C81" s="69"/>
@@ -5234,7 +5379,7 @@
       <c r="Q81" s="20"/>
       <c r="AB81" s="15"/>
     </row>
-    <row r="82" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="75" t="s">
@@ -5258,7 +5403,7 @@
       <c r="Q82" s="20"/>
       <c r="AB82" s="15"/>
     </row>
-    <row r="83" spans="1:28" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="59" t="s">
         <v>35</v>
       </c>
@@ -5306,7 +5451,7 @@
       <c r="Q83" s="20"/>
       <c r="AB83" s="15"/>
     </row>
-    <row r="84" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="71" t="s">
         <v>0</v>
       </c>
@@ -5358,7 +5503,7 @@
       <c r="Q84" s="20"/>
       <c r="AB84" s="15"/>
     </row>
-    <row r="85" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="71"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
@@ -5406,7 +5551,7 @@
       <c r="Q85" s="50"/>
       <c r="AB85" s="15"/>
     </row>
-    <row r="86" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="71"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
@@ -5454,7 +5599,7 @@
       <c r="Q86" s="21"/>
       <c r="AB86" s="15"/>
     </row>
-    <row r="87" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="71"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
@@ -5502,7 +5647,7 @@
       <c r="Q87" s="21"/>
       <c r="AB87" s="15"/>
     </row>
-    <row r="88" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="71"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
@@ -5550,7 +5695,7 @@
       <c r="Q88" s="21"/>
       <c r="AB88" s="15"/>
     </row>
-    <row r="89" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="71"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
@@ -5599,7 +5744,7 @@
       <c r="Q89" s="21"/>
       <c r="AB89" s="15"/>
     </row>
-    <row r="90" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="71"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
@@ -5646,7 +5791,7 @@
       </c>
       <c r="AB90" s="15"/>
     </row>
-    <row r="91" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="71"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
@@ -5693,7 +5838,7 @@
       </c>
       <c r="AB91" s="15"/>
     </row>
-    <row r="92" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="71"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
@@ -5740,7 +5885,7 @@
       </c>
       <c r="AB92" s="15"/>
     </row>
-    <row r="93" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="71"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
@@ -5787,7 +5932,7 @@
       </c>
       <c r="AB93" s="15"/>
     </row>
-    <row r="94" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="71"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
@@ -5834,7 +5979,7 @@
       </c>
       <c r="AB94" s="15"/>
     </row>
-    <row r="95" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="71"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
@@ -5883,7 +6028,7 @@
       <c r="Q95" s="20"/>
       <c r="AB95" s="15"/>
     </row>
-    <row r="96" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="71"/>
       <c r="B96" s="38" t="s">
         <v>41</v>
@@ -5932,7 +6077,7 @@
       <c r="Q96" s="20"/>
       <c r="AB96" s="15"/>
     </row>
-    <row r="97" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="71"/>
       <c r="B97" s="38" t="s">
         <v>42</v>
@@ -5981,7 +6126,7 @@
       <c r="Q97" s="20"/>
       <c r="AB97" s="15"/>
     </row>
-    <row r="98" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="71"/>
       <c r="B98" s="38" t="s">
         <v>43</v>
@@ -6029,7 +6174,7 @@
       <c r="P98" s="20"/>
       <c r="Q98" s="20"/>
     </row>
-    <row r="99" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="71"/>
       <c r="B99" s="38" t="s">
         <v>44</v>
@@ -6077,7 +6222,7 @@
       <c r="P99" s="20"/>
       <c r="Q99" s="20"/>
     </row>
-    <row r="100" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
       <c r="B100" s="54"/>
       <c r="C100" s="20"/>
@@ -6096,7 +6241,7 @@
       <c r="P100" s="20"/>
       <c r="Q100" s="20"/>
     </row>
-    <row r="101" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="72" t="s">
         <v>1</v>
       </c>
@@ -6148,7 +6293,7 @@
       <c r="P101" s="20"/>
       <c r="Q101" s="20"/>
     </row>
-    <row r="102" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="73"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
@@ -6196,7 +6341,7 @@
       <c r="P102" s="20"/>
       <c r="Q102" s="20"/>
     </row>
-    <row r="103" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="73"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
@@ -6244,7 +6389,7 @@
       <c r="P103" s="20"/>
       <c r="Q103" s="20"/>
     </row>
-    <row r="104" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="73"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
@@ -6292,7 +6437,7 @@
       <c r="P104" s="20"/>
       <c r="Q104" s="20"/>
     </row>
-    <row r="105" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="73"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
@@ -6340,7 +6485,7 @@
       <c r="P105" s="20"/>
       <c r="Q105" s="20"/>
     </row>
-    <row r="106" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="73"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
@@ -6388,7 +6533,7 @@
       <c r="P106" s="20"/>
       <c r="Q106" s="20"/>
     </row>
-    <row r="107" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="73"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
@@ -6436,7 +6581,7 @@
       <c r="P107" s="20"/>
       <c r="Q107" s="20"/>
     </row>
-    <row r="108" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="73"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
@@ -6484,7 +6629,7 @@
       <c r="P108" s="20"/>
       <c r="Q108" s="20"/>
     </row>
-    <row r="109" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="73"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
@@ -6532,7 +6677,7 @@
       <c r="P109" s="20"/>
       <c r="Q109" s="20"/>
     </row>
-    <row r="110" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="73"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
@@ -6580,7 +6725,7 @@
       <c r="P110" s="20"/>
       <c r="Q110" s="20"/>
     </row>
-    <row r="111" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="73"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
@@ -6628,7 +6773,7 @@
       <c r="P111" s="20"/>
       <c r="Q111" s="20"/>
     </row>
-    <row r="112" spans="1:28" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="73"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
@@ -6676,7 +6821,7 @@
       <c r="P112" s="20"/>
       <c r="Q112" s="20"/>
     </row>
-    <row r="113" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="73"/>
       <c r="B113" s="38" t="s">
         <v>41</v>
@@ -6724,7 +6869,7 @@
       <c r="P113" s="20"/>
       <c r="Q113" s="20"/>
     </row>
-    <row r="114" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="73"/>
       <c r="B114" s="38" t="s">
         <v>42</v>
@@ -6772,7 +6917,7 @@
       <c r="P114" s="20"/>
       <c r="Q114" s="20"/>
     </row>
-    <row r="115" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="73"/>
       <c r="B115" s="38" t="s">
         <v>43</v>
@@ -6820,7 +6965,7 @@
       <c r="P115" s="20"/>
       <c r="Q115" s="20"/>
     </row>
-    <row r="116" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="74"/>
       <c r="B116" s="38" t="s">
         <v>44</v>
@@ -6868,7 +7013,7 @@
       <c r="P116" s="20"/>
       <c r="Q116" s="20"/>
     </row>
-    <row r="117" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H117" s="57"/>
       <c r="I117" s="54"/>
       <c r="J117" s="21"/>
@@ -6880,7 +7025,7 @@
       <c r="P117" s="20"/>
       <c r="Q117" s="20"/>
     </row>
-    <row r="118" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="10"/>
       <c r="C118" s="10"/>
@@ -6905,7 +7050,7 @@
       <c r="V118" s="10"/>
       <c r="W118" s="10"/>
     </row>
-    <row r="119" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
@@ -6930,7 +7075,7 @@
       <c r="V119" s="10"/>
       <c r="W119" s="10"/>
     </row>
-    <row r="120" spans="1:23" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -6955,7 +7100,7 @@
       <c r="V120" s="10"/>
       <c r="W120" s="10"/>
     </row>
-    <row r="121" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="62"/>
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
@@ -6980,7 +7125,7 @@
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
     </row>
-    <row r="122" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="16"/>
       <c r="B122" s="62"/>
       <c r="C122" s="62"/>
@@ -7005,7 +7150,7 @@
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
     </row>
-    <row r="123" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="53"/>
       <c r="B123" s="53"/>
       <c r="C123" s="53"/>
@@ -7030,7 +7175,7 @@
       <c r="V123" s="10"/>
       <c r="W123" s="10"/>
     </row>
-    <row r="124" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="53"/>
       <c r="B124" s="53"/>
       <c r="C124" s="53"/>
@@ -7055,7 +7200,7 @@
       <c r="V124" s="10"/>
       <c r="W124" s="10"/>
     </row>
-    <row r="125" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="53"/>
       <c r="B125" s="53"/>
       <c r="C125" s="53"/>
@@ -7080,7 +7225,7 @@
       <c r="V125" s="10"/>
       <c r="W125" s="10"/>
     </row>
-    <row r="126" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="53"/>
       <c r="B126" s="53"/>
       <c r="C126" s="53"/>
@@ -7105,7 +7250,7 @@
       <c r="V126" s="10"/>
       <c r="W126" s="10"/>
     </row>
-    <row r="127" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="53"/>
       <c r="B127" s="53"/>
       <c r="C127" s="53"/>
@@ -7130,7 +7275,7 @@
       <c r="V127" s="10"/>
       <c r="W127" s="10"/>
     </row>
-    <row r="128" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="53"/>
       <c r="B128" s="53"/>
       <c r="C128" s="53"/>
@@ -7155,7 +7300,7 @@
       <c r="V128" s="10"/>
       <c r="W128" s="10"/>
     </row>
-    <row r="129" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="53"/>
       <c r="B129" s="53"/>
       <c r="C129" s="53"/>
@@ -7180,7 +7325,7 @@
       <c r="V129" s="10"/>
       <c r="W129" s="10"/>
     </row>
-    <row r="130" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="53"/>
       <c r="B130" s="53"/>
       <c r="C130" s="53"/>
@@ -7205,7 +7350,7 @@
       <c r="V130" s="10"/>
       <c r="W130" s="10"/>
     </row>
-    <row r="131" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="53"/>
       <c r="B131" s="53"/>
       <c r="C131" s="53"/>
@@ -7230,7 +7375,7 @@
       <c r="V131" s="10"/>
       <c r="W131" s="10"/>
     </row>
-    <row r="132" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="53"/>
       <c r="B132" s="53"/>
       <c r="C132" s="53"/>
@@ -7255,7 +7400,7 @@
       <c r="V132" s="10"/>
       <c r="W132" s="10"/>
     </row>
-    <row r="133" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="53"/>
       <c r="B133" s="53"/>
       <c r="C133" s="53"/>
@@ -7280,7 +7425,7 @@
       <c r="V133" s="10"/>
       <c r="W133" s="10"/>
     </row>
-    <row r="134" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="53"/>
       <c r="B134" s="53"/>
       <c r="C134" s="53"/>
@@ -7305,7 +7450,7 @@
       <c r="V134" s="10"/>
       <c r="W134" s="10"/>
     </row>
-    <row r="135" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="65"/>
       <c r="B135" s="53"/>
       <c r="C135" s="53"/>
@@ -7330,7 +7475,7 @@
       <c r="V135" s="10"/>
       <c r="W135" s="10"/>
     </row>
-    <row r="136" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="65"/>
       <c r="B136" s="53"/>
       <c r="C136" s="53"/>
@@ -7355,7 +7500,7 @@
       <c r="V136" s="10"/>
       <c r="W136" s="10"/>
     </row>
-    <row r="137" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="65"/>
       <c r="B137" s="53"/>
       <c r="C137" s="53"/>
@@ -7380,7 +7525,7 @@
       <c r="V137" s="10"/>
       <c r="W137" s="10"/>
     </row>
-    <row r="138" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="65"/>
       <c r="B138" s="53"/>
       <c r="C138" s="53"/>
@@ -7405,7 +7550,7 @@
       <c r="V138" s="10"/>
       <c r="W138" s="10"/>
     </row>
-    <row r="139" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="28"/>
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
@@ -7430,7 +7575,7 @@
       <c r="V139" s="10"/>
       <c r="W139" s="10"/>
     </row>
-    <row r="140" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="28"/>
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
@@ -7455,7 +7600,7 @@
       <c r="V140" s="10"/>
       <c r="W140" s="10"/>
     </row>
-    <row r="141" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="28"/>
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
@@ -7480,7 +7625,7 @@
       <c r="V141" s="10"/>
       <c r="W141" s="10"/>
     </row>
-    <row r="142" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="28"/>
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
@@ -7505,7 +7650,7 @@
       <c r="V142" s="10"/>
       <c r="W142" s="10"/>
     </row>
-    <row r="143" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="28"/>
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
@@ -7530,7 +7675,7 @@
       <c r="V143" s="10"/>
       <c r="W143" s="10"/>
     </row>
-    <row r="144" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="60"/>
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
@@ -7555,7 +7700,7 @@
       <c r="V144" s="10"/>
       <c r="W144" s="10"/>
     </row>
-    <row r="145" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="61"/>
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
@@ -7580,7 +7725,7 @@
       <c r="V145" s="10"/>
       <c r="W145" s="10"/>
     </row>
-    <row r="146" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="70"/>
       <c r="B146" s="70"/>
       <c r="C146" s="28"/>
@@ -7605,7 +7750,7 @@
       <c r="V146" s="10"/>
       <c r="W146" s="10"/>
     </row>
-    <row r="147" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="28"/>
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
@@ -7630,7 +7775,7 @@
       <c r="V147" s="10"/>
       <c r="W147" s="10"/>
     </row>
-    <row r="148" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="28"/>
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
@@ -7655,7 +7800,7 @@
       <c r="V148" s="10"/>
       <c r="W148" s="10"/>
     </row>
-    <row r="149" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="28"/>
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
@@ -7680,7 +7825,7 @@
       <c r="V149" s="10"/>
       <c r="W149" s="10"/>
     </row>
-    <row r="150" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="28"/>
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
@@ -7705,7 +7850,7 @@
       <c r="V150" s="10"/>
       <c r="W150" s="10"/>
     </row>
-    <row r="151" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="70"/>
       <c r="B151" s="70"/>
       <c r="C151" s="28"/>
@@ -7730,7 +7875,7 @@
       <c r="V151" s="10"/>
       <c r="W151" s="10"/>
     </row>
-    <row r="152" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="28"/>
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
@@ -7755,7 +7900,7 @@
       <c r="V152" s="10"/>
       <c r="W152" s="10"/>
     </row>
-    <row r="153" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="28"/>
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
@@ -7780,7 +7925,7 @@
       <c r="V153" s="10"/>
       <c r="W153" s="10"/>
     </row>
-    <row r="154" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="28"/>
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
@@ -7805,7 +7950,7 @@
       <c r="V154" s="10"/>
       <c r="W154" s="10"/>
     </row>
-    <row r="155" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="28"/>
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
@@ -7830,7 +7975,7 @@
       <c r="V155" s="10"/>
       <c r="W155" s="10"/>
     </row>
-    <row r="156" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="28"/>
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
@@ -7855,7 +8000,7 @@
       <c r="V156" s="10"/>
       <c r="W156" s="10"/>
     </row>
-    <row r="157" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="20"/>
       <c r="C157" s="20"/>
@@ -7874,7 +8019,7 @@
       <c r="P157" s="20"/>
       <c r="Q157" s="20"/>
     </row>
-    <row r="158" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="28"/>
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
@@ -7911,7 +8056,7 @@
       <c r="AH158" s="10"/>
       <c r="AI158" s="10"/>
     </row>
-    <row r="159" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="28"/>
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
@@ -7948,7 +8093,7 @@
       <c r="AH159" s="10"/>
       <c r="AI159" s="10"/>
     </row>
-    <row r="160" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="60"/>
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
@@ -7985,7 +8130,7 @@
       <c r="AH160" s="10"/>
       <c r="AI160" s="10"/>
     </row>
-    <row r="161" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="61"/>
       <c r="B161" s="28"/>
       <c r="C161" s="28"/>
@@ -8022,7 +8167,7 @@
       <c r="AH161" s="10"/>
       <c r="AI161" s="10"/>
     </row>
-    <row r="162" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="61"/>
       <c r="B162" s="28"/>
       <c r="C162" s="28"/>
@@ -8059,7 +8204,7 @@
       <c r="AH162" s="10"/>
       <c r="AI162" s="10"/>
     </row>
-    <row r="163" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="28"/>
       <c r="B163" s="60"/>
       <c r="C163" s="60"/>
@@ -8096,7 +8241,7 @@
       <c r="AH163" s="10"/>
       <c r="AI163" s="10"/>
     </row>
-    <row r="164" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="63"/>
       <c r="B164" s="28"/>
       <c r="C164" s="28"/>
@@ -8133,7 +8278,7 @@
       <c r="AH164" s="10"/>
       <c r="AI164" s="10"/>
     </row>
-    <row r="165" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="28"/>
       <c r="B165" s="28"/>
       <c r="C165" s="28"/>
@@ -8170,7 +8315,7 @@
       <c r="AH165" s="10"/>
       <c r="AI165" s="10"/>
     </row>
-    <row r="166" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="62"/>
       <c r="B166" s="62"/>
       <c r="C166" s="62"/>
@@ -8207,7 +8352,7 @@
       <c r="AH166" s="10"/>
       <c r="AI166" s="10"/>
     </row>
-    <row r="167" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="62"/>
       <c r="B167" s="1"/>
       <c r="C167" s="53"/>
@@ -8244,7 +8389,7 @@
       <c r="AH167" s="10"/>
       <c r="AI167" s="10"/>
     </row>
-    <row r="168" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="28"/>
       <c r="B168" s="28"/>
       <c r="C168" s="28"/>
@@ -8281,7 +8426,7 @@
       <c r="AH168" s="10"/>
       <c r="AI168" s="10"/>
     </row>
-    <row r="169" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="B169" s="10"/>
       <c r="C169" s="10"/>
@@ -8318,7 +8463,7 @@
       <c r="AH169" s="10"/>
       <c r="AI169" s="10"/>
     </row>
-    <row r="170" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
       <c r="B170" s="10"/>
       <c r="C170" s="10"/>
@@ -8355,7 +8500,7 @@
       <c r="AH170" s="10"/>
       <c r="AI170" s="10"/>
     </row>
-    <row r="171" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="28"/>
       <c r="B171" s="28"/>
       <c r="C171" s="28"/>
@@ -8392,7 +8537,7 @@
       <c r="AH171" s="10"/>
       <c r="AI171" s="10"/>
     </row>
-    <row r="172" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="10"/>
       <c r="B172" s="10"/>
       <c r="C172" s="10"/>
@@ -8429,7 +8574,7 @@
       <c r="AH172" s="10"/>
       <c r="AI172" s="10"/>
     </row>
-    <row r="173" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="10"/>
       <c r="C173" s="10"/>
@@ -8466,7 +8611,7 @@
       <c r="AH173" s="10"/>
       <c r="AI173" s="10"/>
     </row>
-    <row r="174" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="28"/>
       <c r="B174" s="28"/>
       <c r="C174" s="28"/>
@@ -8503,7 +8648,7 @@
       <c r="AH174" s="10"/>
       <c r="AI174" s="10"/>
     </row>
-    <row r="175" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="28"/>
       <c r="B175" s="28"/>
       <c r="C175" s="28"/>
@@ -8540,7 +8685,7 @@
       <c r="AH175" s="10"/>
       <c r="AI175" s="10"/>
     </row>
-    <row r="176" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="28"/>
       <c r="B176" s="28"/>
       <c r="C176" s="28"/>
@@ -8577,7 +8722,7 @@
       <c r="AH176" s="10"/>
       <c r="AI176" s="10"/>
     </row>
-    <row r="177" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="20"/>
@@ -8596,7 +8741,7 @@
       <c r="P177" s="20"/>
       <c r="Q177" s="20"/>
     </row>
-    <row r="178" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="20"/>
       <c r="C178" s="20"/>
@@ -8615,7 +8760,7 @@
       <c r="P178" s="20"/>
       <c r="Q178" s="20"/>
     </row>
-    <row r="179" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="20"/>
       <c r="C179" s="20"/>
@@ -8634,7 +8779,7 @@
       <c r="P179" s="20"/>
       <c r="Q179" s="20"/>
     </row>
-    <row r="180" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="20"/>
       <c r="B180" s="20"/>
       <c r="C180" s="20"/>
@@ -8653,7 +8798,7 @@
       <c r="P180" s="20"/>
       <c r="Q180" s="20"/>
     </row>
-    <row r="181" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="20"/>
@@ -8672,7 +8817,7 @@
       <c r="P181" s="20"/>
       <c r="Q181" s="20"/>
     </row>
-    <row r="182" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="20"/>
       <c r="B182" s="20"/>
       <c r="C182" s="20"/>
@@ -8691,7 +8836,7 @@
       <c r="P182" s="20"/>
       <c r="Q182" s="20"/>
     </row>
-    <row r="183" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="20"/>
       <c r="B183" s="20"/>
       <c r="C183" s="20"/>
@@ -8710,7 +8855,7 @@
       <c r="P183" s="20"/>
       <c r="Q183" s="20"/>
     </row>
-    <row r="184" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="20"/>
       <c r="B184" s="20"/>
       <c r="C184" s="20"/>
@@ -8729,7 +8874,7 @@
       <c r="P184" s="20"/>
       <c r="Q184" s="20"/>
     </row>
-    <row r="185" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="20"/>
       <c r="B185" s="20"/>
       <c r="C185" s="20"/>
@@ -8748,7 +8893,7 @@
       <c r="P185" s="20"/>
       <c r="Q185" s="20"/>
     </row>
-    <row r="186" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="20"/>
       <c r="B186" s="20"/>
       <c r="C186" s="20"/>
@@ -8767,7 +8912,7 @@
       <c r="P186" s="20"/>
       <c r="Q186" s="20"/>
     </row>
-    <row r="187" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="20"/>
       <c r="B187" s="20"/>
       <c r="C187" s="20"/>

</xml_diff>

<commit_message>
Add HIV-associated mortality for persons on ART
Particulary in the early years when ART was started only with low CD4
count, evidence shows treated (suppressed) persons have HIV-associated
mortality. This is important for our model results of cervical cancer
outcomes stratified by ART use.

Define HIV-associated mortality for persons on ART relative to
background mortality rate. This is because relative risks relative to
HIV-negative persons are available as an all-cause relative risk.
Background mortality is stratified by age and gender and currently is
stable after 1985. However, code is set up for easy calculation of muART
if background mortality is decreasing during ART years.

Relative risk decreases over time as the average CD4 count at ART
initiation increases.

Related to #60
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="78">
   <si>
     <t>Male</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>CD4&lt;200 cells/uL</t>
-  </si>
-  <si>
-    <t>ART</t>
   </si>
   <si>
     <t>Age</t>
@@ -643,6 +640,11 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -679,11 +681,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1028,7 +1025,7 @@
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1096,7 +1093,7 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="22">
         <v>0.1</v>
@@ -1258,7 +1255,7 @@
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -1296,7 +1293,7 @@
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -1334,7 +1331,7 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -1372,7 +1369,7 @@
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
@@ -1410,7 +1407,7 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -1448,7 +1445,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -1486,7 +1483,7 @@
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -1525,13 +1522,13 @@
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>29</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -1555,7 +1552,7 @@
     </row>
     <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="22">
         <v>0.6</v>
@@ -1584,7 +1581,7 @@
     </row>
     <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="22">
         <v>0.8</v>
@@ -1664,7 +1661,7 @@
       <c r="AI21" s="4"/>
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="30"/>
       <c r="C22" s="19"/>
       <c r="Q22" s="4"/>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
-      <c r="B25" s="80"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="19"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -1856,23 +1853,23 @@
       <c r="AI29" s="4"/>
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="66"/>
-      <c r="N30" s="66"/>
-      <c r="O30" s="66"/>
+      <c r="A30" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -1894,23 +1891,23 @@
       <c r="AI30" s="4"/>
     </row>
     <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
+      <c r="A31" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -1936,10 +1933,10 @@
         <v>15</v>
       </c>
       <c r="B32" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>77</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -2481,7 +2478,7 @@
   <dimension ref="A1:AX187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2526,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -2551,10 +2548,10 @@
     </row>
     <row r="2" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2578,7 +2575,7 @@
         <v>2005</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2599,10 +2596,10 @@
     </row>
     <row r="4" spans="1:38" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2638,7 +2635,7 @@
     </row>
     <row r="6" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="12">
         <v>0.34</v>
@@ -2668,7 +2665,7 @@
     </row>
     <row r="8" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="43">
         <v>7.0999999999999994E-2</v>
@@ -2738,7 +2735,7 @@
     </row>
     <row r="14" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -2770,10 +2767,10 @@
     </row>
     <row r="15" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -2804,10 +2801,10 @@
     </row>
     <row r="16" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -2838,10 +2835,10 @@
     </row>
     <row r="17" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -2872,7 +2869,7 @@
     </row>
     <row r="18" spans="1:38" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -2880,8 +2877,8 @@
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="19"/>
       <c r="AC18" s="4"/>
       <c r="AD18" s="6"/>
@@ -2899,7 +2896,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>19</v>
@@ -2916,10 +2913,8 @@
       <c r="G19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="35" t="s">
-        <v>23</v>
-      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="19"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="8"/>
@@ -2954,8 +2949,8 @@
       <c r="G20" s="22">
         <v>0.47</v>
       </c>
-      <c r="H20" s="35"/>
-      <c r="I20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="19"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="8"/>
@@ -2978,20 +2973,20 @@
       <c r="C21" s="22">
         <v>0</v>
       </c>
-      <c r="D21" s="78">
+      <c r="D21" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F21" s="78">
+      <c r="F21" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G21" s="78">
+      <c r="G21" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="26"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="19"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="8"/>
@@ -3014,20 +3009,20 @@
       <c r="C22" s="22">
         <v>0</v>
       </c>
-      <c r="D22" s="78">
+      <c r="D22" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F22" s="78">
+      <c r="F22" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G22" s="78">
+      <c r="G22" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="26"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="19"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="8"/>
@@ -3050,20 +3045,20 @@
       <c r="C23" s="22">
         <v>0</v>
       </c>
-      <c r="D23" s="78">
+      <c r="D23" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E23" s="78">
+      <c r="E23" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F23" s="78">
+      <c r="F23" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G23" s="78">
+      <c r="G23" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="26"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="19"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="8"/>
@@ -3086,20 +3081,20 @@
       <c r="C24" s="22">
         <v>0</v>
       </c>
-      <c r="D24" s="78">
+      <c r="D24" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E24" s="78">
+      <c r="E24" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F24" s="78">
+      <c r="F24" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G24" s="78">
+      <c r="G24" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="26"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="19"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="8"/>
@@ -3122,20 +3117,20 @@
       <c r="C25" s="22">
         <v>0</v>
       </c>
-      <c r="D25" s="78">
+      <c r="D25" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E25" s="78">
+      <c r="E25" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F25" s="78">
+      <c r="F25" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G25" s="78">
+      <c r="G25" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="26"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="19"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="8"/>
@@ -3158,20 +3153,20 @@
       <c r="C26" s="22">
         <v>0</v>
       </c>
-      <c r="D26" s="78">
+      <c r="D26" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E26" s="78">
+      <c r="E26" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F26" s="78">
+      <c r="F26" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G26" s="78">
+      <c r="G26" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="26"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="19"/>
       <c r="AC26" s="4"/>
       <c r="AD26" s="8"/>
@@ -3194,20 +3189,20 @@
       <c r="C27" s="22">
         <v>0</v>
       </c>
-      <c r="D27" s="78">
+      <c r="D27" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E27" s="78">
+      <c r="E27" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F27" s="78">
+      <c r="F27" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G27" s="78">
+      <c r="G27" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="26"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="19"/>
       <c r="AC27" s="4"/>
       <c r="AD27" s="8"/>
@@ -3230,20 +3225,20 @@
       <c r="C28" s="22">
         <v>0</v>
       </c>
-      <c r="D28" s="78">
+      <c r="D28" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E28" s="78">
+      <c r="E28" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F28" s="78">
+      <c r="F28" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G28" s="78">
+      <c r="G28" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="26"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="19"/>
       <c r="AC28" s="4"/>
       <c r="AD28" s="8"/>
@@ -3266,20 +3261,20 @@
       <c r="C29" s="22">
         <v>0</v>
       </c>
-      <c r="D29" s="78">
+      <c r="D29" s="66">
         <v>3.5300000000000002E-3</v>
       </c>
-      <c r="E29" s="78">
+      <c r="E29" s="66">
         <v>2.5530000000000001E-2</v>
       </c>
-      <c r="F29" s="78">
+      <c r="F29" s="66">
         <v>4.5530000000000001E-2</v>
       </c>
-      <c r="G29" s="78">
+      <c r="G29" s="66">
         <v>0.26552999999999999</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="26"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="19"/>
       <c r="AC29" s="4"/>
       <c r="AD29" s="8"/>
@@ -3318,8 +3313,8 @@
         <f t="shared" si="0"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="26"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="19"/>
       <c r="AC30" s="4"/>
       <c r="AD30" s="8"/>
@@ -3358,8 +3353,8 @@
         <f t="shared" si="1"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="26"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="19"/>
       <c r="AC31" s="4"/>
       <c r="AD31" s="4"/>
@@ -3374,7 +3369,7 @@
     </row>
     <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="22">
         <v>0</v>
@@ -3398,8 +3393,8 @@
         <f t="shared" si="1"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="26"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="19"/>
       <c r="AC32" s="4"/>
       <c r="AD32" s="4"/>
@@ -3414,7 +3409,7 @@
     </row>
     <row r="33" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="22">
         <v>0</v>
@@ -3438,8 +3433,8 @@
         <f t="shared" si="1"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="26"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="19"/>
       <c r="AC33" s="4"/>
       <c r="AD33" s="4"/>
@@ -3454,7 +3449,7 @@
     </row>
     <row r="34" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="22">
         <v>0</v>
@@ -3478,8 +3473,8 @@
         <f t="shared" si="1"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="26"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="19"/>
       <c r="AC34" s="4"/>
       <c r="AD34" s="4"/>
@@ -3494,7 +3489,7 @@
     </row>
     <row r="35" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="22">
         <v>0</v>
@@ -3518,8 +3513,8 @@
         <f t="shared" si="1"/>
         <v>0.53105999999999998</v>
       </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="26"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="19"/>
       <c r="AC35" s="4"/>
       <c r="AD35" s="4"/>
@@ -3608,7 +3603,7 @@
     </row>
     <row r="41" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
@@ -3630,10 +3625,10 @@
     </row>
     <row r="42" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
       <c r="F42" s="19"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
@@ -3647,72 +3642,72 @@
     <row r="43" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="26"/>
       <c r="B43" s="53"/>
-      <c r="C43" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69"/>
+      <c r="C43" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="72"/>
       <c r="G43" s="50"/>
       <c r="H43" s="26"/>
       <c r="I43" s="56"/>
-      <c r="J43" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="69"/>
+      <c r="J43" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="K43" s="71"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="N43" s="72"/>
       <c r="O43" s="26"/>
     </row>
     <row r="44" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="F44" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="M44" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="N44" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N44" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="O44" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AX44" s="16"/>
     </row>
     <row r="45" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="73" t="s">
+      <c r="A45" s="76" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3735,7 +3730,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G45" s="20"/>
-      <c r="H45" s="74" t="s">
+      <c r="H45" s="77" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -3763,7 +3758,7 @@
       <c r="AX45" s="15"/>
     </row>
     <row r="46" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="73"/>
+      <c r="A46" s="76"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3784,7 +3779,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="20"/>
-      <c r="H46" s="75"/>
+      <c r="H46" s="78"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3810,7 +3805,7 @@
       <c r="AX46" s="9"/>
     </row>
     <row r="47" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="73"/>
+      <c r="A47" s="76"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3831,7 +3826,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="20"/>
-      <c r="H47" s="75"/>
+      <c r="H47" s="78"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3857,7 +3852,7 @@
       <c r="AX47" s="9"/>
     </row>
     <row r="48" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="73"/>
+      <c r="A48" s="76"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3878,7 +3873,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="20"/>
-      <c r="H48" s="75"/>
+      <c r="H48" s="78"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3904,7 +3899,7 @@
       <c r="AX48" s="9"/>
     </row>
     <row r="49" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="73"/>
+      <c r="A49" s="76"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3925,7 +3920,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="20"/>
-      <c r="H49" s="75"/>
+      <c r="H49" s="78"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3950,7 +3945,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="73"/>
+      <c r="A50" s="76"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -3971,7 +3966,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="20"/>
-      <c r="H50" s="75"/>
+      <c r="H50" s="78"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -3996,7 +3991,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="73"/>
+      <c r="A51" s="76"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4017,7 +4012,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="20"/>
-      <c r="H51" s="75"/>
+      <c r="H51" s="78"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4042,7 +4037,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="73"/>
+      <c r="A52" s="76"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4063,7 +4058,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="20"/>
-      <c r="H52" s="75"/>
+      <c r="H52" s="78"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4088,7 +4083,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="73"/>
+      <c r="A53" s="76"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4109,7 +4104,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="20"/>
-      <c r="H53" s="75"/>
+      <c r="H53" s="78"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4134,7 +4129,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="73"/>
+      <c r="A54" s="76"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4155,7 +4150,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="20"/>
-      <c r="H54" s="75"/>
+      <c r="H54" s="78"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4180,7 +4175,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="73"/>
+      <c r="A55" s="76"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4201,7 +4196,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="20"/>
-      <c r="H55" s="75"/>
+      <c r="H55" s="78"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4226,7 +4221,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="73"/>
+      <c r="A56" s="76"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4247,7 +4242,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="20"/>
-      <c r="H56" s="75"/>
+      <c r="H56" s="78"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4272,9 +4267,9 @@
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="73"/>
+      <c r="A57" s="76"/>
       <c r="B57" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" s="22">
         <f t="shared" si="2"/>
@@ -4293,9 +4288,9 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="20"/>
-      <c r="H57" s="75"/>
+      <c r="H57" s="78"/>
       <c r="I57" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J57" s="26">
         <v>0.25</v>
@@ -4318,9 +4313,9 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
+      <c r="A58" s="76"/>
       <c r="B58" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C58" s="22">
         <f t="shared" si="2"/>
@@ -4339,9 +4334,9 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="20"/>
-      <c r="H58" s="75"/>
+      <c r="H58" s="78"/>
       <c r="I58" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J58" s="26">
         <v>0.25</v>
@@ -4364,9 +4359,9 @@
       </c>
     </row>
     <row r="59" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="73"/>
+      <c r="A59" s="76"/>
       <c r="B59" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59" s="22">
         <f t="shared" si="2"/>
@@ -4385,9 +4380,9 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="20"/>
-      <c r="H59" s="75"/>
+      <c r="H59" s="78"/>
       <c r="I59" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J59" s="26">
         <v>0.25</v>
@@ -4410,9 +4405,9 @@
       </c>
     </row>
     <row r="60" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="73"/>
+      <c r="A60" s="76"/>
       <c r="B60" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C60" s="22">
         <f t="shared" si="2"/>
@@ -4431,9 +4426,9 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="20"/>
-      <c r="H60" s="76"/>
+      <c r="H60" s="79"/>
       <c r="I60" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J60" s="26">
         <v>0.25</v>
@@ -4473,7 +4468,7 @@
       <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="74" t="s">
+      <c r="A62" s="77" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -4496,7 +4491,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G62" s="20"/>
-      <c r="H62" s="74" t="s">
+      <c r="H62" s="77" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -4523,7 +4518,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="75"/>
+      <c r="A63" s="78"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4544,7 +4539,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="20"/>
-      <c r="H63" s="75"/>
+      <c r="H63" s="78"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4569,7 +4564,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="75"/>
+      <c r="A64" s="78"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4590,7 +4585,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="20"/>
-      <c r="H64" s="75"/>
+      <c r="H64" s="78"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4615,7 +4610,7 @@
       </c>
     </row>
     <row r="65" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="75"/>
+      <c r="A65" s="78"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4636,7 +4631,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="20"/>
-      <c r="H65" s="75"/>
+      <c r="H65" s="78"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4661,7 +4656,7 @@
       </c>
     </row>
     <row r="66" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="75"/>
+      <c r="A66" s="78"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4682,7 +4677,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="20"/>
-      <c r="H66" s="75"/>
+      <c r="H66" s="78"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4707,7 +4702,7 @@
       </c>
     </row>
     <row r="67" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="75"/>
+      <c r="A67" s="78"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4728,7 +4723,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="20"/>
-      <c r="H67" s="75"/>
+      <c r="H67" s="78"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4753,7 +4748,7 @@
       </c>
     </row>
     <row r="68" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="75"/>
+      <c r="A68" s="78"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4774,7 +4769,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="20"/>
-      <c r="H68" s="75"/>
+      <c r="H68" s="78"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4799,7 +4794,7 @@
       </c>
     </row>
     <row r="69" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
+      <c r="A69" s="78"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4820,7 +4815,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="20"/>
-      <c r="H69" s="75"/>
+      <c r="H69" s="78"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4845,7 +4840,7 @@
       </c>
     </row>
     <row r="70" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="75"/>
+      <c r="A70" s="78"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4866,7 +4861,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="20"/>
-      <c r="H70" s="75"/>
+      <c r="H70" s="78"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4891,7 +4886,7 @@
       </c>
     </row>
     <row r="71" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="75"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4912,7 +4907,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="20"/>
-      <c r="H71" s="75"/>
+      <c r="H71" s="78"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4937,7 +4932,7 @@
       </c>
     </row>
     <row r="72" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="75"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
@@ -4958,7 +4953,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="20"/>
-      <c r="H72" s="75"/>
+      <c r="H72" s="78"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -4983,7 +4978,7 @@
       </c>
     </row>
     <row r="73" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="75"/>
+      <c r="A73" s="78"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5004,7 +4999,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="20"/>
-      <c r="H73" s="75"/>
+      <c r="H73" s="78"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5029,9 +5024,9 @@
       </c>
     </row>
     <row r="74" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="75"/>
+      <c r="A74" s="78"/>
       <c r="B74" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C74" s="22">
         <f t="shared" si="7"/>
@@ -5050,9 +5045,9 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="20"/>
-      <c r="H74" s="75"/>
+      <c r="H74" s="78"/>
       <c r="I74" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J74" s="26">
         <v>0.25</v>
@@ -5075,9 +5070,9 @@
       </c>
     </row>
     <row r="75" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="75"/>
+      <c r="A75" s="78"/>
       <c r="B75" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C75" s="22">
         <f t="shared" si="7"/>
@@ -5096,9 +5091,9 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="20"/>
-      <c r="H75" s="75"/>
+      <c r="H75" s="78"/>
       <c r="I75" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J75" s="26">
         <v>0.25</v>
@@ -5121,9 +5116,9 @@
       </c>
     </row>
     <row r="76" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="75"/>
+      <c r="A76" s="78"/>
       <c r="B76" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C76" s="22">
         <f t="shared" si="7"/>
@@ -5142,9 +5137,9 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="20"/>
-      <c r="H76" s="75"/>
+      <c r="H76" s="78"/>
       <c r="I76" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J76" s="26">
         <v>0.25</v>
@@ -5167,9 +5162,9 @@
       </c>
     </row>
     <row r="77" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="76"/>
+      <c r="A77" s="79"/>
       <c r="B77" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C77" s="22">
         <f t="shared" si="7"/>
@@ -5188,9 +5183,9 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="20"/>
-      <c r="H77" s="76"/>
+      <c r="H77" s="79"/>
       <c r="I77" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J77" s="26">
         <v>0.25</v>
@@ -5252,7 +5247,7 @@
     </row>
     <row r="80" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
@@ -5275,10 +5270,10 @@
     </row>
     <row r="81" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
-      <c r="B81" s="71"/>
-      <c r="C81" s="71"/>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71"/>
+      <c r="B81" s="74"/>
+      <c r="C81" s="74"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
       <c r="F81" s="19"/>
       <c r="G81" s="48"/>
       <c r="H81" s="48"/>
@@ -5296,22 +5291,22 @@
     <row r="82" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="37"/>
       <c r="B82" s="37"/>
-      <c r="C82" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="D82" s="77"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="77"/>
+      <c r="C82" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="D82" s="80"/>
+      <c r="E82" s="80"/>
+      <c r="F82" s="80"/>
       <c r="G82" s="20"/>
       <c r="H82" s="26"/>
       <c r="I82" s="56"/>
-      <c r="J82" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="K82" s="68"/>
-      <c r="L82" s="68"/>
-      <c r="M82" s="68"/>
-      <c r="N82" s="69"/>
+      <c r="J82" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="K82" s="71"/>
+      <c r="L82" s="71"/>
+      <c r="M82" s="71"/>
+      <c r="N82" s="72"/>
       <c r="O82" s="26"/>
       <c r="P82" s="19"/>
       <c r="Q82" s="19"/>
@@ -5319,54 +5314,54 @@
     </row>
     <row r="83" spans="1:28" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B83" s="57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="F83" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="G83" s="48"/>
       <c r="H83" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I83" s="57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J83" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K83" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L83" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L83" s="5" t="s">
+      <c r="M83" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M83" s="5" t="s">
+      <c r="N83" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N83" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="O83" s="54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P83" s="19"/>
       <c r="Q83" s="19"/>
       <c r="AB83" s="14"/>
     </row>
     <row r="84" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="73" t="s">
+      <c r="A84" s="76" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5389,7 +5384,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="48"/>
-      <c r="H84" s="74" t="s">
+      <c r="H84" s="77" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5418,7 +5413,7 @@
       <c r="AB84" s="14"/>
     </row>
     <row r="85" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="73"/>
+      <c r="A85" s="76"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5439,7 +5434,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="48"/>
-      <c r="H85" s="75"/>
+      <c r="H85" s="78"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5466,7 +5461,7 @@
       <c r="AB85" s="14"/>
     </row>
     <row r="86" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="73"/>
+      <c r="A86" s="76"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="48"/>
-      <c r="H86" s="75"/>
+      <c r="H86" s="78"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5514,7 +5509,7 @@
       <c r="AB86" s="14"/>
     </row>
     <row r="87" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="73"/>
+      <c r="A87" s="76"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5535,7 +5530,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="20"/>
-      <c r="H87" s="75"/>
+      <c r="H87" s="78"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5562,7 +5557,7 @@
       <c r="AB87" s="14"/>
     </row>
     <row r="88" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="73"/>
+      <c r="A88" s="76"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="48"/>
-      <c r="H88" s="75"/>
+      <c r="H88" s="78"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5610,7 +5605,7 @@
       <c r="AB88" s="14"/>
     </row>
     <row r="89" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="73"/>
+      <c r="A89" s="76"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5631,7 +5626,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="20"/>
-      <c r="H89" s="75"/>
+      <c r="H89" s="78"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5659,7 +5654,7 @@
       <c r="AB89" s="14"/>
     </row>
     <row r="90" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="73"/>
+      <c r="A90" s="76"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5680,7 +5675,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="48"/>
-      <c r="H90" s="75"/>
+      <c r="H90" s="78"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5706,7 +5701,7 @@
       <c r="AB90" s="14"/>
     </row>
     <row r="91" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="73"/>
+      <c r="A91" s="76"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5727,7 +5722,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="48"/>
-      <c r="H91" s="75"/>
+      <c r="H91" s="78"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5753,7 +5748,7 @@
       <c r="AB91" s="14"/>
     </row>
     <row r="92" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="73"/>
+      <c r="A92" s="76"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5774,7 +5769,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="48"/>
-      <c r="H92" s="75"/>
+      <c r="H92" s="78"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5800,7 +5795,7 @@
       <c r="AB92" s="14"/>
     </row>
     <row r="93" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="73"/>
+      <c r="A93" s="76"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5821,7 +5816,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="48"/>
-      <c r="H93" s="75"/>
+      <c r="H93" s="78"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5847,7 +5842,7 @@
       <c r="AB93" s="14"/>
     </row>
     <row r="94" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="73"/>
+      <c r="A94" s="76"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5868,7 +5863,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="20"/>
-      <c r="H94" s="75"/>
+      <c r="H94" s="78"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5894,7 +5889,7 @@
       <c r="AB94" s="14"/>
     </row>
     <row r="95" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="73"/>
+      <c r="A95" s="76"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5915,7 +5910,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="20"/>
-      <c r="H95" s="75"/>
+      <c r="H95" s="78"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5943,9 +5938,9 @@
       <c r="AB95" s="14"/>
     </row>
     <row r="96" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="73"/>
+      <c r="A96" s="76"/>
       <c r="B96" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C96" s="22">
         <f t="shared" si="13"/>
@@ -5964,9 +5959,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="20"/>
-      <c r="H96" s="75"/>
+      <c r="H96" s="78"/>
       <c r="I96" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J96" s="26">
         <v>0.25</v>
@@ -5992,9 +5987,9 @@
       <c r="AB96" s="14"/>
     </row>
     <row r="97" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="73"/>
+      <c r="A97" s="76"/>
       <c r="B97" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C97" s="22">
         <f t="shared" si="13"/>
@@ -6013,9 +6008,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="19"/>
-      <c r="H97" s="75"/>
+      <c r="H97" s="78"/>
       <c r="I97" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J97" s="26">
         <v>0.25</v>
@@ -6041,9 +6036,9 @@
       <c r="AB97" s="14"/>
     </row>
     <row r="98" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="73"/>
+      <c r="A98" s="76"/>
       <c r="B98" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C98" s="22">
         <f t="shared" si="13"/>
@@ -6062,9 +6057,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="19"/>
-      <c r="H98" s="75"/>
+      <c r="H98" s="78"/>
       <c r="I98" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J98" s="26">
         <v>0.25</v>
@@ -6089,9 +6084,9 @@
       <c r="Q98" s="19"/>
     </row>
     <row r="99" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="73"/>
+      <c r="A99" s="76"/>
       <c r="B99" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C99" s="22">
         <f t="shared" si="13"/>
@@ -6110,9 +6105,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="19"/>
-      <c r="H99" s="76"/>
+      <c r="H99" s="79"/>
       <c r="I99" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J99" s="26">
         <v>0.25</v>
@@ -6156,7 +6151,7 @@
       <c r="Q100" s="19"/>
     </row>
     <row r="101" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="74" t="s">
+      <c r="A101" s="77" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6179,7 +6174,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="19"/>
-      <c r="H101" s="74" t="s">
+      <c r="H101" s="77" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6208,7 +6203,7 @@
       <c r="Q101" s="19"/>
     </row>
     <row r="102" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="75"/>
+      <c r="A102" s="78"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6229,7 +6224,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="19"/>
-      <c r="H102" s="75"/>
+      <c r="H102" s="78"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6256,7 +6251,7 @@
       <c r="Q102" s="19"/>
     </row>
     <row r="103" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="75"/>
+      <c r="A103" s="78"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6277,7 +6272,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="19"/>
-      <c r="H103" s="75"/>
+      <c r="H103" s="78"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6304,7 +6299,7 @@
       <c r="Q103" s="19"/>
     </row>
     <row r="104" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="75"/>
+      <c r="A104" s="78"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6325,7 +6320,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="19"/>
-      <c r="H104" s="75"/>
+      <c r="H104" s="78"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6352,7 +6347,7 @@
       <c r="Q104" s="19"/>
     </row>
     <row r="105" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="75"/>
+      <c r="A105" s="78"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6373,7 +6368,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="19"/>
-      <c r="H105" s="75"/>
+      <c r="H105" s="78"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6400,7 +6395,7 @@
       <c r="Q105" s="19"/>
     </row>
     <row r="106" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="75"/>
+      <c r="A106" s="78"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6421,7 +6416,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="19"/>
-      <c r="H106" s="75"/>
+      <c r="H106" s="78"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6448,7 +6443,7 @@
       <c r="Q106" s="19"/>
     </row>
     <row r="107" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="75"/>
+      <c r="A107" s="78"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6469,7 +6464,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="19"/>
-      <c r="H107" s="75"/>
+      <c r="H107" s="78"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6496,7 +6491,7 @@
       <c r="Q107" s="19"/>
     </row>
     <row r="108" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="75"/>
+      <c r="A108" s="78"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6517,7 +6512,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="19"/>
-      <c r="H108" s="75"/>
+      <c r="H108" s="78"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6544,7 +6539,7 @@
       <c r="Q108" s="19"/>
     </row>
     <row r="109" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="75"/>
+      <c r="A109" s="78"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6565,7 +6560,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="19"/>
-      <c r="H109" s="75"/>
+      <c r="H109" s="78"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6592,7 +6587,7 @@
       <c r="Q109" s="19"/>
     </row>
     <row r="110" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="75"/>
+      <c r="A110" s="78"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6613,7 +6608,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="19"/>
-      <c r="H110" s="75"/>
+      <c r="H110" s="78"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6640,7 +6635,7 @@
       <c r="Q110" s="19"/>
     </row>
     <row r="111" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="75"/>
+      <c r="A111" s="78"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6661,7 +6656,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="19"/>
-      <c r="H111" s="75"/>
+      <c r="H111" s="78"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6688,7 +6683,7 @@
       <c r="Q111" s="19"/>
     </row>
     <row r="112" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="75"/>
+      <c r="A112" s="78"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6709,7 +6704,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="19"/>
-      <c r="H112" s="75"/>
+      <c r="H112" s="78"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6736,9 +6731,9 @@
       <c r="Q112" s="19"/>
     </row>
     <row r="113" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="75"/>
+      <c r="A113" s="78"/>
       <c r="B113" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C113" s="22">
         <f t="shared" si="16"/>
@@ -6757,9 +6752,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="19"/>
-      <c r="H113" s="75"/>
+      <c r="H113" s="78"/>
       <c r="I113" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J113" s="26">
         <v>0.25</v>
@@ -6784,9 +6779,9 @@
       <c r="Q113" s="19"/>
     </row>
     <row r="114" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="75"/>
+      <c r="A114" s="78"/>
       <c r="B114" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C114" s="22">
         <f t="shared" si="16"/>
@@ -6805,9 +6800,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="19"/>
-      <c r="H114" s="75"/>
+      <c r="H114" s="78"/>
       <c r="I114" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J114" s="26">
         <v>0.25</v>
@@ -6832,9 +6827,9 @@
       <c r="Q114" s="19"/>
     </row>
     <row r="115" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="75"/>
+      <c r="A115" s="78"/>
       <c r="B115" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C115" s="22">
         <f t="shared" si="16"/>
@@ -6853,9 +6848,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="19"/>
-      <c r="H115" s="75"/>
+      <c r="H115" s="78"/>
       <c r="I115" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J115" s="26">
         <v>0.25</v>
@@ -6880,9 +6875,9 @@
       <c r="Q115" s="19"/>
     </row>
     <row r="116" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="76"/>
+      <c r="A116" s="79"/>
       <c r="B116" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C116" s="22">
         <f t="shared" si="16"/>
@@ -6901,9 +6896,9 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="14"/>
-      <c r="H116" s="76"/>
+      <c r="H116" s="79"/>
       <c r="I116" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J116" s="26">
         <v>0.25</v>
@@ -7640,8 +7635,8 @@
       <c r="W145" s="9"/>
     </row>
     <row r="146" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="72"/>
-      <c r="B146" s="72"/>
+      <c r="A146" s="75"/>
+      <c r="B146" s="75"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
       <c r="E146" s="27"/>
@@ -7765,8 +7760,8 @@
       <c r="W150" s="9"/>
     </row>
     <row r="151" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="72"/>
-      <c r="B151" s="72"/>
+      <c r="A151" s="75"/>
+      <c r="B151" s="75"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
       <c r="E151" s="27"/>

</xml_diff>

<commit_message>
Update sources for HIV-associated mortality
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -186,23 +186,7 @@
     <t>M. L. Newell et al., Mortality of infected and uninfected infants born to HIV-infected mothers in Africa: a pooled analysis. Lancet 364, 1236-1243 (2004).</t>
   </si>
   <si>
-    <t>M. Badri, S. D. Lawn, R. Wood, Short-term risk of AIDS or death in people infected with HIV-1 before antiretroviral therapy in South Africa: a longitudinal study. Lancet 368, 1254-1259 (2006).</t>
-  </si>
-  <si>
     <t>W. H. Adler et al., HIV infection and aging: mechanisms to explain the accelerated rate of progression in the older patient. Mech Ageing Dev 96, 137-155 (1997).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HIV-associated mortality. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Values are estimates from observational studies of untreated HIV-positive persons. Persons age 0 to 4 and older than 50 are assumed to have greater mortality as observed.</t>
-    </r>
   </si>
   <si>
     <t>HIV-associated Mortality</t>
@@ -280,6 +264,22 @@
   </si>
   <si>
     <t>Viral suppression among all PLWHIV on ART in KZN</t>
+  </si>
+  <si>
+    <t>M. Badri, S. D. Lawn, R. Wood, Short-term risk of AIDS or death in people infected with HIV-1 before antiretroviral therapy in South Africa: a longitudinal study. Lancet 368, 1254-1259 (2006).; Lewden C. et al., CD4-specific mortality rates among HIV-infected adults with high CD4 counts and no antiretroviral treatment in West Africa. J Acquir Immune Defic Syndr. (2012) 1; 59(2):213-219.; Maduna, PH. et al. Morbidity and mortality according to latest CD4+ cell count among HIV positive individuals in South Africa who enrolled in project Phidisa. PLoS One. (2015). 9;10(4).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HIV-associated mortality. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Values are estimates from studies of untreated HIV-positive persons. Persons age 0 to 4 and older than 50 are assumed to have greater mortality as observed. Related to GitHub issue #85.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -680,6 +680,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1854,7 +1857,7 @@
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="69" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="69"/>
       <c r="C30" s="69"/>
@@ -1892,7 +1895,7 @@
     </row>
     <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="70" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" s="70"/>
       <c r="C31" s="70"/>
@@ -1933,10 +1936,10 @@
         <v>15</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -2478,7 +2481,7 @@
   <dimension ref="A1:AX187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,7 +2529,7 @@
   <sheetData>
     <row r="1" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -2548,10 +2551,10 @@
     </row>
     <row r="2" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -2575,7 +2578,7 @@
         <v>2005</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2596,10 +2599,10 @@
     </row>
     <row r="4" spans="1:38" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -2635,7 +2638,7 @@
     </row>
     <row r="6" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="12">
         <v>0.34</v>
@@ -2665,7 +2668,7 @@
     </row>
     <row r="8" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="43">
         <v>7.0999999999999994E-2</v>
@@ -2735,7 +2738,7 @@
     </row>
     <row r="14" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -2799,24 +2802,24 @@
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" s="14" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="B16" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
@@ -2838,7 +2841,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -2869,7 +2872,7 @@
     </row>
     <row r="18" spans="1:38" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -3603,7 +3606,7 @@
     </row>
     <row r="41" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
@@ -3643,7 +3646,7 @@
       <c r="A43" s="26"/>
       <c r="B43" s="53"/>
       <c r="C43" s="73" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D43" s="71"/>
       <c r="E43" s="71"/>
@@ -3652,7 +3655,7 @@
       <c r="H43" s="26"/>
       <c r="I43" s="56"/>
       <c r="J43" s="71" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K43" s="71"/>
       <c r="L43" s="71"/>
@@ -5247,7 +5250,7 @@
     </row>
     <row r="80" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
@@ -5292,7 +5295,7 @@
       <c r="A82" s="37"/>
       <c r="B82" s="37"/>
       <c r="C82" s="80" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D82" s="80"/>
       <c r="E82" s="80"/>
@@ -5301,7 +5304,7 @@
       <c r="H82" s="26"/>
       <c r="I82" s="56"/>
       <c r="J82" s="71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K82" s="71"/>
       <c r="L82" s="71"/>
@@ -5323,13 +5326,13 @@
         <v>17</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="G83" s="48"/>
       <c r="H83" s="57" t="s">
@@ -5342,16 +5345,16 @@
         <v>17</v>
       </c>
       <c r="K83" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L83" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M83" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="L83" s="5" t="s">
+      <c r="N83" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="M83" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N83" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="O83" s="54" t="s">
         <v>31</v>
@@ -8841,7 +8844,8 @@
       <c r="Q187" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="B16:M16"/>
     <mergeCell ref="J43:N43"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="B42:E42"/>

</xml_diff>

<commit_message>
Update Excel documentation of VMMC parameters
</commit_message>
<xml_diff>
--- a/Config/HIV_parameters.xlsx
+++ b/Config/HIV_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Protection" sheetId="5" r:id="rId1"/>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>R. V. Barnabas et al., paper presented at the Treatment as Prevention, Vancouver, Canada, 2012.</t>
-  </si>
-  <si>
-    <t>Circumcision rate in KZN.</t>
   </si>
   <si>
     <t>Protection probability conferred by circumcision and condom use.</t>
@@ -308,6 +305,20 @@
   </si>
   <si>
     <t>Hubert JB, Burgard M, Dussaix E, Tamalet C, Deveau C, Le Chenadec J, et al. Natural history of serum HIV-1 RNA levels in 330 patients with a known date of infection. The SEROCO Study Group. AIDS 2000;14:123–31. https://doi.org/10.1097/00002030-200001280-00007.;                                                                Lyles RH, Muñoz A, Yamashita TE, Bazmi H, Detels R, Rinaldo CR, et al. Natural history of human immunodeficiency virus type 1 viremia after seroconversion and proximal to AIDS in a large cohort of homosexual men. Multicenter AIDS Cohort Study. J Infect Dis 2000;181:872–80. https://doi.org/10.1086/315339.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Circumcision rate in KZN. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Not currently used. Hardcoded instead based on the Circumcision_parameters_04092020.xlsx spreadsheet. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -672,23 +683,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -705,14 +705,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1003,25 +1014,25 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1057,7 +1068,7 @@
       <c r="AH1" s="4"/>
       <c r="AI1" s="4"/>
     </row>
-    <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>40</v>
       </c>
@@ -1095,7 +1106,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>15</v>
       </c>
@@ -1125,14 +1136,14 @@
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
     </row>
-    <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="34">
         <v>0.1</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="34">
         <v>0.1</v>
       </c>
       <c r="Q4" s="4"/>
@@ -1155,7 +1166,7 @@
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
     </row>
-    <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -1179,7 +1190,7 @@
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
     </row>
-    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -1206,7 +1217,7 @@
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
     </row>
-    <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1233,7 +1244,7 @@
       <c r="AH7" s="4"/>
       <c r="AI7" s="4"/>
     </row>
-    <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1260,7 +1271,7 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
     </row>
-    <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -1287,9 +1298,9 @@
       <c r="AH9" s="4"/>
       <c r="AI9" s="4"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -1325,9 +1336,9 @@
       <c r="AH10" s="4"/>
       <c r="AI10" s="4"/>
     </row>
-    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -1363,9 +1374,9 @@
       <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
     </row>
-    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -1401,9 +1412,9 @@
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
     </row>
-    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -1439,9 +1450,9 @@
       <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
     </row>
-    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -1477,9 +1488,9 @@
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
     </row>
-    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -1515,9 +1526,9 @@
       <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
     </row>
-    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -1553,7 +1564,7 @@
       <c r="AH16" s="4"/>
       <c r="AI16" s="4"/>
     </row>
-    <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="25"/>
       <c r="B17" s="25" t="s">
         <v>25</v>
@@ -1584,7 +1595,7 @@
       <c r="AH17" s="4"/>
       <c r="AI17" s="4"/>
     </row>
-    <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
@@ -1613,7 +1624,7 @@
       <c r="AH18" s="4"/>
       <c r="AI18" s="4"/>
     </row>
-    <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
@@ -1646,7 +1657,7 @@
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
     </row>
-    <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1670,7 +1681,7 @@
       <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
     </row>
-    <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="26"/>
       <c r="B21" s="4"/>
       <c r="C21" s="18"/>
@@ -1694,7 +1705,7 @@
       <c r="AH21" s="4"/>
       <c r="AI21" s="4"/>
     </row>
-    <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="66"/>
       <c r="B22" s="29"/>
       <c r="C22" s="18"/>
@@ -1718,7 +1729,7 @@
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
     </row>
-    <row r="23" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="18"/>
@@ -1742,7 +1753,7 @@
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
     </row>
-    <row r="24" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="18"/>
@@ -1766,7 +1777,7 @@
       <c r="AH24" s="4"/>
       <c r="AI24" s="4"/>
     </row>
-    <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="29"/>
       <c r="B25" s="67"/>
       <c r="C25" s="18"/>
@@ -1790,7 +1801,7 @@
       <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
     </row>
-    <row r="26" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -1814,7 +1825,7 @@
       <c r="AH26" s="4"/>
       <c r="AI26" s="4"/>
     </row>
-    <row r="27" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1838,7 +1849,7 @@
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
     </row>
-    <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -1862,7 +1873,7 @@
       <c r="AH28" s="4"/>
       <c r="AI28" s="4"/>
     </row>
-    <row r="29" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -1886,24 +1897,24 @@
       <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
     </row>
-    <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="68"/>
+    <row r="30" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -1924,24 +1935,24 @@
       <c r="AH30" s="4"/>
       <c r="AI30" s="4"/>
     </row>
-    <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
+    <row r="31" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
@@ -1962,15 +1973,15 @@
       <c r="AH31" s="4"/>
       <c r="AI31" s="4"/>
     </row>
-    <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -1992,7 +2003,7 @@
       <c r="AH32" s="4"/>
       <c r="AI32" s="4"/>
     </row>
-    <row r="33" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="64">
         <v>2004</v>
       </c>
@@ -2022,7 +2033,7 @@
       <c r="AH33" s="4"/>
       <c r="AI33" s="4"/>
     </row>
-    <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="64">
         <v>2005</v>
       </c>
@@ -2053,7 +2064,7 @@
       <c r="AH34" s="4"/>
       <c r="AI34" s="4"/>
     </row>
-    <row r="35" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="64">
         <v>2006</v>
       </c>
@@ -2084,7 +2095,7 @@
       <c r="AH35" s="4"/>
       <c r="AI35" s="4"/>
     </row>
-    <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="64">
         <v>2007</v>
       </c>
@@ -2115,7 +2126,7 @@
       <c r="AH36" s="4"/>
       <c r="AI36" s="4"/>
     </row>
-    <row r="37" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="64">
         <v>2008</v>
       </c>
@@ -2146,7 +2157,7 @@
       <c r="AH37" s="4"/>
       <c r="AI37" s="4"/>
     </row>
-    <row r="38" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="64">
         <v>2009</v>
       </c>
@@ -2177,7 +2188,7 @@
       <c r="AH38" s="4"/>
       <c r="AI38" s="4"/>
     </row>
-    <row r="39" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="64">
         <v>2010</v>
       </c>
@@ -2208,7 +2219,7 @@
       <c r="AH39" s="4"/>
       <c r="AI39" s="4"/>
     </row>
-    <row r="40" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="64">
         <v>2011</v>
       </c>
@@ -2239,7 +2250,7 @@
       <c r="AH40" s="4"/>
       <c r="AI40" s="4"/>
     </row>
-    <row r="41" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="64">
         <v>2017</v>
       </c>
@@ -2270,7 +2281,7 @@
       <c r="AH41" s="4"/>
       <c r="AI41" s="4"/>
     </row>
-    <row r="42" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="63"/>
       <c r="B42" s="63"/>
       <c r="C42" s="63"/>
@@ -2294,7 +2305,7 @@
       <c r="AH42" s="4"/>
       <c r="AI42" s="4"/>
     </row>
-    <row r="43" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="63"/>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -2318,7 +2329,7 @@
       <c r="AH43" s="4"/>
       <c r="AI43" s="4"/>
     </row>
-    <row r="44" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="63"/>
       <c r="B44" s="63"/>
       <c r="C44" s="63"/>
@@ -2342,7 +2353,7 @@
       <c r="AH44" s="4"/>
       <c r="AI44" s="4"/>
     </row>
-    <row r="45" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="63"/>
       <c r="B45" s="63"/>
       <c r="C45" s="63"/>
@@ -2366,7 +2377,7 @@
       <c r="AH45" s="4"/>
       <c r="AI45" s="4"/>
     </row>
-    <row r="46" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="63"/>
       <c r="B46" s="63"/>
       <c r="C46" s="63"/>
@@ -2390,7 +2401,7 @@
       <c r="AH46" s="4"/>
       <c r="AI46" s="4"/>
     </row>
-    <row r="47" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
@@ -2411,7 +2422,7 @@
       <c r="AH47" s="4"/>
       <c r="AI47" s="4"/>
     </row>
-    <row r="48" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
@@ -2432,7 +2443,7 @@
       <c r="AH48" s="4"/>
       <c r="AI48" s="4"/>
     </row>
-    <row r="49" spans="17:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="17:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
@@ -2453,7 +2464,7 @@
       <c r="AH49" s="4"/>
       <c r="AI49" s="4"/>
     </row>
-    <row r="50" spans="17:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="17:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
@@ -2474,7 +2485,7 @@
       <c r="AH50" s="4"/>
       <c r="AI50" s="4"/>
     </row>
-    <row r="51" spans="17:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="17:35" x14ac:dyDescent="0.35">
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
@@ -2511,56 +2522,56 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AX187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="4" width="29.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.1796875" customWidth="1"/>
+    <col min="2" max="4" width="29.7265625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" customWidth="1"/>
     <col min="14" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.140625" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" customWidth="1"/>
-    <col min="32" max="33" width="12.5703125" customWidth="1"/>
-    <col min="34" max="34" width="13.85546875" customWidth="1"/>
-    <col min="40" max="40" width="14.42578125" customWidth="1"/>
-    <col min="41" max="41" width="14.5703125" customWidth="1"/>
-    <col min="42" max="42" width="18.140625" customWidth="1"/>
-    <col min="44" max="44" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.140625" customWidth="1"/>
-    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.140625" customWidth="1"/>
-    <col min="53" max="53" width="13.140625" customWidth="1"/>
-    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.1796875" customWidth="1"/>
+    <col min="31" max="31" width="14.81640625" customWidth="1"/>
+    <col min="32" max="33" width="12.54296875" customWidth="1"/>
+    <col min="34" max="34" width="13.81640625" customWidth="1"/>
+    <col min="40" max="40" width="14.453125" customWidth="1"/>
+    <col min="41" max="41" width="14.54296875" customWidth="1"/>
+    <col min="42" max="42" width="18.1796875" customWidth="1"/>
+    <col min="44" max="44" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.1796875" customWidth="1"/>
+    <col min="51" max="51" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.1796875" customWidth="1"/>
+    <col min="53" max="53" width="13.1796875" customWidth="1"/>
+    <col min="55" max="55" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="18" customWidth="1"/>
-    <col min="57" max="57" width="13.42578125" customWidth="1"/>
-    <col min="58" max="58" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.42578125" customWidth="1"/>
-    <col min="60" max="60" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.453125" customWidth="1"/>
+    <col min="58" max="58" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.453125" customWidth="1"/>
+    <col min="60" max="60" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="15" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -2580,12 +2591,12 @@
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2604,12 +2615,12 @@
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="44">
         <v>2005</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2628,12 +2639,12 @@
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
     </row>
-    <row r="4" spans="1:38" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" s="14" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2652,7 +2663,7 @@
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
     </row>
-    <row r="5" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>15</v>
       </c>
@@ -2667,9 +2678,9 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="12">
         <v>0.34</v>
@@ -2682,7 +2693,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2005</v>
       </c>
@@ -2697,9 +2708,9 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="42">
         <v>7.0999999999999994E-2</v>
@@ -2712,7 +2723,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -2723,7 +2734,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2734,7 +2745,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -2745,7 +2756,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -2756,7 +2767,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -2767,9 +2778,9 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -2799,12 +2810,12 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15" spans="1:38" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -2833,24 +2844,24 @@
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:38" s="14" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" s="14" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
+        <v>49</v>
+      </c>
+      <c r="B16" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
@@ -2867,12 +2878,12 @@
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
     </row>
-    <row r="17" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -2901,9 +2912,9 @@
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18" spans="1:38" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -2925,7 +2936,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>14</v>
       </c>
@@ -2961,7 +2972,7 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="1:38" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2997,7 +3008,7 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
     </row>
-    <row r="21" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -3033,7 +3044,7 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
     </row>
-    <row r="22" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -3069,7 +3080,7 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
     </row>
-    <row r="23" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3116,7 @@
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
     </row>
-    <row r="24" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -3141,7 +3152,7 @@
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
     </row>
-    <row r="25" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -3177,7 +3188,7 @@
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
     </row>
-    <row r="26" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3213,7 +3224,7 @@
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3249,7 +3260,7 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
     </row>
-    <row r="28" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3285,7 +3296,7 @@
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
     </row>
-    <row r="29" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3321,7 +3332,7 @@
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
     </row>
-    <row r="30" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3361,7 +3372,7 @@
       <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
     </row>
-    <row r="31" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -3401,7 +3412,7 @@
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
     </row>
-    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="35" t="s">
         <v>36</v>
       </c>
@@ -3441,7 +3452,7 @@
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="35" t="s">
         <v>37</v>
       </c>
@@ -3481,7 +3492,7 @@
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
     </row>
-    <row r="34" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
         <v>38</v>
       </c>
@@ -3521,7 +3532,7 @@
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
     </row>
-    <row r="35" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="35" t="s">
         <v>39</v>
       </c>
@@ -3561,7 +3572,7 @@
       <c r="AK35" s="4"/>
       <c r="AL35" s="4"/>
     </row>
-    <row r="36" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -3573,7 +3584,7 @@
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -3585,7 +3596,7 @@
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
     </row>
-    <row r="38" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -3597,7 +3608,7 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:50" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -3616,7 +3627,7 @@
       <c r="P39" s="18"/>
       <c r="Q39" s="18"/>
     </row>
-    <row r="40" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -3635,9 +3646,9 @@
       <c r="P40" s="18"/>
       <c r="Q40" s="18"/>
     </row>
-    <row r="41" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
@@ -3657,50 +3668,50 @@
       <c r="Q41" s="23"/>
       <c r="R41" s="13"/>
     </row>
-    <row r="42" spans="1:50" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="80"/>
-      <c r="H42" s="80"/>
-      <c r="I42" s="80"/>
-      <c r="J42" s="80"/>
-      <c r="K42" s="80"/>
-      <c r="L42" s="80"/>
-      <c r="M42" s="80"/>
+    <row r="42" spans="1:50" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="82"/>
+      <c r="J42" s="82"/>
+      <c r="K42" s="82"/>
+      <c r="L42" s="82"/>
+      <c r="M42" s="82"/>
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
     </row>
-    <row r="43" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="25"/>
       <c r="B43" s="52"/>
-      <c r="C43" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="72"/>
+      <c r="C43" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="77"/>
       <c r="G43" s="49"/>
       <c r="H43" s="25"/>
       <c r="I43" s="55"/>
-      <c r="J43" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="72"/>
+      <c r="J43" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="77"/>
       <c r="O43" s="25"/>
     </row>
-    <row r="44" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="36" t="s">
         <v>30</v>
       </c>
@@ -3746,8 +3757,8 @@
       </c>
       <c r="AX44" s="16"/>
     </row>
-    <row r="45" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="75" t="s">
+    <row r="45" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3770,7 +3781,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G45" s="19"/>
-      <c r="H45" s="76" t="s">
+      <c r="H45" s="73" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -3797,8 +3808,8 @@
       </c>
       <c r="AX45" s="15"/>
     </row>
-    <row r="46" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="75"/>
+    <row r="46" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="72"/>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3819,7 +3830,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G46" s="19"/>
-      <c r="H46" s="77"/>
+      <c r="H46" s="74"/>
       <c r="I46" s="2" t="s">
         <v>3</v>
       </c>
@@ -3844,8 +3855,8 @@
       </c>
       <c r="AX46" s="9"/>
     </row>
-    <row r="47" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="75"/>
+    <row r="47" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="72"/>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3866,7 +3877,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G47" s="19"/>
-      <c r="H47" s="77"/>
+      <c r="H47" s="74"/>
       <c r="I47" s="2" t="s">
         <v>4</v>
       </c>
@@ -3891,8 +3902,8 @@
       </c>
       <c r="AX47" s="9"/>
     </row>
-    <row r="48" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="75"/>
+    <row r="48" spans="1:50" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="72"/>
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3913,7 +3924,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G48" s="19"/>
-      <c r="H48" s="77"/>
+      <c r="H48" s="74"/>
       <c r="I48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3938,8 +3949,8 @@
       </c>
       <c r="AX48" s="9"/>
     </row>
-    <row r="49" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="75"/>
+    <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="72"/>
       <c r="B49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3960,7 +3971,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G49" s="19"/>
-      <c r="H49" s="77"/>
+      <c r="H49" s="74"/>
       <c r="I49" s="2" t="s">
         <v>6</v>
       </c>
@@ -3984,8 +3995,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="75"/>
+    <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="72"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4006,7 +4017,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G50" s="19"/>
-      <c r="H50" s="77"/>
+      <c r="H50" s="74"/>
       <c r="I50" s="2" t="s">
         <v>7</v>
       </c>
@@ -4030,8 +4041,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="75"/>
+    <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="72"/>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4052,7 +4063,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G51" s="19"/>
-      <c r="H51" s="77"/>
+      <c r="H51" s="74"/>
       <c r="I51" s="2" t="s">
         <v>13</v>
       </c>
@@ -4076,8 +4087,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="75"/>
+    <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="72"/>
       <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4098,7 +4109,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G52" s="19"/>
-      <c r="H52" s="77"/>
+      <c r="H52" s="74"/>
       <c r="I52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4122,8 +4133,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="75"/>
+    <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="72"/>
       <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4144,7 +4155,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G53" s="19"/>
-      <c r="H53" s="77"/>
+      <c r="H53" s="74"/>
       <c r="I53" s="2" t="s">
         <v>9</v>
       </c>
@@ -4168,8 +4179,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="75"/>
+    <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="72"/>
       <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4190,7 +4201,7 @@
         <v>0.21413276231263384</v>
       </c>
       <c r="G54" s="19"/>
-      <c r="H54" s="77"/>
+      <c r="H54" s="74"/>
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
@@ -4214,8 +4225,8 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="75"/>
+    <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="72"/>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4236,7 +4247,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G55" s="19"/>
-      <c r="H55" s="77"/>
+      <c r="H55" s="74"/>
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
@@ -4260,8 +4271,8 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="75"/>
+    <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="72"/>
       <c r="B56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4282,7 +4293,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G56" s="19"/>
-      <c r="H56" s="77"/>
+      <c r="H56" s="74"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4306,8 +4317,8 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="75"/>
+    <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="72"/>
       <c r="B57" s="35" t="s">
         <v>36</v>
       </c>
@@ -4328,7 +4339,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G57" s="19"/>
-      <c r="H57" s="77"/>
+      <c r="H57" s="74"/>
       <c r="I57" s="35" t="s">
         <v>36</v>
       </c>
@@ -4352,8 +4363,8 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="75"/>
+    <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="72"/>
       <c r="B58" s="35" t="s">
         <v>37</v>
       </c>
@@ -4374,7 +4385,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G58" s="19"/>
-      <c r="H58" s="77"/>
+      <c r="H58" s="74"/>
       <c r="I58" s="35" t="s">
         <v>37</v>
       </c>
@@ -4398,8 +4409,8 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="75"/>
+    <row r="59" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="72"/>
       <c r="B59" s="35" t="s">
         <v>38</v>
       </c>
@@ -4420,7 +4431,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G59" s="19"/>
-      <c r="H59" s="77"/>
+      <c r="H59" s="74"/>
       <c r="I59" s="35" t="s">
         <v>38</v>
       </c>
@@ -4444,8 +4455,8 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="75"/>
+    <row r="60" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="72"/>
       <c r="B60" s="35" t="s">
         <v>39</v>
       </c>
@@ -4466,7 +4477,7 @@
         <v>0.22172949002217296</v>
       </c>
       <c r="G60" s="19"/>
-      <c r="H60" s="78"/>
+      <c r="H60" s="75"/>
       <c r="I60" s="35" t="s">
         <v>39</v>
       </c>
@@ -4490,7 +4501,7 @@
         <v>9.7099999999999991</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="18"/>
       <c r="B61" s="51"/>
       <c r="C61" s="18"/>
@@ -4507,8 +4518,8 @@
       <c r="N61" s="18"/>
       <c r="O61" s="18"/>
     </row>
-    <row r="62" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="76" t="s">
+    <row r="62" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="73" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -4531,7 +4542,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G62" s="19"/>
-      <c r="H62" s="76" t="s">
+      <c r="H62" s="73" t="s">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -4557,8 +4568,8 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="77"/>
+    <row r="63" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="74"/>
       <c r="B63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4579,7 +4590,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G63" s="19"/>
-      <c r="H63" s="77"/>
+      <c r="H63" s="74"/>
       <c r="I63" s="2" t="s">
         <v>3</v>
       </c>
@@ -4603,8 +4614,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="77"/>
+    <row r="64" spans="1:15" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="74"/>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4625,7 +4636,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G64" s="19"/>
-      <c r="H64" s="77"/>
+      <c r="H64" s="74"/>
       <c r="I64" s="2" t="s">
         <v>4</v>
       </c>
@@ -4649,8 +4660,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="77"/>
+    <row r="65" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="74"/>
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4671,7 +4682,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G65" s="19"/>
-      <c r="H65" s="77"/>
+      <c r="H65" s="74"/>
       <c r="I65" s="2" t="s">
         <v>5</v>
       </c>
@@ -4695,8 +4706,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="77"/>
+    <row r="66" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="74"/>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4717,7 +4728,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G66" s="19"/>
-      <c r="H66" s="77"/>
+      <c r="H66" s="74"/>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4741,8 +4752,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="77"/>
+    <row r="67" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="74"/>
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4763,7 +4774,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G67" s="19"/>
-      <c r="H67" s="77"/>
+      <c r="H67" s="74"/>
       <c r="I67" s="2" t="s">
         <v>7</v>
       </c>
@@ -4787,8 +4798,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="77"/>
+    <row r="68" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="74"/>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4809,7 +4820,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G68" s="19"/>
-      <c r="H68" s="77"/>
+      <c r="H68" s="74"/>
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
@@ -4833,8 +4844,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="77"/>
+    <row r="69" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="74"/>
       <c r="B69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4855,7 +4866,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G69" s="19"/>
-      <c r="H69" s="77"/>
+      <c r="H69" s="74"/>
       <c r="I69" s="2" t="s">
         <v>8</v>
       </c>
@@ -4879,8 +4890,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="77"/>
+    <row r="70" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="74"/>
       <c r="B70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4901,7 +4912,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G70" s="19"/>
-      <c r="H70" s="77"/>
+      <c r="H70" s="74"/>
       <c r="I70" s="2" t="s">
         <v>9</v>
       </c>
@@ -4925,8 +4936,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="77"/>
+    <row r="71" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="74"/>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4947,7 +4958,7 @@
         <v>0.21367521367521369</v>
       </c>
       <c r="G71" s="19"/>
-      <c r="H71" s="77"/>
+      <c r="H71" s="74"/>
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
@@ -4971,8 +4982,8 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="77"/>
+    <row r="72" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="74"/>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
@@ -4993,7 +5004,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G72" s="19"/>
-      <c r="H72" s="77"/>
+      <c r="H72" s="74"/>
       <c r="I72" s="2" t="s">
         <v>11</v>
       </c>
@@ -5017,8 +5028,8 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="77"/>
+    <row r="73" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="74"/>
       <c r="B73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5039,7 +5050,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G73" s="19"/>
-      <c r="H73" s="77"/>
+      <c r="H73" s="74"/>
       <c r="I73" s="2" t="s">
         <v>12</v>
       </c>
@@ -5063,8 +5074,8 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="77"/>
+    <row r="74" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="74"/>
       <c r="B74" s="35" t="s">
         <v>36</v>
       </c>
@@ -5085,7 +5096,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G74" s="19"/>
-      <c r="H74" s="77"/>
+      <c r="H74" s="74"/>
       <c r="I74" s="35" t="s">
         <v>36</v>
       </c>
@@ -5109,8 +5120,8 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="77"/>
+    <row r="75" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="74"/>
       <c r="B75" s="35" t="s">
         <v>37</v>
       </c>
@@ -5131,7 +5142,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G75" s="19"/>
-      <c r="H75" s="77"/>
+      <c r="H75" s="74"/>
       <c r="I75" s="35" t="s">
         <v>37</v>
       </c>
@@ -5155,8 +5166,8 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="77"/>
+    <row r="76" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="74"/>
       <c r="B76" s="35" t="s">
         <v>38</v>
       </c>
@@ -5177,7 +5188,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G76" s="19"/>
-      <c r="H76" s="77"/>
+      <c r="H76" s="74"/>
       <c r="I76" s="35" t="s">
         <v>38</v>
       </c>
@@ -5201,8 +5212,8 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="78"/>
+    <row r="77" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="75"/>
       <c r="B77" s="35" t="s">
         <v>39</v>
       </c>
@@ -5223,7 +5234,7 @@
         <v>0.23640661938534277</v>
       </c>
       <c r="G77" s="19"/>
-      <c r="H77" s="78"/>
+      <c r="H77" s="75"/>
       <c r="I77" s="35" t="s">
         <v>39</v>
       </c>
@@ -5247,7 +5258,7 @@
         <v>9.9599999999999991</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="18"/>
       <c r="B78" s="18"/>
       <c r="C78" s="18"/>
@@ -5266,7 +5277,7 @@
       <c r="P78" s="18"/>
       <c r="Q78" s="18"/>
     </row>
-    <row r="79" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="18"/>
       <c r="B79" s="18"/>
       <c r="C79" s="18"/>
@@ -5285,9 +5296,9 @@
       <c r="P79" s="18"/>
       <c r="Q79" s="18"/>
     </row>
-    <row r="80" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="23"/>
@@ -5308,54 +5319,54 @@
       <c r="R80" s="13"/>
       <c r="AB80" s="14"/>
     </row>
-    <row r="81" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" s="82"/>
-      <c r="C81" s="82"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="82"/>
-      <c r="F81" s="82"/>
-      <c r="G81" s="82"/>
-      <c r="H81" s="82"/>
-      <c r="I81" s="82"/>
-      <c r="J81" s="82"/>
-      <c r="K81" s="82"/>
-      <c r="L81" s="82"/>
-      <c r="M81" s="82"/>
-      <c r="N81" s="81"/>
+    <row r="81" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="79"/>
+      <c r="C81" s="79"/>
+      <c r="D81" s="79"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="79"/>
+      <c r="H81" s="79"/>
+      <c r="I81" s="79"/>
+      <c r="J81" s="79"/>
+      <c r="K81" s="79"/>
+      <c r="L81" s="79"/>
+      <c r="M81" s="79"/>
+      <c r="N81" s="68"/>
       <c r="O81" s="23"/>
       <c r="P81" s="23"/>
       <c r="Q81" s="23"/>
       <c r="R81" s="13"/>
       <c r="AB81" s="14"/>
     </row>
-    <row r="82" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="36"/>
       <c r="B82" s="36"/>
-      <c r="C82" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="79"/>
+      <c r="C82" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="D82" s="78"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="78"/>
       <c r="G82" s="19"/>
       <c r="H82" s="25"/>
       <c r="I82" s="55"/>
-      <c r="J82" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="K82" s="71"/>
-      <c r="L82" s="71"/>
-      <c r="M82" s="71"/>
-      <c r="N82" s="72"/>
+      <c r="J82" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="K82" s="76"/>
+      <c r="L82" s="76"/>
+      <c r="M82" s="76"/>
+      <c r="N82" s="77"/>
       <c r="O82" s="25"/>
       <c r="P82" s="18"/>
       <c r="Q82" s="18"/>
       <c r="AB82" s="14"/>
     </row>
-    <row r="83" spans="1:28" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="56" t="s">
         <v>30</v>
       </c>
@@ -5366,13 +5377,13 @@
         <v>17</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="F83" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="G83" s="47"/>
       <c r="H83" s="56" t="s">
@@ -5385,16 +5396,16 @@
         <v>17</v>
       </c>
       <c r="K83" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L83" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L83" s="5" t="s">
+      <c r="M83" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="M83" s="5" t="s">
+      <c r="N83" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="N83" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="O83" s="53" t="s">
         <v>31</v>
@@ -5403,8 +5414,8 @@
       <c r="Q83" s="18"/>
       <c r="AB83" s="14"/>
     </row>
-    <row r="84" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="75" t="s">
+    <row r="84" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5427,7 +5438,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G84" s="47"/>
-      <c r="H84" s="76" t="s">
+      <c r="H84" s="73" t="s">
         <v>0</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5455,8 +5466,8 @@
       <c r="Q84" s="18"/>
       <c r="AB84" s="14"/>
     </row>
-    <row r="85" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="75"/>
+    <row r="85" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="72"/>
       <c r="B85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5477,7 +5488,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G85" s="47"/>
-      <c r="H85" s="77"/>
+      <c r="H85" s="74"/>
       <c r="I85" s="2" t="s">
         <v>3</v>
       </c>
@@ -5503,8 +5514,8 @@
       <c r="Q85" s="47"/>
       <c r="AB85" s="14"/>
     </row>
-    <row r="86" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="75"/>
+    <row r="86" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="72"/>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5525,7 +5536,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G86" s="47"/>
-      <c r="H86" s="77"/>
+      <c r="H86" s="74"/>
       <c r="I86" s="2" t="s">
         <v>4</v>
       </c>
@@ -5551,8 +5562,8 @@
       <c r="Q86" s="19"/>
       <c r="AB86" s="14"/>
     </row>
-    <row r="87" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="75"/>
+    <row r="87" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="72"/>
       <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5573,7 +5584,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G87" s="19"/>
-      <c r="H87" s="77"/>
+      <c r="H87" s="74"/>
       <c r="I87" s="2" t="s">
         <v>5</v>
       </c>
@@ -5599,8 +5610,8 @@
       <c r="Q87" s="19"/>
       <c r="AB87" s="14"/>
     </row>
-    <row r="88" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="75"/>
+    <row r="88" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="72"/>
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5621,7 +5632,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G88" s="47"/>
-      <c r="H88" s="77"/>
+      <c r="H88" s="74"/>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
@@ -5647,8 +5658,8 @@
       <c r="Q88" s="19"/>
       <c r="AB88" s="14"/>
     </row>
-    <row r="89" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="75"/>
+    <row r="89" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="72"/>
       <c r="B89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5669,7 +5680,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G89" s="19"/>
-      <c r="H89" s="77"/>
+      <c r="H89" s="74"/>
       <c r="I89" s="2" t="s">
         <v>7</v>
       </c>
@@ -5696,8 +5707,8 @@
       <c r="Q89" s="19"/>
       <c r="AB89" s="14"/>
     </row>
-    <row r="90" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="75"/>
+    <row r="90" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="72"/>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5718,7 +5729,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G90" s="47"/>
-      <c r="H90" s="77"/>
+      <c r="H90" s="74"/>
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5743,8 +5754,8 @@
       </c>
       <c r="AB90" s="14"/>
     </row>
-    <row r="91" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="75"/>
+    <row r="91" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A91" s="72"/>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5765,7 +5776,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G91" s="47"/>
-      <c r="H91" s="77"/>
+      <c r="H91" s="74"/>
       <c r="I91" s="2" t="s">
         <v>8</v>
       </c>
@@ -5790,8 +5801,8 @@
       </c>
       <c r="AB91" s="14"/>
     </row>
-    <row r="92" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="75"/>
+    <row r="92" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="72"/>
       <c r="B92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5812,7 +5823,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G92" s="47"/>
-      <c r="H92" s="77"/>
+      <c r="H92" s="74"/>
       <c r="I92" s="2" t="s">
         <v>9</v>
       </c>
@@ -5837,8 +5848,8 @@
       </c>
       <c r="AB92" s="14"/>
     </row>
-    <row r="93" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="75"/>
+    <row r="93" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="72"/>
       <c r="B93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5859,7 +5870,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G93" s="47"/>
-      <c r="H93" s="77"/>
+      <c r="H93" s="74"/>
       <c r="I93" s="2" t="s">
         <v>10</v>
       </c>
@@ -5884,8 +5895,8 @@
       </c>
       <c r="AB93" s="14"/>
     </row>
-    <row r="94" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="75"/>
+    <row r="94" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="72"/>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5906,7 +5917,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G94" s="19"/>
-      <c r="H94" s="77"/>
+      <c r="H94" s="74"/>
       <c r="I94" s="2" t="s">
         <v>11</v>
       </c>
@@ -5931,8 +5942,8 @@
       </c>
       <c r="AB94" s="14"/>
     </row>
-    <row r="95" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="75"/>
+    <row r="95" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="72"/>
       <c r="B95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5953,7 +5964,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G95" s="19"/>
-      <c r="H95" s="77"/>
+      <c r="H95" s="74"/>
       <c r="I95" s="2" t="s">
         <v>12</v>
       </c>
@@ -5980,8 +5991,8 @@
       <c r="Q95" s="18"/>
       <c r="AB95" s="14"/>
     </row>
-    <row r="96" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="75"/>
+    <row r="96" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="72"/>
       <c r="B96" s="35" t="s">
         <v>36</v>
       </c>
@@ -6002,7 +6013,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G96" s="19"/>
-      <c r="H96" s="77"/>
+      <c r="H96" s="74"/>
       <c r="I96" s="35" t="s">
         <v>36</v>
       </c>
@@ -6029,8 +6040,8 @@
       <c r="Q96" s="18"/>
       <c r="AB96" s="14"/>
     </row>
-    <row r="97" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="75"/>
+    <row r="97" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="72"/>
       <c r="B97" s="35" t="s">
         <v>37</v>
       </c>
@@ -6051,7 +6062,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G97" s="18"/>
-      <c r="H97" s="77"/>
+      <c r="H97" s="74"/>
       <c r="I97" s="35" t="s">
         <v>37</v>
       </c>
@@ -6078,8 +6089,8 @@
       <c r="Q97" s="18"/>
       <c r="AB97" s="14"/>
     </row>
-    <row r="98" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="75"/>
+    <row r="98" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="72"/>
       <c r="B98" s="35" t="s">
         <v>38</v>
       </c>
@@ -6100,7 +6111,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G98" s="18"/>
-      <c r="H98" s="77"/>
+      <c r="H98" s="74"/>
       <c r="I98" s="35" t="s">
         <v>38</v>
       </c>
@@ -6126,8 +6137,8 @@
       <c r="P98" s="18"/>
       <c r="Q98" s="18"/>
     </row>
-    <row r="99" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="75"/>
+    <row r="99" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="72"/>
       <c r="B99" s="35" t="s">
         <v>39</v>
       </c>
@@ -6148,7 +6159,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G99" s="18"/>
-      <c r="H99" s="78"/>
+      <c r="H99" s="75"/>
       <c r="I99" s="35" t="s">
         <v>39</v>
       </c>
@@ -6174,7 +6185,7 @@
       <c r="P99" s="18"/>
       <c r="Q99" s="18"/>
     </row>
-    <row r="100" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="18"/>
       <c r="B100" s="51"/>
       <c r="C100" s="18"/>
@@ -6193,8 +6204,8 @@
       <c r="P100" s="18"/>
       <c r="Q100" s="18"/>
     </row>
-    <row r="101" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="76" t="s">
+    <row r="101" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="73" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -6217,7 +6228,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G101" s="18"/>
-      <c r="H101" s="76" t="s">
+      <c r="H101" s="73" t="s">
         <v>1</v>
       </c>
       <c r="I101" s="2" t="s">
@@ -6245,8 +6256,8 @@
       <c r="P101" s="18"/>
       <c r="Q101" s="18"/>
     </row>
-    <row r="102" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="77"/>
+    <row r="102" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="74"/>
       <c r="B102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6267,7 +6278,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G102" s="18"/>
-      <c r="H102" s="77"/>
+      <c r="H102" s="74"/>
       <c r="I102" s="2" t="s">
         <v>3</v>
       </c>
@@ -6293,8 +6304,8 @@
       <c r="P102" s="18"/>
       <c r="Q102" s="18"/>
     </row>
-    <row r="103" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="77"/>
+    <row r="103" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="74"/>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6315,7 +6326,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G103" s="18"/>
-      <c r="H103" s="77"/>
+      <c r="H103" s="74"/>
       <c r="I103" s="2" t="s">
         <v>4</v>
       </c>
@@ -6341,8 +6352,8 @@
       <c r="P103" s="18"/>
       <c r="Q103" s="18"/>
     </row>
-    <row r="104" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="77"/>
+    <row r="104" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="74"/>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6363,7 +6374,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G104" s="18"/>
-      <c r="H104" s="77"/>
+      <c r="H104" s="74"/>
       <c r="I104" s="2" t="s">
         <v>5</v>
       </c>
@@ -6389,8 +6400,8 @@
       <c r="P104" s="18"/>
       <c r="Q104" s="18"/>
     </row>
-    <row r="105" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="77"/>
+    <row r="105" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="74"/>
       <c r="B105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6411,7 +6422,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G105" s="18"/>
-      <c r="H105" s="77"/>
+      <c r="H105" s="74"/>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
@@ -6437,8 +6448,8 @@
       <c r="P105" s="18"/>
       <c r="Q105" s="18"/>
     </row>
-    <row r="106" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="77"/>
+    <row r="106" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="74"/>
       <c r="B106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6459,7 +6470,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G106" s="18"/>
-      <c r="H106" s="77"/>
+      <c r="H106" s="74"/>
       <c r="I106" s="2" t="s">
         <v>7</v>
       </c>
@@ -6485,8 +6496,8 @@
       <c r="P106" s="18"/>
       <c r="Q106" s="18"/>
     </row>
-    <row r="107" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="77"/>
+    <row r="107" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="74"/>
       <c r="B107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6507,7 +6518,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G107" s="18"/>
-      <c r="H107" s="77"/>
+      <c r="H107" s="74"/>
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
@@ -6533,8 +6544,8 @@
       <c r="P107" s="18"/>
       <c r="Q107" s="18"/>
     </row>
-    <row r="108" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="77"/>
+    <row r="108" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="74"/>
       <c r="B108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6555,7 +6566,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G108" s="18"/>
-      <c r="H108" s="77"/>
+      <c r="H108" s="74"/>
       <c r="I108" s="2" t="s">
         <v>8</v>
       </c>
@@ -6581,8 +6592,8 @@
       <c r="P108" s="18"/>
       <c r="Q108" s="18"/>
     </row>
-    <row r="109" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="77"/>
+    <row r="109" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="74"/>
       <c r="B109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6603,7 +6614,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G109" s="18"/>
-      <c r="H109" s="77"/>
+      <c r="H109" s="74"/>
       <c r="I109" s="2" t="s">
         <v>9</v>
       </c>
@@ -6629,8 +6640,8 @@
       <c r="P109" s="18"/>
       <c r="Q109" s="18"/>
     </row>
-    <row r="110" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="77"/>
+    <row r="110" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="74"/>
       <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6651,7 +6662,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G110" s="18"/>
-      <c r="H110" s="77"/>
+      <c r="H110" s="74"/>
       <c r="I110" s="2" t="s">
         <v>10</v>
       </c>
@@ -6677,8 +6688,8 @@
       <c r="P110" s="18"/>
       <c r="Q110" s="18"/>
     </row>
-    <row r="111" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="77"/>
+    <row r="111" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="74"/>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6699,7 +6710,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G111" s="18"/>
-      <c r="H111" s="77"/>
+      <c r="H111" s="74"/>
       <c r="I111" s="2" t="s">
         <v>11</v>
       </c>
@@ -6725,8 +6736,8 @@
       <c r="P111" s="18"/>
       <c r="Q111" s="18"/>
     </row>
-    <row r="112" spans="1:28" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="77"/>
+    <row r="112" spans="1:28" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="74"/>
       <c r="B112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6747,7 +6758,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G112" s="18"/>
-      <c r="H112" s="77"/>
+      <c r="H112" s="74"/>
       <c r="I112" s="2" t="s">
         <v>12</v>
       </c>
@@ -6773,8 +6784,8 @@
       <c r="P112" s="18"/>
       <c r="Q112" s="18"/>
     </row>
-    <row r="113" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="77"/>
+    <row r="113" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="74"/>
       <c r="B113" s="35" t="s">
         <v>36</v>
       </c>
@@ -6795,7 +6806,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G113" s="18"/>
-      <c r="H113" s="77"/>
+      <c r="H113" s="74"/>
       <c r="I113" s="35" t="s">
         <v>36</v>
       </c>
@@ -6821,8 +6832,8 @@
       <c r="P113" s="18"/>
       <c r="Q113" s="18"/>
     </row>
-    <row r="114" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="77"/>
+    <row r="114" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="74"/>
       <c r="B114" s="35" t="s">
         <v>37</v>
       </c>
@@ -6843,7 +6854,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G114" s="18"/>
-      <c r="H114" s="77"/>
+      <c r="H114" s="74"/>
       <c r="I114" s="35" t="s">
         <v>37</v>
       </c>
@@ -6869,8 +6880,8 @@
       <c r="P114" s="18"/>
       <c r="Q114" s="18"/>
     </row>
-    <row r="115" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="77"/>
+    <row r="115" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="74"/>
       <c r="B115" s="35" t="s">
         <v>38</v>
       </c>
@@ -6891,7 +6902,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G115" s="18"/>
-      <c r="H115" s="77"/>
+      <c r="H115" s="74"/>
       <c r="I115" s="35" t="s">
         <v>38</v>
       </c>
@@ -6917,8 +6928,8 @@
       <c r="P115" s="18"/>
       <c r="Q115" s="18"/>
     </row>
-    <row r="116" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="78"/>
+    <row r="116" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="75"/>
       <c r="B116" s="35" t="s">
         <v>39</v>
       </c>
@@ -6939,7 +6950,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G116" s="14"/>
-      <c r="H116" s="78"/>
+      <c r="H116" s="75"/>
       <c r="I116" s="35" t="s">
         <v>39</v>
       </c>
@@ -6965,7 +6976,7 @@
       <c r="P116" s="18"/>
       <c r="Q116" s="18"/>
     </row>
-    <row r="117" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="H117" s="54"/>
       <c r="I117" s="51"/>
       <c r="J117" s="19"/>
@@ -6977,7 +6988,7 @@
       <c r="P117" s="18"/>
       <c r="Q117" s="18"/>
     </row>
-    <row r="118" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
@@ -7002,7 +7013,7 @@
       <c r="V118" s="9"/>
       <c r="W118" s="9"/>
     </row>
-    <row r="119" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -7027,7 +7038,7 @@
       <c r="V119" s="9"/>
       <c r="W119" s="9"/>
     </row>
-    <row r="120" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" s="14" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
@@ -7052,7 +7063,7 @@
       <c r="V120" s="9"/>
       <c r="W120" s="9"/>
     </row>
-    <row r="121" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A121" s="59"/>
       <c r="B121" s="26"/>
       <c r="C121" s="26"/>
@@ -7077,7 +7088,7 @@
       <c r="V121" s="9"/>
       <c r="W121" s="9"/>
     </row>
-    <row r="122" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A122" s="15"/>
       <c r="B122" s="59"/>
       <c r="C122" s="59"/>
@@ -7102,7 +7113,7 @@
       <c r="V122" s="9"/>
       <c r="W122" s="9"/>
     </row>
-    <row r="123" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A123" s="50"/>
       <c r="B123" s="50"/>
       <c r="C123" s="50"/>
@@ -7127,7 +7138,7 @@
       <c r="V123" s="9"/>
       <c r="W123" s="9"/>
     </row>
-    <row r="124" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A124" s="50"/>
       <c r="B124" s="50"/>
       <c r="C124" s="50"/>
@@ -7152,7 +7163,7 @@
       <c r="V124" s="9"/>
       <c r="W124" s="9"/>
     </row>
-    <row r="125" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A125" s="50"/>
       <c r="B125" s="50"/>
       <c r="C125" s="50"/>
@@ -7177,7 +7188,7 @@
       <c r="V125" s="9"/>
       <c r="W125" s="9"/>
     </row>
-    <row r="126" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A126" s="50"/>
       <c r="B126" s="50"/>
       <c r="C126" s="50"/>
@@ -7202,7 +7213,7 @@
       <c r="V126" s="9"/>
       <c r="W126" s="9"/>
     </row>
-    <row r="127" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A127" s="50"/>
       <c r="B127" s="50"/>
       <c r="C127" s="50"/>
@@ -7227,7 +7238,7 @@
       <c r="V127" s="9"/>
       <c r="W127" s="9"/>
     </row>
-    <row r="128" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A128" s="50"/>
       <c r="B128" s="50"/>
       <c r="C128" s="50"/>
@@ -7252,7 +7263,7 @@
       <c r="V128" s="9"/>
       <c r="W128" s="9"/>
     </row>
-    <row r="129" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A129" s="50"/>
       <c r="B129" s="50"/>
       <c r="C129" s="50"/>
@@ -7277,7 +7288,7 @@
       <c r="V129" s="9"/>
       <c r="W129" s="9"/>
     </row>
-    <row r="130" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A130" s="50"/>
       <c r="B130" s="50"/>
       <c r="C130" s="50"/>
@@ -7302,7 +7313,7 @@
       <c r="V130" s="9"/>
       <c r="W130" s="9"/>
     </row>
-    <row r="131" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A131" s="50"/>
       <c r="B131" s="50"/>
       <c r="C131" s="50"/>
@@ -7327,7 +7338,7 @@
       <c r="V131" s="9"/>
       <c r="W131" s="9"/>
     </row>
-    <row r="132" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A132" s="50"/>
       <c r="B132" s="50"/>
       <c r="C132" s="50"/>
@@ -7352,7 +7363,7 @@
       <c r="V132" s="9"/>
       <c r="W132" s="9"/>
     </row>
-    <row r="133" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A133" s="50"/>
       <c r="B133" s="50"/>
       <c r="C133" s="50"/>
@@ -7377,7 +7388,7 @@
       <c r="V133" s="9"/>
       <c r="W133" s="9"/>
     </row>
-    <row r="134" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A134" s="50"/>
       <c r="B134" s="50"/>
       <c r="C134" s="50"/>
@@ -7402,7 +7413,7 @@
       <c r="V134" s="9"/>
       <c r="W134" s="9"/>
     </row>
-    <row r="135" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A135" s="62"/>
       <c r="B135" s="50"/>
       <c r="C135" s="50"/>
@@ -7427,7 +7438,7 @@
       <c r="V135" s="9"/>
       <c r="W135" s="9"/>
     </row>
-    <row r="136" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A136" s="62"/>
       <c r="B136" s="50"/>
       <c r="C136" s="50"/>
@@ -7452,7 +7463,7 @@
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
     </row>
-    <row r="137" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A137" s="62"/>
       <c r="B137" s="50"/>
       <c r="C137" s="50"/>
@@ -7477,7 +7488,7 @@
       <c r="V137" s="9"/>
       <c r="W137" s="9"/>
     </row>
-    <row r="138" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A138" s="62"/>
       <c r="B138" s="50"/>
       <c r="C138" s="50"/>
@@ -7502,7 +7513,7 @@
       <c r="V138" s="9"/>
       <c r="W138" s="9"/>
     </row>
-    <row r="139" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A139" s="26"/>
       <c r="B139" s="26"/>
       <c r="C139" s="26"/>
@@ -7527,7 +7538,7 @@
       <c r="V139" s="9"/>
       <c r="W139" s="9"/>
     </row>
-    <row r="140" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A140" s="26"/>
       <c r="B140" s="26"/>
       <c r="C140" s="26"/>
@@ -7552,7 +7563,7 @@
       <c r="V140" s="9"/>
       <c r="W140" s="9"/>
     </row>
-    <row r="141" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A141" s="26"/>
       <c r="B141" s="26"/>
       <c r="C141" s="26"/>
@@ -7577,7 +7588,7 @@
       <c r="V141" s="9"/>
       <c r="W141" s="9"/>
     </row>
-    <row r="142" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A142" s="26"/>
       <c r="B142" s="26"/>
       <c r="C142" s="26"/>
@@ -7602,7 +7613,7 @@
       <c r="V142" s="9"/>
       <c r="W142" s="9"/>
     </row>
-    <row r="143" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A143" s="26"/>
       <c r="B143" s="26"/>
       <c r="C143" s="26"/>
@@ -7627,7 +7638,7 @@
       <c r="V143" s="9"/>
       <c r="W143" s="9"/>
     </row>
-    <row r="144" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A144" s="57"/>
       <c r="B144" s="26"/>
       <c r="C144" s="26"/>
@@ -7652,7 +7663,7 @@
       <c r="V144" s="9"/>
       <c r="W144" s="9"/>
     </row>
-    <row r="145" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A145" s="58"/>
       <c r="B145" s="26"/>
       <c r="C145" s="26"/>
@@ -7677,9 +7688,9 @@
       <c r="V145" s="9"/>
       <c r="W145" s="9"/>
     </row>
-    <row r="146" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="74"/>
-      <c r="B146" s="74"/>
+    <row r="146" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="71"/>
+      <c r="B146" s="71"/>
       <c r="C146" s="26"/>
       <c r="D146" s="26"/>
       <c r="E146" s="26"/>
@@ -7702,7 +7713,7 @@
       <c r="V146" s="9"/>
       <c r="W146" s="9"/>
     </row>
-    <row r="147" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A147" s="26"/>
       <c r="B147" s="26"/>
       <c r="C147" s="26"/>
@@ -7727,7 +7738,7 @@
       <c r="V147" s="9"/>
       <c r="W147" s="9"/>
     </row>
-    <row r="148" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A148" s="26"/>
       <c r="B148" s="26"/>
       <c r="C148" s="26"/>
@@ -7752,7 +7763,7 @@
       <c r="V148" s="9"/>
       <c r="W148" s="9"/>
     </row>
-    <row r="149" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A149" s="26"/>
       <c r="B149" s="26"/>
       <c r="C149" s="26"/>
@@ -7777,7 +7788,7 @@
       <c r="V149" s="9"/>
       <c r="W149" s="9"/>
     </row>
-    <row r="150" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A150" s="26"/>
       <c r="B150" s="26"/>
       <c r="C150" s="26"/>
@@ -7802,9 +7813,9 @@
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
     </row>
-    <row r="151" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="74"/>
-      <c r="B151" s="74"/>
+    <row r="151" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A151" s="71"/>
+      <c r="B151" s="71"/>
       <c r="C151" s="26"/>
       <c r="D151" s="26"/>
       <c r="E151" s="26"/>
@@ -7827,7 +7838,7 @@
       <c r="V151" s="9"/>
       <c r="W151" s="9"/>
     </row>
-    <row r="152" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A152" s="26"/>
       <c r="B152" s="26"/>
       <c r="C152" s="26"/>
@@ -7852,7 +7863,7 @@
       <c r="V152" s="9"/>
       <c r="W152" s="9"/>
     </row>
-    <row r="153" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A153" s="26"/>
       <c r="B153" s="26"/>
       <c r="C153" s="26"/>
@@ -7877,7 +7888,7 @@
       <c r="V153" s="9"/>
       <c r="W153" s="9"/>
     </row>
-    <row r="154" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A154" s="26"/>
       <c r="B154" s="26"/>
       <c r="C154" s="26"/>
@@ -7902,7 +7913,7 @@
       <c r="V154" s="9"/>
       <c r="W154" s="9"/>
     </row>
-    <row r="155" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A155" s="26"/>
       <c r="B155" s="26"/>
       <c r="C155" s="26"/>
@@ -7927,7 +7938,7 @@
       <c r="V155" s="9"/>
       <c r="W155" s="9"/>
     </row>
-    <row r="156" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A156" s="26"/>
       <c r="B156" s="26"/>
       <c r="C156" s="26"/>
@@ -7952,7 +7963,7 @@
       <c r="V156" s="9"/>
       <c r="W156" s="9"/>
     </row>
-    <row r="157" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A157" s="18"/>
       <c r="B157" s="18"/>
       <c r="C157" s="18"/>
@@ -7971,7 +7982,7 @@
       <c r="P157" s="18"/>
       <c r="Q157" s="18"/>
     </row>
-    <row r="158" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A158" s="26"/>
       <c r="B158" s="26"/>
       <c r="C158" s="26"/>
@@ -8008,7 +8019,7 @@
       <c r="AH158" s="9"/>
       <c r="AI158" s="9"/>
     </row>
-    <row r="159" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A159" s="26"/>
       <c r="B159" s="26"/>
       <c r="C159" s="26"/>
@@ -8045,7 +8056,7 @@
       <c r="AH159" s="9"/>
       <c r="AI159" s="9"/>
     </row>
-    <row r="160" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A160" s="57"/>
       <c r="B160" s="26"/>
       <c r="C160" s="26"/>
@@ -8082,7 +8093,7 @@
       <c r="AH160" s="9"/>
       <c r="AI160" s="9"/>
     </row>
-    <row r="161" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A161" s="58"/>
       <c r="B161" s="26"/>
       <c r="C161" s="26"/>
@@ -8119,7 +8130,7 @@
       <c r="AH161" s="9"/>
       <c r="AI161" s="9"/>
     </row>
-    <row r="162" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A162" s="58"/>
       <c r="B162" s="26"/>
       <c r="C162" s="26"/>
@@ -8156,7 +8167,7 @@
       <c r="AH162" s="9"/>
       <c r="AI162" s="9"/>
     </row>
-    <row r="163" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A163" s="26"/>
       <c r="B163" s="57"/>
       <c r="C163" s="57"/>
@@ -8193,7 +8204,7 @@
       <c r="AH163" s="9"/>
       <c r="AI163" s="9"/>
     </row>
-    <row r="164" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A164" s="60"/>
       <c r="B164" s="26"/>
       <c r="C164" s="26"/>
@@ -8230,7 +8241,7 @@
       <c r="AH164" s="9"/>
       <c r="AI164" s="9"/>
     </row>
-    <row r="165" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A165" s="26"/>
       <c r="B165" s="26"/>
       <c r="C165" s="26"/>
@@ -8267,7 +8278,7 @@
       <c r="AH165" s="9"/>
       <c r="AI165" s="9"/>
     </row>
-    <row r="166" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A166" s="59"/>
       <c r="B166" s="59"/>
       <c r="C166" s="59"/>
@@ -8304,7 +8315,7 @@
       <c r="AH166" s="9"/>
       <c r="AI166" s="9"/>
     </row>
-    <row r="167" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A167" s="59"/>
       <c r="B167" s="1"/>
       <c r="C167" s="50"/>
@@ -8341,7 +8352,7 @@
       <c r="AH167" s="9"/>
       <c r="AI167" s="9"/>
     </row>
-    <row r="168" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A168" s="26"/>
       <c r="B168" s="26"/>
       <c r="C168" s="26"/>
@@ -8378,7 +8389,7 @@
       <c r="AH168" s="9"/>
       <c r="AI168" s="9"/>
     </row>
-    <row r="169" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A169" s="9"/>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -8415,7 +8426,7 @@
       <c r="AH169" s="9"/>
       <c r="AI169" s="9"/>
     </row>
-    <row r="170" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A170" s="9"/>
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
@@ -8452,7 +8463,7 @@
       <c r="AH170" s="9"/>
       <c r="AI170" s="9"/>
     </row>
-    <row r="171" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A171" s="26"/>
       <c r="B171" s="26"/>
       <c r="C171" s="26"/>
@@ -8489,7 +8500,7 @@
       <c r="AH171" s="9"/>
       <c r="AI171" s="9"/>
     </row>
-    <row r="172" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A172" s="9"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -8526,7 +8537,7 @@
       <c r="AH172" s="9"/>
       <c r="AI172" s="9"/>
     </row>
-    <row r="173" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A173" s="9"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -8563,7 +8574,7 @@
       <c r="AH173" s="9"/>
       <c r="AI173" s="9"/>
     </row>
-    <row r="174" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A174" s="26"/>
       <c r="B174" s="26"/>
       <c r="C174" s="26"/>
@@ -8600,7 +8611,7 @@
       <c r="AH174" s="9"/>
       <c r="AI174" s="9"/>
     </row>
-    <row r="175" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A175" s="26"/>
       <c r="B175" s="26"/>
       <c r="C175" s="26"/>
@@ -8637,7 +8648,7 @@
       <c r="AH175" s="9"/>
       <c r="AI175" s="9"/>
     </row>
-    <row r="176" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A176" s="26"/>
       <c r="B176" s="26"/>
       <c r="C176" s="26"/>
@@ -8674,7 +8685,7 @@
       <c r="AH176" s="9"/>
       <c r="AI176" s="9"/>
     </row>
-    <row r="177" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A177" s="18"/>
       <c r="B177" s="18"/>
       <c r="C177" s="18"/>
@@ -8693,7 +8704,7 @@
       <c r="P177" s="18"/>
       <c r="Q177" s="18"/>
     </row>
-    <row r="178" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A178" s="18"/>
       <c r="B178" s="18"/>
       <c r="C178" s="18"/>
@@ -8712,7 +8723,7 @@
       <c r="P178" s="18"/>
       <c r="Q178" s="18"/>
     </row>
-    <row r="179" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A179" s="18"/>
       <c r="B179" s="18"/>
       <c r="C179" s="18"/>
@@ -8731,7 +8742,7 @@
       <c r="P179" s="18"/>
       <c r="Q179" s="18"/>
     </row>
-    <row r="180" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A180" s="18"/>
       <c r="B180" s="18"/>
       <c r="C180" s="18"/>
@@ -8750,7 +8761,7 @@
       <c r="P180" s="18"/>
       <c r="Q180" s="18"/>
     </row>
-    <row r="181" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A181" s="18"/>
       <c r="B181" s="18"/>
       <c r="C181" s="18"/>
@@ -8769,7 +8780,7 @@
       <c r="P181" s="18"/>
       <c r="Q181" s="18"/>
     </row>
-    <row r="182" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A182" s="18"/>
       <c r="B182" s="18"/>
       <c r="C182" s="18"/>
@@ -8788,7 +8799,7 @@
       <c r="P182" s="18"/>
       <c r="Q182" s="18"/>
     </row>
-    <row r="183" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A183" s="18"/>
       <c r="B183" s="18"/>
       <c r="C183" s="18"/>
@@ -8807,7 +8818,7 @@
       <c r="P183" s="18"/>
       <c r="Q183" s="18"/>
     </row>
-    <row r="184" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A184" s="18"/>
       <c r="B184" s="18"/>
       <c r="C184" s="18"/>
@@ -8826,7 +8837,7 @@
       <c r="P184" s="18"/>
       <c r="Q184" s="18"/>
     </row>
-    <row r="185" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A185" s="18"/>
       <c r="B185" s="18"/>
       <c r="C185" s="18"/>
@@ -8845,7 +8856,7 @@
       <c r="P185" s="18"/>
       <c r="Q185" s="18"/>
     </row>
-    <row r="186" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A186" s="18"/>
       <c r="B186" s="18"/>
       <c r="C186" s="18"/>
@@ -8864,7 +8875,7 @@
       <c r="P186" s="18"/>
       <c r="Q186" s="18"/>
     </row>
-    <row r="187" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A187" s="18"/>
       <c r="B187" s="18"/>
       <c r="C187" s="18"/>
@@ -8885,13 +8896,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A84:A99"/>
-    <mergeCell ref="A101:A116"/>
-    <mergeCell ref="J82:N82"/>
-    <mergeCell ref="H84:H99"/>
-    <mergeCell ref="H101:H116"/>
-    <mergeCell ref="C82:F82"/>
     <mergeCell ref="A81:M81"/>
     <mergeCell ref="B16:M16"/>
     <mergeCell ref="J43:N43"/>
@@ -8902,6 +8906,13 @@
     <mergeCell ref="H62:H77"/>
     <mergeCell ref="H45:H60"/>
     <mergeCell ref="A42:M42"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A84:A99"/>
+    <mergeCell ref="A101:A116"/>
+    <mergeCell ref="J82:N82"/>
+    <mergeCell ref="H84:H99"/>
+    <mergeCell ref="H101:H116"/>
+    <mergeCell ref="C82:F82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>